<commit_message>
cambios en tiempos de cirugía
</commit_message>
<xml_diff>
--- a/app_salud/app/logic/data/set_de_datos_1.xlsx
+++ b/app_salud/app/logic/data/set_de_datos_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rstudio\software_salud\app_salud\app\logic\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CDEF717-1D88-4BCF-89D0-E273366A2836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC03895F-60AB-427B-BE13-B8521A74EDFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A035267E-5D3E-4097-B788-79B64BEF5509}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{A035267E-5D3E-4097-B788-79B64BEF5509}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="21">
   <si>
     <t>Febrero</t>
   </si>
@@ -85,6 +85,21 @@
   </si>
   <si>
     <t>Porcentaje de horas mensuales de Quirófanos en trabajo</t>
+  </si>
+  <si>
+    <t>Especialidad</t>
+  </si>
+  <si>
+    <t>Cirugía general</t>
+  </si>
+  <si>
+    <t>Neurocirugía</t>
+  </si>
+  <si>
+    <t>Cirugía cardiovascular</t>
+  </si>
+  <si>
+    <t>Minutos</t>
   </si>
 </sst>
 </file>
@@ -448,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E76CA52-FDC3-4172-B462-57143B56E1E7}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -660,12 +675,1215 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{338D3236-E8E6-4099-8AC3-E37AC86733EF}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B150"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B148" sqref="B148"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>17</v>
+      </c>
+      <c r="B43">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>17</v>
+      </c>
+      <c r="B44">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>17</v>
+      </c>
+      <c r="B46">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>17</v>
+      </c>
+      <c r="B48">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>17</v>
+      </c>
+      <c r="B49">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>17</v>
+      </c>
+      <c r="B50">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>18</v>
+      </c>
+      <c r="B51">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>18</v>
+      </c>
+      <c r="B52">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>18</v>
+      </c>
+      <c r="B53">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>18</v>
+      </c>
+      <c r="B54">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>18</v>
+      </c>
+      <c r="B55">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>18</v>
+      </c>
+      <c r="B56">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>18</v>
+      </c>
+      <c r="B57">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>18</v>
+      </c>
+      <c r="B58">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>18</v>
+      </c>
+      <c r="B59">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>18</v>
+      </c>
+      <c r="B60">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>18</v>
+      </c>
+      <c r="B61">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>18</v>
+      </c>
+      <c r="B62">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>18</v>
+      </c>
+      <c r="B63">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>18</v>
+      </c>
+      <c r="B64">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>18</v>
+      </c>
+      <c r="B65">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>18</v>
+      </c>
+      <c r="B66">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>18</v>
+      </c>
+      <c r="B67">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>18</v>
+      </c>
+      <c r="B68">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>18</v>
+      </c>
+      <c r="B69">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>18</v>
+      </c>
+      <c r="B70">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>18</v>
+      </c>
+      <c r="B71">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>18</v>
+      </c>
+      <c r="B72">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>18</v>
+      </c>
+      <c r="B73">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>18</v>
+      </c>
+      <c r="B74">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>18</v>
+      </c>
+      <c r="B75">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>18</v>
+      </c>
+      <c r="B76">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>18</v>
+      </c>
+      <c r="B77">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>18</v>
+      </c>
+      <c r="B78">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>18</v>
+      </c>
+      <c r="B79">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>18</v>
+      </c>
+      <c r="B80">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>18</v>
+      </c>
+      <c r="B81">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>18</v>
+      </c>
+      <c r="B82">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>18</v>
+      </c>
+      <c r="B83">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>18</v>
+      </c>
+      <c r="B84">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>18</v>
+      </c>
+      <c r="B85">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>18</v>
+      </c>
+      <c r="B86">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>18</v>
+      </c>
+      <c r="B87">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>18</v>
+      </c>
+      <c r="B88">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>18</v>
+      </c>
+      <c r="B89">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>18</v>
+      </c>
+      <c r="B90">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>18</v>
+      </c>
+      <c r="B91">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>18</v>
+      </c>
+      <c r="B92">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>18</v>
+      </c>
+      <c r="B93">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>18</v>
+      </c>
+      <c r="B94">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>18</v>
+      </c>
+      <c r="B95">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>18</v>
+      </c>
+      <c r="B96">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>18</v>
+      </c>
+      <c r="B97">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>18</v>
+      </c>
+      <c r="B98">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>18</v>
+      </c>
+      <c r="B99">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>18</v>
+      </c>
+      <c r="B100">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>19</v>
+      </c>
+      <c r="B101">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>19</v>
+      </c>
+      <c r="B102">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>19</v>
+      </c>
+      <c r="B103">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>19</v>
+      </c>
+      <c r="B104">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>19</v>
+      </c>
+      <c r="B105">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>19</v>
+      </c>
+      <c r="B106">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>19</v>
+      </c>
+      <c r="B107">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>19</v>
+      </c>
+      <c r="B108">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>19</v>
+      </c>
+      <c r="B109">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>19</v>
+      </c>
+      <c r="B110">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>19</v>
+      </c>
+      <c r="B111">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>19</v>
+      </c>
+      <c r="B112">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>19</v>
+      </c>
+      <c r="B113">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>19</v>
+      </c>
+      <c r="B114">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>19</v>
+      </c>
+      <c r="B115">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>19</v>
+      </c>
+      <c r="B116">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>19</v>
+      </c>
+      <c r="B117">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>19</v>
+      </c>
+      <c r="B118">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>19</v>
+      </c>
+      <c r="B119">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>19</v>
+      </c>
+      <c r="B120">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>19</v>
+      </c>
+      <c r="B121">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>19</v>
+      </c>
+      <c r="B122">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>19</v>
+      </c>
+      <c r="B123">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>19</v>
+      </c>
+      <c r="B124">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>19</v>
+      </c>
+      <c r="B125">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>19</v>
+      </c>
+      <c r="B126">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>19</v>
+      </c>
+      <c r="B127">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>19</v>
+      </c>
+      <c r="B128">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>19</v>
+      </c>
+      <c r="B129">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>19</v>
+      </c>
+      <c r="B130">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>19</v>
+      </c>
+      <c r="B131">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>19</v>
+      </c>
+      <c r="B132">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>19</v>
+      </c>
+      <c r="B133">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>19</v>
+      </c>
+      <c r="B134">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>19</v>
+      </c>
+      <c r="B135">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>19</v>
+      </c>
+      <c r="B136">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>19</v>
+      </c>
+      <c r="B137">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>19</v>
+      </c>
+      <c r="B138">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>19</v>
+      </c>
+      <c r="B139">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>19</v>
+      </c>
+      <c r="B140">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>19</v>
+      </c>
+      <c r="B141">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>19</v>
+      </c>
+      <c r="B142">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>19</v>
+      </c>
+      <c r="B143">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>19</v>
+      </c>
+      <c r="B144">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>19</v>
+      </c>
+      <c r="B145">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>19</v>
+      </c>
+      <c r="B146">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>19</v>
+      </c>
+      <c r="B147">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>19</v>
+      </c>
+      <c r="B148">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>19</v>
+      </c>
+      <c r="B149">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>19</v>
+      </c>
+      <c r="B150">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se modifica estructura de modulo utilizacion de quirofanos y se actualiza grafico y tabla
</commit_message>
<xml_diff>
--- a/app_salud/app/logic/data/set_de_datos_1.xlsx
+++ b/app_salud/app/logic/data/set_de_datos_1.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rstudio\software_salud\app_salud\app\logic\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\documentos juan\Salud\software_salud\app_salud\app\logic\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC03895F-60AB-427B-BE13-B8521A74EDFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA9C54A-050E-41D5-A036-A8BC996B68FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{A035267E-5D3E-4097-B788-79B64BEF5509}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja1_1" sheetId="3" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,8 +29,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="36">
   <si>
     <t>Febrero</t>
   </si>
@@ -100,13 +99,58 @@
   </si>
   <si>
     <t>Minutos</t>
+  </si>
+  <si>
+    <t>Porcentaje de horas programadas</t>
+  </si>
+  <si>
+    <t>Agosto</t>
+  </si>
+  <si>
+    <t>De cirugia electiva</t>
+  </si>
+  <si>
+    <t>Tipo de quirofano</t>
+  </si>
+  <si>
+    <t>Horas mensuales habilitadas</t>
+  </si>
+  <si>
+    <t>Horas mensuales programadas</t>
+  </si>
+  <si>
+    <t>Horas mensuales en trabajo</t>
+  </si>
+  <si>
+    <t>Horas mensuales ocupadas horario habil</t>
+  </si>
+  <si>
+    <t>% trabajo respecto a habilitado</t>
+  </si>
+  <si>
+    <t>% programado respecto a habilitado</t>
+  </si>
+  <si>
+    <t>% trabajo respecto a programado</t>
+  </si>
+  <si>
+    <t>% ocupadas hh respecto a programadas</t>
+  </si>
+  <si>
+    <t>% ocupación respecto a habilitados</t>
+  </si>
+  <si>
+    <t>Tipo de hora</t>
+  </si>
+  <si>
+    <t>Valor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +161,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -143,13 +193,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -165,7 +219,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -461,20 +515,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E76CA52-FDC3-4172-B462-57143B56E1E7}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection sqref="A1:A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="51" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -487,8 +542,11 @@
       <c r="D1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -503,7 +561,7 @@
         <v>0.42517006802721086</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -518,7 +576,7 @@
         <v>0.44172932330827069</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -533,7 +591,7 @@
         <v>0.39208074534161491</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -548,7 +606,7 @@
         <v>0.6964285714285714</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -563,7 +621,7 @@
         <v>0.61688311688311692</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -578,7 +636,7 @@
         <v>0.6428571428571429</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -593,7 +651,7 @@
         <v>0.66326530612244894</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -608,7 +666,7 @@
         <v>0.70578231292517002</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -623,7 +681,7 @@
         <v>0.7142857142857143</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -638,7 +696,7 @@
         <v>0.67011278195488722</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -653,7 +711,7 @@
         <v>0.73129251700680276</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -674,14 +732,1018 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CF449E3-331A-4A7F-AB26-A48D8D1A9D4F}">
+  <dimension ref="A1:K59"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="13.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2">
+        <v>1176</v>
+      </c>
+      <c r="D2">
+        <v>677</v>
+      </c>
+      <c r="E2">
+        <v>491</v>
+      </c>
+      <c r="F2">
+        <v>500</v>
+      </c>
+      <c r="G2" s="2">
+        <f>E2/C2</f>
+        <v>0.41751700680272108</v>
+      </c>
+      <c r="H2" s="2">
+        <f>D2/C2</f>
+        <v>0.57568027210884354</v>
+      </c>
+      <c r="I2" s="2">
+        <f>E2/D2</f>
+        <v>0.72525849335302806</v>
+      </c>
+      <c r="J2" s="2">
+        <f>F2/D2</f>
+        <v>0.73855243722304287</v>
+      </c>
+      <c r="K2" s="2">
+        <f>F2/C2</f>
+        <v>0.42517006802721086</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3">
+        <v>1064</v>
+      </c>
+      <c r="D3">
+        <v>517</v>
+      </c>
+      <c r="E3">
+        <v>445</v>
+      </c>
+      <c r="F3">
+        <v>445</v>
+      </c>
+      <c r="G3" s="2">
+        <f t="shared" ref="G3:G12" si="0">E3/C3</f>
+        <v>0.4182330827067669</v>
+      </c>
+      <c r="H3" s="2">
+        <f t="shared" ref="H3:H12" si="1">D3/C3</f>
+        <v>0.48590225563909772</v>
+      </c>
+      <c r="I3" s="2">
+        <f t="shared" ref="I3:I12" si="2">E3/D3</f>
+        <v>0.86073500967117988</v>
+      </c>
+      <c r="J3" s="2">
+        <f t="shared" ref="J3:J12" si="3">F3/D3</f>
+        <v>0.86073500967117988</v>
+      </c>
+      <c r="K3" s="2">
+        <f t="shared" ref="K3:K12" si="4">F3/C3</f>
+        <v>0.4182330827067669</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4">
+        <v>1288</v>
+      </c>
+      <c r="D4">
+        <v>579</v>
+      </c>
+      <c r="E4">
+        <v>491</v>
+      </c>
+      <c r="F4">
+        <v>491</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" si="0"/>
+        <v>0.38121118012422361</v>
+      </c>
+      <c r="H4" s="2">
+        <f t="shared" si="1"/>
+        <v>0.4495341614906832</v>
+      </c>
+      <c r="I4" s="2">
+        <f t="shared" si="2"/>
+        <v>0.84801381692573408</v>
+      </c>
+      <c r="J4" s="2">
+        <f t="shared" si="3"/>
+        <v>0.84801381692573408</v>
+      </c>
+      <c r="K4" s="2">
+        <f t="shared" si="4"/>
+        <v>0.38121118012422361</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5">
+        <v>1120</v>
+      </c>
+      <c r="D5">
+        <v>923</v>
+      </c>
+      <c r="E5">
+        <v>740</v>
+      </c>
+      <c r="F5">
+        <v>740</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>0.6607142857142857</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" si="1"/>
+        <v>0.82410714285714282</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" si="2"/>
+        <v>0.80173347778981585</v>
+      </c>
+      <c r="J5" s="2">
+        <f t="shared" si="3"/>
+        <v>0.80173347778981585</v>
+      </c>
+      <c r="K5" s="2">
+        <f t="shared" si="4"/>
+        <v>0.6607142857142857</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6">
+        <v>1232</v>
+      </c>
+      <c r="D6">
+        <v>1157</v>
+      </c>
+      <c r="E6">
+        <v>845</v>
+      </c>
+      <c r="F6">
+        <v>845</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.68587662337662336</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="1"/>
+        <v>0.93912337662337664</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" si="2"/>
+        <v>0.7303370786516854</v>
+      </c>
+      <c r="J6" s="2">
+        <f t="shared" si="3"/>
+        <v>0.7303370786516854</v>
+      </c>
+      <c r="K6" s="2">
+        <f t="shared" si="4"/>
+        <v>0.68587662337662336</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7">
+        <v>1120</v>
+      </c>
+      <c r="D7">
+        <v>1168</v>
+      </c>
+      <c r="E7">
+        <v>800</v>
+      </c>
+      <c r="F7">
+        <v>800</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0428571428571429</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" si="2"/>
+        <v>0.68493150684931503</v>
+      </c>
+      <c r="J7" s="2">
+        <f t="shared" si="3"/>
+        <v>0.68493150684931503</v>
+      </c>
+      <c r="K7" s="2">
+        <f t="shared" si="4"/>
+        <v>0.7142857142857143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8">
+        <v>1176</v>
+      </c>
+      <c r="D8">
+        <v>834</v>
+      </c>
+      <c r="E8">
+        <v>822</v>
+      </c>
+      <c r="F8">
+        <v>822</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.69897959183673475</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="1"/>
+        <v>0.70918367346938771</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="2"/>
+        <v>0.98561151079136688</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" si="3"/>
+        <v>0.98561151079136688</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" si="4"/>
+        <v>0.69897959183673475</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9">
+        <v>1268</v>
+      </c>
+      <c r="D9">
+        <v>1268</v>
+      </c>
+      <c r="E9">
+        <v>910</v>
+      </c>
+      <c r="F9">
+        <v>910</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.71766561514195581</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="2"/>
+        <v>0.71766561514195581</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="3"/>
+        <v>0.71766561514195581</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" si="4"/>
+        <v>0.71766561514195581</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10">
+        <v>1176</v>
+      </c>
+      <c r="D10">
+        <v>1018</v>
+      </c>
+      <c r="E10">
+        <v>858</v>
+      </c>
+      <c r="F10">
+        <v>858</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.72959183673469385</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="1"/>
+        <v>0.86564625850340138</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="2"/>
+        <v>0.84282907662082518</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="3"/>
+        <v>0.84282907662082518</v>
+      </c>
+      <c r="K10" s="2">
+        <f t="shared" si="4"/>
+        <v>0.72959183673469385</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11">
+        <v>1064</v>
+      </c>
+      <c r="D11">
+        <v>920</v>
+      </c>
+      <c r="E11">
+        <v>716</v>
+      </c>
+      <c r="F11">
+        <v>716</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>0.67293233082706772</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.86466165413533835</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="2"/>
+        <v>0.77826086956521734</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="3"/>
+        <v>0.77826086956521734</v>
+      </c>
+      <c r="K11" s="2">
+        <f t="shared" si="4"/>
+        <v>0.67293233082706772</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12">
+        <v>1176</v>
+      </c>
+      <c r="D12">
+        <v>1093</v>
+      </c>
+      <c r="E12">
+        <v>876</v>
+      </c>
+      <c r="F12">
+        <v>876</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.74489795918367352</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="1"/>
+        <v>0.92942176870748294</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="2"/>
+        <v>0.80146386093321131</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="3"/>
+        <v>0.80146386093321131</v>
+      </c>
+      <c r="K12" s="2">
+        <f t="shared" si="4"/>
+        <v>0.74489795918367352</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16">
+        <f>C2</f>
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17">
+        <f>D2</f>
+        <v>677</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18">
+        <f>E2</f>
+        <v>491</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19">
+        <f>F2</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20">
+        <f t="array" ref="C20:C23">TRANSPOSE(C3:F3)</f>
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24">
+        <f t="array" ref="C24:C27">TRANSPOSE(C4:F4)</f>
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28">
+        <f t="array" ref="C28:C31">TRANSPOSE(C5:F5)</f>
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32">
+        <f t="array" ref="C32:C35">TRANSPOSE(C6:F6)</f>
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36">
+        <f t="array" ref="C36:C39">TRANSPOSE(C7:F7)</f>
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40">
+        <f t="array" ref="C40:C43">TRANSPOSE(C8:F8)</f>
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C41">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C42">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C43">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44">
+        <f t="array" ref="C44:C47">TRANSPOSE(C9:F9)</f>
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C46">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C47">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48">
+        <f t="array" ref="C48:C51">TRANSPOSE(C10:F10)</f>
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C50">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>9</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C52">
+        <f t="array" ref="C52:C55">TRANSPOSE(C11:F11)</f>
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>9</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C53">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>9</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C54">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>9</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C55">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>10</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C56">
+        <f t="array" ref="C56:C59">TRANSPOSE(C12:F12)</f>
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>10</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C57">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>10</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C58">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>10</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C59">
+        <v>876</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{338D3236-E8E6-4099-8AC3-E37AC86733EF}">
   <dimension ref="A1:B150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B148" sqref="B148"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
se actualiza set de datos
</commit_message>
<xml_diff>
--- a/app_salud/app/logic/data/set_de_datos_1.xlsx
+++ b/app_salud/app/logic/data/set_de_datos_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rstudio\software_salud\app_salud\app\logic\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9492EF96-20CE-427E-BEF7-8591E17014CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81F656E-A015-4923-87EF-06D7A54C4F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{A035267E-5D3E-4097-B788-79B64BEF5509}"/>
   </bookViews>
@@ -16,7 +16,8 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="tiempo_cirugía" sheetId="2" r:id="rId2"/>
     <sheet name="Calendario_semanal" sheetId="3" r:id="rId3"/>
-    <sheet name="Hoja2" sheetId="4" r:id="rId4"/>
+    <sheet name="Hoja3" sheetId="5" r:id="rId4"/>
+    <sheet name="Hoja2" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="116">
   <si>
     <t>Febrero</t>
   </si>
@@ -309,6 +310,84 @@
   </si>
   <si>
     <t>Total general</t>
+  </si>
+  <si>
+    <t>Año de Mes</t>
+  </si>
+  <si>
+    <t>Mes de Mes</t>
+  </si>
+  <si>
+    <t>Tipo De Quirófanos</t>
+  </si>
+  <si>
+    <t>Horas mensuales habilitadas</t>
+  </si>
+  <si>
+    <t>Horas mensuales programadas</t>
+  </si>
+  <si>
+    <t>Horas mensuales en trabajo</t>
+  </si>
+  <si>
+    <t>Horas mensuales ocupadas horario hábil</t>
+  </si>
+  <si>
+    <t>% trabajo respecto a habilitado</t>
+  </si>
+  <si>
+    <t>% programado respecto a habilitado</t>
+  </si>
+  <si>
+    <t>% trabajo respecto a programado</t>
+  </si>
+  <si>
+    <t>% ocupadas hh respecto a programadas</t>
+  </si>
+  <si>
+    <t>% ocupación respecto a habilitados</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>noviembre</t>
+  </si>
+  <si>
+    <t>DE CIRUGÍA ELECTIVA</t>
+  </si>
+  <si>
+    <t>octubre</t>
+  </si>
+  <si>
+    <t>septiembre</t>
+  </si>
+  <si>
+    <t>agosto</t>
+  </si>
+  <si>
+    <t>julio</t>
+  </si>
+  <si>
+    <t>junio</t>
+  </si>
+  <si>
+    <t>mayo</t>
+  </si>
+  <si>
+    <t>abril</t>
+  </si>
+  <si>
+    <t>marzo</t>
+  </si>
+  <si>
+    <t>febrero</t>
+  </si>
+  <si>
+    <t>enero</t>
+  </si>
+  <si>
+    <t>Promedio mensual</t>
   </si>
 </sst>
 </file>
@@ -318,7 +397,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m\-d\-yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,6 +417,16 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -361,10 +450,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2163,7 +2276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFF02165-7DDF-4DB7-89ED-75083A28E198}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -2611,10 +2724,511 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9808375D-D5D5-4E71-A87A-5B28F2320F53}">
+  <dimension ref="A1:M13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="14.109375" customWidth="1"/>
+    <col min="4" max="4" width="23.109375" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.88671875" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="M1" s="10"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1176</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1092.5999999999999</v>
+      </c>
+      <c r="F2" s="6">
+        <v>875.80359999999996</v>
+      </c>
+      <c r="G2" s="6">
+        <v>875.80360000000007</v>
+      </c>
+      <c r="H2" s="7">
+        <v>0.74473095238095233</v>
+      </c>
+      <c r="I2" s="7">
+        <v>0.9290816326530611</v>
+      </c>
+      <c r="J2" s="7">
+        <v>0.80157752150832884</v>
+      </c>
+      <c r="K2" s="7">
+        <v>0.80157752150832884</v>
+      </c>
+      <c r="L2" s="7">
+        <v>0.74473095238095244</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1064</v>
+      </c>
+      <c r="E3" s="6">
+        <v>919.75</v>
+      </c>
+      <c r="F3" s="6">
+        <v>715.97230000000002</v>
+      </c>
+      <c r="G3" s="6">
+        <v>715.97230000000002</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0.67290629699248117</v>
+      </c>
+      <c r="I3" s="7">
+        <v>0.86442669172932329</v>
+      </c>
+      <c r="J3" s="7">
+        <v>0.77844229410165811</v>
+      </c>
+      <c r="K3" s="7">
+        <v>0.77844229410165811</v>
+      </c>
+      <c r="L3" s="7">
+        <v>0.67290629699248117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1176</v>
+      </c>
+      <c r="E4" s="6">
+        <v>1017.55</v>
+      </c>
+      <c r="F4" s="6">
+        <v>858.42156666666665</v>
+      </c>
+      <c r="G4" s="6">
+        <v>858.42156666666665</v>
+      </c>
+      <c r="H4" s="7">
+        <v>0.72995031179138326</v>
+      </c>
+      <c r="I4" s="7">
+        <v>0.86526360544217684</v>
+      </c>
+      <c r="J4" s="7">
+        <v>0.84361610404075149</v>
+      </c>
+      <c r="K4" s="7">
+        <v>0.84361610404075149</v>
+      </c>
+      <c r="L4" s="7">
+        <v>0.72995031179138326</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1268</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1267.75</v>
+      </c>
+      <c r="F5" s="6">
+        <v>909.65266666666662</v>
+      </c>
+      <c r="G5" s="6">
+        <v>909.65266666666662</v>
+      </c>
+      <c r="H5" s="7">
+        <v>0.71739169295478444</v>
+      </c>
+      <c r="I5" s="7">
+        <v>0.99980283911671919</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0.71753316242687171</v>
+      </c>
+      <c r="K5" s="7">
+        <v>0.71753316242687171</v>
+      </c>
+      <c r="L5" s="7">
+        <v>0.71739169295478444</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1176</v>
+      </c>
+      <c r="E6" s="6">
+        <v>834.05000000000007</v>
+      </c>
+      <c r="F6" s="6">
+        <v>821.85403333333329</v>
+      </c>
+      <c r="G6" s="6">
+        <v>821.85403333333329</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0.69885547052154195</v>
+      </c>
+      <c r="I6" s="7">
+        <v>0.70922619047619051</v>
+      </c>
+      <c r="J6" s="7">
+        <v>0.98537741542273627</v>
+      </c>
+      <c r="K6" s="7">
+        <v>0.98537741542273627</v>
+      </c>
+      <c r="L6" s="7">
+        <v>0.69885547052154195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" s="6">
+        <v>1120</v>
+      </c>
+      <c r="E7" s="6">
+        <v>1168.1000000000001</v>
+      </c>
+      <c r="F7" s="6">
+        <v>799.7036333333333</v>
+      </c>
+      <c r="G7" s="6">
+        <v>799.7036333333333</v>
+      </c>
+      <c r="H7" s="7">
+        <v>0.71402110119047613</v>
+      </c>
+      <c r="I7" s="7">
+        <v>1.0429464285714287</v>
+      </c>
+      <c r="J7" s="7">
+        <v>0.68461915361127745</v>
+      </c>
+      <c r="K7" s="7">
+        <v>0.68461915361127745</v>
+      </c>
+      <c r="L7" s="7">
+        <v>0.71402110119047613</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1232</v>
+      </c>
+      <c r="E8" s="6">
+        <v>1156.9000000000001</v>
+      </c>
+      <c r="F8" s="6">
+        <v>845.42060000000004</v>
+      </c>
+      <c r="G8" s="6">
+        <v>845.42059999999992</v>
+      </c>
+      <c r="H8" s="7">
+        <v>0.68621801948051953</v>
+      </c>
+      <c r="I8" s="7">
+        <v>0.93904220779220782</v>
+      </c>
+      <c r="J8" s="7">
+        <v>0.7307637652346789</v>
+      </c>
+      <c r="K8" s="7">
+        <v>0.73076376523467879</v>
+      </c>
+      <c r="L8" s="7">
+        <v>0.68621801948051941</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1120</v>
+      </c>
+      <c r="E9" s="6">
+        <v>923.15</v>
+      </c>
+      <c r="F9" s="6">
+        <v>739.87</v>
+      </c>
+      <c r="G9" s="6">
+        <v>739.87196666666671</v>
+      </c>
+      <c r="H9" s="7">
+        <v>0.6605982142857143</v>
+      </c>
+      <c r="I9" s="7">
+        <v>0.82424107142857139</v>
+      </c>
+      <c r="J9" s="7">
+        <v>0.80146238422791527</v>
+      </c>
+      <c r="K9" s="7">
+        <v>0.80146451461481527</v>
+      </c>
+      <c r="L9" s="7">
+        <v>0.66059997023809525</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1288</v>
+      </c>
+      <c r="E10" s="6">
+        <v>579.1</v>
+      </c>
+      <c r="F10" s="6">
+        <v>490.98</v>
+      </c>
+      <c r="G10" s="6">
+        <v>490.98</v>
+      </c>
+      <c r="H10" s="7">
+        <v>0.38119565217391305</v>
+      </c>
+      <c r="I10" s="7">
+        <v>0.44961180124223604</v>
+      </c>
+      <c r="J10" s="7">
+        <v>0.847832844068382</v>
+      </c>
+      <c r="K10" s="7">
+        <v>0.847832844068382</v>
+      </c>
+      <c r="L10" s="7">
+        <v>0.38119565217391305</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" s="6">
+        <v>1064</v>
+      </c>
+      <c r="E11" s="6">
+        <v>517.25</v>
+      </c>
+      <c r="F11" s="6">
+        <v>444.84346666666664</v>
+      </c>
+      <c r="G11" s="6">
+        <v>444.84346666666664</v>
+      </c>
+      <c r="H11" s="7">
+        <v>0.41808596491228067</v>
+      </c>
+      <c r="I11" s="7">
+        <v>0.48613721804511278</v>
+      </c>
+      <c r="J11" s="7">
+        <v>0.86001636861607855</v>
+      </c>
+      <c r="K11" s="7">
+        <v>0.86001636861607855</v>
+      </c>
+      <c r="L11" s="7">
+        <v>0.41808596491228067</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1176</v>
+      </c>
+      <c r="E12" s="6">
+        <v>676.6</v>
+      </c>
+      <c r="F12" s="6">
+        <v>490.98</v>
+      </c>
+      <c r="G12" s="6">
+        <v>499.51</v>
+      </c>
+      <c r="H12" s="7">
+        <v>0.41750000000000004</v>
+      </c>
+      <c r="I12" s="7">
+        <v>0.5753401360544218</v>
+      </c>
+      <c r="J12" s="7">
+        <v>0.72565770026603604</v>
+      </c>
+      <c r="K12" s="7">
+        <v>0.73826485368016548</v>
+      </c>
+      <c r="L12" s="7">
+        <v>0.42475340136054424</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="6">
+        <v>1169.090909090909</v>
+      </c>
+      <c r="E13" s="6">
+        <v>922.98181818181808</v>
+      </c>
+      <c r="F13" s="6">
+        <v>726.68198787878782</v>
+      </c>
+      <c r="G13" s="6">
+        <v>727.45762121212124</v>
+      </c>
+      <c r="H13" s="7">
+        <v>0.62195033424400425</v>
+      </c>
+      <c r="I13" s="7">
+        <v>0.78955634750467718</v>
+      </c>
+      <c r="J13" s="7">
+        <v>0.79789988304770132</v>
+      </c>
+      <c r="K13" s="7">
+        <v>0.79904618157506746</v>
+      </c>
+      <c r="L13" s="7">
+        <v>0.62260989399972477</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A12"/>
+    <mergeCell ref="A13:C13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22BBA4D-C85A-4304-A112-5E7EF2BBD7F1}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
se actualizan datos para quirofanos
</commit_message>
<xml_diff>
--- a/app_salud/app/logic/data/set_de_datos_1.xlsx
+++ b/app_salud/app/logic/data/set_de_datos_1.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rstudio\software_salud\app_salud\app\logic\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\documentos juan\Salud\software_salud\app_salud\app\logic\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81F656E-A015-4923-87EF-06D7A54C4F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C10B74-872F-4024-A805-1EF5B2F13D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{A035267E-5D3E-4097-B788-79B64BEF5509}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A035267E-5D3E-4097-B788-79B64BEF5509}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="tiempo_cirugía" sheetId="2" r:id="rId2"/>
     <sheet name="Calendario_semanal" sheetId="3" r:id="rId3"/>
-    <sheet name="Hoja3" sheetId="5" r:id="rId4"/>
+    <sheet name="Horas" sheetId="5" r:id="rId4"/>
     <sheet name="Hoja2" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -31,8 +31,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -40,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="118">
   <si>
     <t>Febrero</t>
   </si>
@@ -315,9 +313,6 @@
     <t>Año de Mes</t>
   </si>
   <si>
-    <t>Mes de Mes</t>
-  </si>
-  <si>
     <t>Tipo De Quirófanos</t>
   </si>
   <si>
@@ -388,6 +383,15 @@
   </si>
   <si>
     <t>Promedio mensual</t>
+  </si>
+  <si>
+    <t>Agosto</t>
+  </si>
+  <si>
+    <t>Tipo de hora</t>
+  </si>
+  <si>
+    <t>Valor</t>
   </si>
 </sst>
 </file>
@@ -422,11 +426,13 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -450,15 +456,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -478,10 +481,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -546,7 +553,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -848,7 +855,7 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" customWidth="1"/>
@@ -1058,11 +1065,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{338D3236-E8E6-4099-8AC3-E37AC86733EF}">
   <dimension ref="A1:B150"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
       <selection activeCell="B148" sqref="B148"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.88671875" customWidth="1"/>
   </cols>
@@ -2280,7 +2287,7 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="31" customWidth="1"/>
     <col min="3" max="3" width="20.5546875" customWidth="1"/>
@@ -2725,15 +2732,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9808375D-D5D5-4E71-A87A-5B28F2320F53}">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:A59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="14.109375" customWidth="1"/>
+    <col min="2" max="2" width="36.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.109375" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" customWidth="1"/>
     <col min="6" max="6" width="18.88671875" customWidth="1"/>
@@ -2744,475 +2752,982 @@
       <c r="A1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="9"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="M1" s="10"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="B2" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5">
+        <v>1176</v>
+      </c>
+      <c r="E2" s="5">
+        <v>1092.5999999999999</v>
+      </c>
+      <c r="F2" s="5">
+        <v>875.80359999999996</v>
+      </c>
+      <c r="G2" s="5">
+        <v>875.80360000000007</v>
+      </c>
+      <c r="H2" s="6">
+        <v>0.74473095238095233</v>
+      </c>
+      <c r="I2" s="6">
+        <v>0.9290816326530611</v>
+      </c>
+      <c r="J2" s="6">
+        <v>0.80157752150832884</v>
+      </c>
+      <c r="K2" s="6">
+        <v>0.80157752150832884</v>
+      </c>
+      <c r="L2" s="6">
+        <v>0.74473095238095244</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="10"/>
+      <c r="B3" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="6">
+      <c r="C3" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="5">
+        <v>1064</v>
+      </c>
+      <c r="E3" s="5">
+        <v>919.75</v>
+      </c>
+      <c r="F3" s="5">
+        <v>715.97230000000002</v>
+      </c>
+      <c r="G3" s="5">
+        <v>715.97230000000002</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0.67290629699248117</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0.86442669172932329</v>
+      </c>
+      <c r="J3" s="6">
+        <v>0.77844229410165811</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0.77844229410165811</v>
+      </c>
+      <c r="L3" s="6">
+        <v>0.67290629699248117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="10"/>
+      <c r="B4" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="5">
         <v>1176</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E4" s="5">
+        <v>1017.55</v>
+      </c>
+      <c r="F4" s="5">
+        <v>858.42156666666665</v>
+      </c>
+      <c r="G4" s="5">
+        <v>858.42156666666665</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0.72995031179138326</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0.86526360544217684</v>
+      </c>
+      <c r="J4" s="6">
+        <v>0.84361610404075149</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0.84361610404075149</v>
+      </c>
+      <c r="L4" s="6">
+        <v>0.72995031179138326</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="10"/>
+      <c r="B5" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1268</v>
+      </c>
+      <c r="E5" s="5">
+        <v>1267.75</v>
+      </c>
+      <c r="F5" s="5">
+        <v>909.65266666666662</v>
+      </c>
+      <c r="G5" s="5">
+        <v>909.65266666666662</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0.71739169295478444</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0.99980283911671919</v>
+      </c>
+      <c r="J5" s="6">
+        <v>0.71753316242687171</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0.71753316242687171</v>
+      </c>
+      <c r="L5" s="6">
+        <v>0.71739169295478444</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="10"/>
+      <c r="B6" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="5">
+        <v>1176</v>
+      </c>
+      <c r="E6" s="5">
+        <v>834.05000000000007</v>
+      </c>
+      <c r="F6" s="5">
+        <v>821.85403333333329</v>
+      </c>
+      <c r="G6" s="5">
+        <v>821.85403333333329</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0.69885547052154195</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0.70922619047619051</v>
+      </c>
+      <c r="J6" s="6">
+        <v>0.98537741542273627</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0.98537741542273627</v>
+      </c>
+      <c r="L6" s="6">
+        <v>0.69885547052154195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="10"/>
+      <c r="B7" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1120</v>
+      </c>
+      <c r="E7" s="5">
+        <v>1168.1000000000001</v>
+      </c>
+      <c r="F7" s="5">
+        <v>799.7036333333333</v>
+      </c>
+      <c r="G7" s="5">
+        <v>799.7036333333333</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0.71402110119047613</v>
+      </c>
+      <c r="I7" s="6">
+        <v>1.0429464285714287</v>
+      </c>
+      <c r="J7" s="6">
+        <v>0.68461915361127745</v>
+      </c>
+      <c r="K7" s="6">
+        <v>0.68461915361127745</v>
+      </c>
+      <c r="L7" s="6">
+        <v>0.71402110119047613</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="10"/>
+      <c r="B8" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1232</v>
+      </c>
+      <c r="E8" s="5">
+        <v>1156.9000000000001</v>
+      </c>
+      <c r="F8" s="5">
+        <v>845.42060000000004</v>
+      </c>
+      <c r="G8" s="5">
+        <v>845.42059999999992</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0.68621801948051953</v>
+      </c>
+      <c r="I8" s="6">
+        <v>0.93904220779220782</v>
+      </c>
+      <c r="J8" s="6">
+        <v>0.7307637652346789</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0.73076376523467879</v>
+      </c>
+      <c r="L8" s="6">
+        <v>0.68621801948051941</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="10"/>
+      <c r="B9" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1120</v>
+      </c>
+      <c r="E9" s="5">
+        <v>923.15</v>
+      </c>
+      <c r="F9" s="5">
+        <v>739.87</v>
+      </c>
+      <c r="G9" s="5">
+        <v>739.87196666666671</v>
+      </c>
+      <c r="H9" s="6">
+        <v>0.6605982142857143</v>
+      </c>
+      <c r="I9" s="6">
+        <v>0.82424107142857139</v>
+      </c>
+      <c r="J9" s="6">
+        <v>0.80146238422791527</v>
+      </c>
+      <c r="K9" s="6">
+        <v>0.80146451461481527</v>
+      </c>
+      <c r="L9" s="6">
+        <v>0.66059997023809525</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="10"/>
+      <c r="B10" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1288</v>
+      </c>
+      <c r="E10" s="5">
+        <v>579.1</v>
+      </c>
+      <c r="F10" s="5">
+        <v>490.98</v>
+      </c>
+      <c r="G10" s="5">
+        <v>490.98</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0.38119565217391305</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0.44961180124223604</v>
+      </c>
+      <c r="J10" s="6">
+        <v>0.847832844068382</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0.847832844068382</v>
+      </c>
+      <c r="L10" s="6">
+        <v>0.38119565217391305</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="10"/>
+      <c r="B11" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1064</v>
+      </c>
+      <c r="E11" s="5">
+        <v>517.25</v>
+      </c>
+      <c r="F11" s="5">
+        <v>444.84346666666664</v>
+      </c>
+      <c r="G11" s="5">
+        <v>444.84346666666664</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0.41808596491228067</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0.48613721804511278</v>
+      </c>
+      <c r="J11" s="6">
+        <v>0.86001636861607855</v>
+      </c>
+      <c r="K11" s="6">
+        <v>0.86001636861607855</v>
+      </c>
+      <c r="L11" s="6">
+        <v>0.41808596491228067</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="10"/>
+      <c r="B12" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" s="5">
+        <v>1176</v>
+      </c>
+      <c r="E12" s="5">
+        <v>676.6</v>
+      </c>
+      <c r="F12" s="5">
+        <v>490.98</v>
+      </c>
+      <c r="G12" s="5">
+        <v>499.51</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0.41750000000000004</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0.5753401360544218</v>
+      </c>
+      <c r="J12" s="6">
+        <v>0.72565770026603604</v>
+      </c>
+      <c r="K12" s="6">
+        <v>0.73826485368016548</v>
+      </c>
+      <c r="L12" s="6">
+        <v>0.42475340136054424</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="5">
+        <v>1169.090909090909</v>
+      </c>
+      <c r="E13" s="5">
+        <v>922.98181818181808</v>
+      </c>
+      <c r="F13" s="5">
+        <v>726.68198787878782</v>
+      </c>
+      <c r="G13" s="5">
+        <v>727.45762121212124</v>
+      </c>
+      <c r="H13" s="6">
+        <v>0.62195033424400425</v>
+      </c>
+      <c r="I13" s="6">
+        <v>0.78955634750467718</v>
+      </c>
+      <c r="J13" s="6">
+        <v>0.79789988304770132</v>
+      </c>
+      <c r="K13" s="6">
+        <v>0.79904618157506746</v>
+      </c>
+      <c r="L13" s="6">
+        <v>0.62260989399972477</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="array" ref="B16:B19">TRANSPOSE(D1:G1)</f>
+        <v>Horas mensuales habilitadas</v>
+      </c>
+      <c r="C16" s="11">
+        <f t="array" ref="C16:C19">TRANSPOSE(D12:G12)</f>
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" t="str">
+        <v>Horas mensuales programadas</v>
+      </c>
+      <c r="C17" s="11">
+        <v>676.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Horas mensuales en trabajo</v>
+      </c>
+      <c r="C18" s="11">
+        <v>490.98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Horas mensuales ocupadas horario hábil</v>
+      </c>
+      <c r="C19" s="11">
+        <v>499.51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="11">
+        <f t="array" ref="C20:C23">TRANSPOSE(D11:G11)</f>
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>93</v>
+      </c>
+      <c r="C21" s="11">
+        <v>517.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" s="11">
+        <v>444.84346666666664</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="11">
+        <v>444.84346666666664</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="11">
+        <f t="array" ref="C24:C27">TRANSPOSE(D10:G10)</f>
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="11">
+        <v>579.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" s="11">
+        <v>490.98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" s="11">
+        <v>490.98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28" s="11">
+        <f t="array" ref="C28:C31">TRANSPOSE(D9:G9)</f>
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29" s="11">
+        <v>923.15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" s="11">
+        <v>739.87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" t="s">
+        <v>95</v>
+      </c>
+      <c r="C31" s="11">
+        <v>739.87196666666671</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" s="11">
+        <f t="array" ref="C32:C35">TRANSPOSE(D8:G8)</f>
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>93</v>
+      </c>
+      <c r="C33" s="11">
+        <v>1156.9000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" s="11">
+        <v>845.42060000000004</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" s="11">
+        <v>845.42059999999992</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" s="11">
+        <f t="array" ref="C36:C39">TRANSPOSE(D7:G7)</f>
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37" s="11">
+        <v>1168.1000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38" s="11">
+        <v>799.7036333333333</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" t="s">
+        <v>95</v>
+      </c>
+      <c r="C39" s="11">
+        <v>799.7036333333333</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" t="s">
+        <v>92</v>
+      </c>
+      <c r="C40" s="11">
+        <f t="array" ref="C40:C43">TRANSPOSE(D6:G6)</f>
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" t="s">
+        <v>93</v>
+      </c>
+      <c r="C41" s="11">
+        <v>834.05000000000007</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" s="11">
+        <v>821.85403333333329</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" t="s">
+        <v>95</v>
+      </c>
+      <c r="C43" s="11">
+        <v>821.85403333333329</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B44" t="s">
+        <v>92</v>
+      </c>
+      <c r="C44" s="11">
+        <f t="array" ref="C44:C47">TRANSPOSE(D5:G5)</f>
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B45" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" s="11">
+        <v>1267.75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B46" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" s="11">
+        <v>909.65266666666662</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B47" t="s">
+        <v>95</v>
+      </c>
+      <c r="C47" s="11">
+        <v>909.65266666666662</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48" t="s">
+        <v>92</v>
+      </c>
+      <c r="C48" s="11">
+        <f t="array" ref="C48:C51">TRANSPOSE(D4:G4)</f>
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49" s="11">
+        <v>1017.55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50" t="s">
+        <v>94</v>
+      </c>
+      <c r="C50" s="11">
+        <v>858.42156666666665</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51" t="s">
+        <v>95</v>
+      </c>
+      <c r="C51" s="11">
+        <v>858.42156666666665</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B52" t="s">
+        <v>92</v>
+      </c>
+      <c r="C52" s="11">
+        <f t="array" ref="C52:C55">TRANSPOSE(D3:G3)</f>
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B53" t="s">
+        <v>93</v>
+      </c>
+      <c r="C53" s="11">
+        <v>919.75</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B54" t="s">
+        <v>94</v>
+      </c>
+      <c r="C54" s="11">
+        <v>715.97230000000002</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B55" t="s">
+        <v>95</v>
+      </c>
+      <c r="C55" s="11">
+        <v>715.97230000000002</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B56" t="s">
+        <v>92</v>
+      </c>
+      <c r="C56" s="11">
+        <f t="array" ref="C56:C59">TRANSPOSE(D2:G2)</f>
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B57" t="s">
+        <v>93</v>
+      </c>
+      <c r="C57" s="11">
         <v>1092.5999999999999</v>
       </c>
-      <c r="F2" s="6">
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B58" t="s">
+        <v>94</v>
+      </c>
+      <c r="C58" s="11">
         <v>875.80359999999996</v>
       </c>
-      <c r="G2" s="6">
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B59" t="s">
+        <v>95</v>
+      </c>
+      <c r="C59" s="11">
         <v>875.80360000000007</v>
-      </c>
-      <c r="H2" s="7">
-        <v>0.74473095238095233</v>
-      </c>
-      <c r="I2" s="7">
-        <v>0.9290816326530611</v>
-      </c>
-      <c r="J2" s="7">
-        <v>0.80157752150832884</v>
-      </c>
-      <c r="K2" s="7">
-        <v>0.80157752150832884</v>
-      </c>
-      <c r="L2" s="7">
-        <v>0.74473095238095244</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D3" s="6">
-        <v>1064</v>
-      </c>
-      <c r="E3" s="6">
-        <v>919.75</v>
-      </c>
-      <c r="F3" s="6">
-        <v>715.97230000000002</v>
-      </c>
-      <c r="G3" s="6">
-        <v>715.97230000000002</v>
-      </c>
-      <c r="H3" s="7">
-        <v>0.67290629699248117</v>
-      </c>
-      <c r="I3" s="7">
-        <v>0.86442669172932329</v>
-      </c>
-      <c r="J3" s="7">
-        <v>0.77844229410165811</v>
-      </c>
-      <c r="K3" s="7">
-        <v>0.77844229410165811</v>
-      </c>
-      <c r="L3" s="7">
-        <v>0.67290629699248117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D4" s="6">
-        <v>1176</v>
-      </c>
-      <c r="E4" s="6">
-        <v>1017.55</v>
-      </c>
-      <c r="F4" s="6">
-        <v>858.42156666666665</v>
-      </c>
-      <c r="G4" s="6">
-        <v>858.42156666666665</v>
-      </c>
-      <c r="H4" s="7">
-        <v>0.72995031179138326</v>
-      </c>
-      <c r="I4" s="7">
-        <v>0.86526360544217684</v>
-      </c>
-      <c r="J4" s="7">
-        <v>0.84361610404075149</v>
-      </c>
-      <c r="K4" s="7">
-        <v>0.84361610404075149</v>
-      </c>
-      <c r="L4" s="7">
-        <v>0.72995031179138326</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D5" s="6">
-        <v>1268</v>
-      </c>
-      <c r="E5" s="6">
-        <v>1267.75</v>
-      </c>
-      <c r="F5" s="6">
-        <v>909.65266666666662</v>
-      </c>
-      <c r="G5" s="6">
-        <v>909.65266666666662</v>
-      </c>
-      <c r="H5" s="7">
-        <v>0.71739169295478444</v>
-      </c>
-      <c r="I5" s="7">
-        <v>0.99980283911671919</v>
-      </c>
-      <c r="J5" s="7">
-        <v>0.71753316242687171</v>
-      </c>
-      <c r="K5" s="7">
-        <v>0.71753316242687171</v>
-      </c>
-      <c r="L5" s="7">
-        <v>0.71739169295478444</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D6" s="6">
-        <v>1176</v>
-      </c>
-      <c r="E6" s="6">
-        <v>834.05000000000007</v>
-      </c>
-      <c r="F6" s="6">
-        <v>821.85403333333329</v>
-      </c>
-      <c r="G6" s="6">
-        <v>821.85403333333329</v>
-      </c>
-      <c r="H6" s="7">
-        <v>0.69885547052154195</v>
-      </c>
-      <c r="I6" s="7">
-        <v>0.70922619047619051</v>
-      </c>
-      <c r="J6" s="7">
-        <v>0.98537741542273627</v>
-      </c>
-      <c r="K6" s="7">
-        <v>0.98537741542273627</v>
-      </c>
-      <c r="L6" s="7">
-        <v>0.69885547052154195</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D7" s="6">
-        <v>1120</v>
-      </c>
-      <c r="E7" s="6">
-        <v>1168.1000000000001</v>
-      </c>
-      <c r="F7" s="6">
-        <v>799.7036333333333</v>
-      </c>
-      <c r="G7" s="6">
-        <v>799.7036333333333</v>
-      </c>
-      <c r="H7" s="7">
-        <v>0.71402110119047613</v>
-      </c>
-      <c r="I7" s="7">
-        <v>1.0429464285714287</v>
-      </c>
-      <c r="J7" s="7">
-        <v>0.68461915361127745</v>
-      </c>
-      <c r="K7" s="7">
-        <v>0.68461915361127745</v>
-      </c>
-      <c r="L7" s="7">
-        <v>0.71402110119047613</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D8" s="6">
-        <v>1232</v>
-      </c>
-      <c r="E8" s="6">
-        <v>1156.9000000000001</v>
-      </c>
-      <c r="F8" s="6">
-        <v>845.42060000000004</v>
-      </c>
-      <c r="G8" s="6">
-        <v>845.42059999999992</v>
-      </c>
-      <c r="H8" s="7">
-        <v>0.68621801948051953</v>
-      </c>
-      <c r="I8" s="7">
-        <v>0.93904220779220782</v>
-      </c>
-      <c r="J8" s="7">
-        <v>0.7307637652346789</v>
-      </c>
-      <c r="K8" s="7">
-        <v>0.73076376523467879</v>
-      </c>
-      <c r="L8" s="7">
-        <v>0.68621801948051941</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D9" s="6">
-        <v>1120</v>
-      </c>
-      <c r="E9" s="6">
-        <v>923.15</v>
-      </c>
-      <c r="F9" s="6">
-        <v>739.87</v>
-      </c>
-      <c r="G9" s="6">
-        <v>739.87196666666671</v>
-      </c>
-      <c r="H9" s="7">
-        <v>0.6605982142857143</v>
-      </c>
-      <c r="I9" s="7">
-        <v>0.82424107142857139</v>
-      </c>
-      <c r="J9" s="7">
-        <v>0.80146238422791527</v>
-      </c>
-      <c r="K9" s="7">
-        <v>0.80146451461481527</v>
-      </c>
-      <c r="L9" s="7">
-        <v>0.66059997023809525</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D10" s="6">
-        <v>1288</v>
-      </c>
-      <c r="E10" s="6">
-        <v>579.1</v>
-      </c>
-      <c r="F10" s="6">
-        <v>490.98</v>
-      </c>
-      <c r="G10" s="6">
-        <v>490.98</v>
-      </c>
-      <c r="H10" s="7">
-        <v>0.38119565217391305</v>
-      </c>
-      <c r="I10" s="7">
-        <v>0.44961180124223604</v>
-      </c>
-      <c r="J10" s="7">
-        <v>0.847832844068382</v>
-      </c>
-      <c r="K10" s="7">
-        <v>0.847832844068382</v>
-      </c>
-      <c r="L10" s="7">
-        <v>0.38119565217391305</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D11" s="6">
-        <v>1064</v>
-      </c>
-      <c r="E11" s="6">
-        <v>517.25</v>
-      </c>
-      <c r="F11" s="6">
-        <v>444.84346666666664</v>
-      </c>
-      <c r="G11" s="6">
-        <v>444.84346666666664</v>
-      </c>
-      <c r="H11" s="7">
-        <v>0.41808596491228067</v>
-      </c>
-      <c r="I11" s="7">
-        <v>0.48613721804511278</v>
-      </c>
-      <c r="J11" s="7">
-        <v>0.86001636861607855</v>
-      </c>
-      <c r="K11" s="7">
-        <v>0.86001636861607855</v>
-      </c>
-      <c r="L11" s="7">
-        <v>0.41808596491228067</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D12" s="6">
-        <v>1176</v>
-      </c>
-      <c r="E12" s="6">
-        <v>676.6</v>
-      </c>
-      <c r="F12" s="6">
-        <v>490.98</v>
-      </c>
-      <c r="G12" s="6">
-        <v>499.51</v>
-      </c>
-      <c r="H12" s="7">
-        <v>0.41750000000000004</v>
-      </c>
-      <c r="I12" s="7">
-        <v>0.5753401360544218</v>
-      </c>
-      <c r="J12" s="7">
-        <v>0.72565770026603604</v>
-      </c>
-      <c r="K12" s="7">
-        <v>0.73826485368016548</v>
-      </c>
-      <c r="L12" s="7">
-        <v>0.42475340136054424</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="6">
-        <v>1169.090909090909</v>
-      </c>
-      <c r="E13" s="6">
-        <v>922.98181818181808</v>
-      </c>
-      <c r="F13" s="6">
-        <v>726.68198787878782</v>
-      </c>
-      <c r="G13" s="6">
-        <v>727.45762121212124</v>
-      </c>
-      <c r="H13" s="7">
-        <v>0.62195033424400425</v>
-      </c>
-      <c r="I13" s="7">
-        <v>0.78955634750467718</v>
-      </c>
-      <c r="J13" s="7">
-        <v>0.79789988304770132</v>
-      </c>
-      <c r="K13" s="7">
-        <v>0.79904618157506746</v>
-      </c>
-      <c r="L13" s="7">
-        <v>0.62260989399972477</v>
       </c>
     </row>
   </sheetData>
@@ -3232,7 +3747,7 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="53.44140625" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" customWidth="1"/>

</xml_diff>

<commit_message>
se redimensiona analisis suspensiones y datos
</commit_message>
<xml_diff>
--- a/app_salud/app/logic/data/set_de_datos_1.xlsx
+++ b/app_salud/app/logic/data/set_de_datos_1.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\documentos juan\Salud\software_salud\app_salud\app\logic\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289B9F0E-811E-4991-A345-9AFB8D8FCD4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C519066-5E00-4D79-B99B-A0A0C5AB5684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="3" xr2:uid="{A035267E-5D3E-4097-B788-79B64BEF5509}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{A035267E-5D3E-4097-B788-79B64BEF5509}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="tiempo_cirugía" sheetId="2" r:id="rId2"/>
     <sheet name="Calendario_semanal" sheetId="3" r:id="rId3"/>
     <sheet name="Horas" sheetId="5" r:id="rId4"/>
-    <sheet name="Hoja2" sheetId="4" r:id="rId5"/>
+    <sheet name="Suspensiones" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -482,10 +482,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2735,7 +2735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9808375D-D5D5-4E71-A87A-5B28F2320F53}">
   <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E37"/>
     </sheetView>
   </sheetViews>
@@ -2789,7 +2789,7 @@
       <c r="M1" s="9"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>101</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -2827,7 +2827,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="11"/>
+      <c r="A3" s="12"/>
       <c r="B3" s="4" t="s">
         <v>104</v>
       </c>
@@ -2863,7 +2863,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="4" t="s">
         <v>105</v>
       </c>
@@ -2899,7 +2899,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="4" t="s">
         <v>106</v>
       </c>
@@ -2935,7 +2935,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="4" t="s">
         <v>107</v>
       </c>
@@ -2971,7 +2971,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="4" t="s">
         <v>108</v>
       </c>
@@ -3007,7 +3007,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="11"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="4" t="s">
         <v>109</v>
       </c>
@@ -3043,7 +3043,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="11"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="4" t="s">
         <v>110</v>
       </c>
@@ -3079,7 +3079,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="4" t="s">
         <v>111</v>
       </c>
@@ -3115,7 +3115,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="11"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="4" t="s">
         <v>112</v>
       </c>
@@ -3151,7 +3151,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="4" t="s">
         <v>113</v>
       </c>
@@ -3187,13 +3187,13 @@
       </c>
     </row>
     <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="12" t="s">
         <v>52</v>
       </c>
       <c r="D13" s="5">
@@ -3263,7 +3263,7 @@
         <f t="array" ref="F16:F17">TRANSPOSE(H1:I1)</f>
         <v>% trabajo respecto a habilitado</v>
       </c>
-      <c r="G16" s="12">
+      <c r="G16" s="11">
         <f t="array" ref="G16:G17">TRANSPOSE(H12:I12)</f>
         <v>0.41750000000000004</v>
       </c>
@@ -3284,7 +3284,7 @@
       <c r="F17" t="str">
         <v>% programado respecto a habilitado</v>
       </c>
-      <c r="G17" s="12">
+      <c r="G17" s="11">
         <v>0.5753401360544218</v>
       </c>
     </row>
@@ -3304,7 +3304,7 @@
       <c r="F18" t="s">
         <v>96</v>
       </c>
-      <c r="G18" s="12">
+      <c r="G18" s="11">
         <f t="array" ref="G18:G19">TRANSPOSE(H11:I11)</f>
         <v>0.41808596491228067</v>
       </c>
@@ -3325,7 +3325,7 @@
       <c r="F19" t="s">
         <v>97</v>
       </c>
-      <c r="G19" s="12">
+      <c r="G19" s="11">
         <v>0.48613721804511278</v>
       </c>
     </row>
@@ -3346,7 +3346,7 @@
       <c r="F20" t="s">
         <v>96</v>
       </c>
-      <c r="G20" s="12">
+      <c r="G20" s="11">
         <f t="array" ref="G20:G21">TRANSPOSE(H10:I10)</f>
         <v>0.38119565217391305</v>
       </c>
@@ -3367,7 +3367,7 @@
       <c r="F21" t="s">
         <v>97</v>
       </c>
-      <c r="G21" s="12">
+      <c r="G21" s="11">
         <v>0.44961180124223604</v>
       </c>
     </row>
@@ -3387,7 +3387,7 @@
       <c r="F22" t="s">
         <v>96</v>
       </c>
-      <c r="G22" s="12">
+      <c r="G22" s="11">
         <f t="array" ref="G22:G23">TRANSPOSE(H9:I9)</f>
         <v>0.6605982142857143</v>
       </c>
@@ -3408,7 +3408,7 @@
       <c r="F23" t="s">
         <v>97</v>
       </c>
-      <c r="G23" s="12">
+      <c r="G23" s="11">
         <v>0.82424107142857139</v>
       </c>
     </row>
@@ -3429,7 +3429,7 @@
       <c r="F24" t="s">
         <v>96</v>
       </c>
-      <c r="G24" s="12">
+      <c r="G24" s="11">
         <f t="array" ref="G24:G25">TRANSPOSE(H8:I8)</f>
         <v>0.68621801948051953</v>
       </c>
@@ -3450,7 +3450,7 @@
       <c r="F25" t="s">
         <v>97</v>
       </c>
-      <c r="G25" s="12">
+      <c r="G25" s="11">
         <v>0.93904220779220782</v>
       </c>
     </row>
@@ -3470,7 +3470,7 @@
       <c r="F26" t="s">
         <v>96</v>
       </c>
-      <c r="G26" s="12">
+      <c r="G26" s="11">
         <f t="array" ref="G26:G27">TRANSPOSE(H7:I7)</f>
         <v>0.71402110119047613</v>
       </c>
@@ -3491,7 +3491,7 @@
       <c r="F27" t="s">
         <v>97</v>
       </c>
-      <c r="G27" s="12">
+      <c r="G27" s="11">
         <v>1</v>
       </c>
     </row>
@@ -3512,7 +3512,7 @@
       <c r="F28" t="s">
         <v>96</v>
       </c>
-      <c r="G28" s="12">
+      <c r="G28" s="11">
         <f t="array" ref="G28:G29">TRANSPOSE(H6:I6)</f>
         <v>0.69885547052154195</v>
       </c>
@@ -3533,7 +3533,7 @@
       <c r="F29" t="s">
         <v>97</v>
       </c>
-      <c r="G29" s="12">
+      <c r="G29" s="11">
         <v>0.70922619047619051</v>
       </c>
     </row>
@@ -3553,7 +3553,7 @@
       <c r="F30" t="s">
         <v>96</v>
       </c>
-      <c r="G30" s="12">
+      <c r="G30" s="11">
         <f t="array" ref="G30:G31">TRANSPOSE(H5:I5)</f>
         <v>0.71739169295478444</v>
       </c>
@@ -3574,7 +3574,7 @@
       <c r="F31" t="s">
         <v>97</v>
       </c>
-      <c r="G31" s="12">
+      <c r="G31" s="11">
         <v>0.99980283911671919</v>
       </c>
     </row>
@@ -3595,7 +3595,7 @@
       <c r="F32" t="s">
         <v>96</v>
       </c>
-      <c r="G32" s="12">
+      <c r="G32" s="11">
         <f t="array" ref="G32:G33">TRANSPOSE(H4:I4)</f>
         <v>0.72995031179138326</v>
       </c>
@@ -3616,7 +3616,7 @@
       <c r="F33" t="s">
         <v>97</v>
       </c>
-      <c r="G33" s="12">
+      <c r="G33" s="11">
         <v>0.86526360544217684</v>
       </c>
     </row>
@@ -3636,7 +3636,7 @@
       <c r="F34" t="s">
         <v>96</v>
       </c>
-      <c r="G34" s="12">
+      <c r="G34" s="11">
         <f t="array" ref="G34:G35">TRANSPOSE(H3:I3)</f>
         <v>0.67290629699248117</v>
       </c>
@@ -3657,7 +3657,7 @@
       <c r="F35" t="s">
         <v>97</v>
       </c>
-      <c r="G35" s="12">
+      <c r="G35" s="11">
         <v>0.86442669172932329</v>
       </c>
     </row>
@@ -3678,7 +3678,7 @@
       <c r="F36" t="s">
         <v>96</v>
       </c>
-      <c r="G36" s="12">
+      <c r="G36" s="11">
         <f t="array" ref="G36:G37">TRANSPOSE(H2:I2)</f>
         <v>0.74473095238095233</v>
       </c>
@@ -3699,7 +3699,7 @@
       <c r="F37" t="s">
         <v>97</v>
       </c>
-      <c r="G37" s="12">
+      <c r="G37" s="11">
         <v>0.9290816326530611</v>
       </c>
     </row>
@@ -3985,7 +3985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22BBA4D-C85A-4304-A112-5E7EF2BBD7F1}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Datos supenciones anuales y tiempos extra
</commit_message>
<xml_diff>
--- a/app_salud/app/logic/data/set_de_datos_1.xlsx
+++ b/app_salud/app/logic/data/set_de_datos_1.xlsx
@@ -5,19 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\documentos juan\Salud\software_salud\app_salud\app\logic\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rstudio\software_salud\app_salud\app\logic\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C519066-5E00-4D79-B99B-A0A0C5AB5684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8707F22-8D35-452A-8175-E929C2622363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{A035267E-5D3E-4097-B788-79B64BEF5509}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{A035267E-5D3E-4097-B788-79B64BEF5509}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="tiempo_cirugía" sheetId="2" r:id="rId2"/>
     <sheet name="Calendario_semanal" sheetId="3" r:id="rId3"/>
     <sheet name="Horas" sheetId="5" r:id="rId4"/>
-    <sheet name="Suspensiones" sheetId="4" r:id="rId5"/>
+    <sheet name="Suspenciones anuales" sheetId="7" r:id="rId5"/>
+    <sheet name="Suspensiones" sheetId="4" r:id="rId6"/>
+    <sheet name="Tiempo extra" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="136">
   <si>
     <t>Febrero</t>
   </si>
@@ -392,6 +394,60 @@
   </si>
   <si>
     <t>Valor</t>
+  </si>
+  <si>
+    <t>Tipo de cirugía</t>
+  </si>
+  <si>
+    <t>Tiempo programado</t>
+  </si>
+  <si>
+    <t>Tiempo real</t>
+  </si>
+  <si>
+    <t>Tiempo adicional</t>
+  </si>
+  <si>
+    <t>Tiempo de inactividad</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Febrero </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mayo </t>
+  </si>
+  <si>
+    <t>Causas De Suspensión Atribuibles A:</t>
+  </si>
+  <si>
+    <t>diciembre</t>
+  </si>
+  <si>
+    <t>PACIENTE</t>
+  </si>
+  <si>
+    <t>% de total 15 Años Y Más junto con Causas De Suspensión Atribuibles A:</t>
+  </si>
+  <si>
+    <t>% de total Suspensiones totales junto con Causas De Suspensión Atribuibles A:</t>
+  </si>
+  <si>
+    <t>EQUIPO QUIRÚRGICO</t>
+  </si>
+  <si>
+    <t>ADMINISTRATIVAS</t>
+  </si>
+  <si>
+    <t>EMERGENCIAS</t>
+  </si>
+  <si>
+    <t>UNIDAD DE APOYO CLÍNICO</t>
+  </si>
+  <si>
+    <t>INFRAESTRUCTURA</t>
   </si>
 </sst>
 </file>
@@ -401,7 +457,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m\-d\-yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -434,6 +490,31 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -452,11 +533,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -486,10 +568,31 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{E3156AE8-1855-485A-AE3C-7436025EFAA8}"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -554,7 +657,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -856,7 +959,7 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" customWidth="1"/>
@@ -1070,7 +1173,7 @@
       <selection activeCell="B148" sqref="B148"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.88671875" customWidth="1"/>
   </cols>
@@ -2288,7 +2391,7 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="31" customWidth="1"/>
     <col min="3" max="3" width="20.5546875" customWidth="1"/>
@@ -2739,7 +2842,7 @@
       <selection activeCell="E1" sqref="E1:E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="36.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.109375" bestFit="1" customWidth="1"/>
@@ -3982,14 +4085,657 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7253C5DD-76E0-4DAF-B9AF-4AE6D659DCEE}">
+  <dimension ref="A1:O14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="48" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="N2" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="O2" s="20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="18">
+        <v>0.31034482758620691</v>
+      </c>
+      <c r="D3" s="18">
+        <v>0.42307692307692307</v>
+      </c>
+      <c r="E3" s="18">
+        <v>0.5357142857142857</v>
+      </c>
+      <c r="F3" s="18">
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="G3" s="18">
+        <v>0.26</v>
+      </c>
+      <c r="H3" s="18">
+        <v>0.51428571428571423</v>
+      </c>
+      <c r="I3" s="18">
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="J3" s="18">
+        <v>0.41463414634146339</v>
+      </c>
+      <c r="K3" s="18">
+        <v>0.62068965517241381</v>
+      </c>
+      <c r="L3" s="18">
+        <v>0.39130434782608697</v>
+      </c>
+      <c r="M3" s="18">
+        <v>0.62962962962962965</v>
+      </c>
+      <c r="N3" s="18">
+        <v>0.53846153846153844</v>
+      </c>
+      <c r="O3" s="18">
+        <v>0.45128205128205129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="19"/>
+      <c r="B4" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="18">
+        <v>0.3235294117647059</v>
+      </c>
+      <c r="D4" s="18">
+        <v>0.40740740740740738</v>
+      </c>
+      <c r="E4" s="18">
+        <v>0.5357142857142857</v>
+      </c>
+      <c r="F4" s="18">
+        <v>0.5757575757575758</v>
+      </c>
+      <c r="G4" s="18">
+        <v>0.31481481481481483</v>
+      </c>
+      <c r="H4" s="18">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="I4" s="18">
+        <v>0.35714285714285715</v>
+      </c>
+      <c r="J4" s="18">
+        <v>0.41304347826086957</v>
+      </c>
+      <c r="K4" s="18">
+        <v>0.62068965517241381</v>
+      </c>
+      <c r="L4" s="18">
+        <v>0.42307692307692307</v>
+      </c>
+      <c r="M4" s="18">
+        <v>0.65517241379310343</v>
+      </c>
+      <c r="N4" s="18">
+        <v>0.56097560975609762</v>
+      </c>
+      <c r="O4" s="18">
+        <v>0.46386946386946387</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" s="18">
+        <v>0.31034482758620691</v>
+      </c>
+      <c r="D5" s="18">
+        <v>0.26923076923076922</v>
+      </c>
+      <c r="E5" s="18">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="F5" s="18">
+        <v>0.3</v>
+      </c>
+      <c r="G5" s="18">
+        <v>0.32</v>
+      </c>
+      <c r="H5" s="18">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="I5" s="18">
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="J5" s="18">
+        <v>0.31707317073170732</v>
+      </c>
+      <c r="K5" s="18">
+        <v>0.2413793103448276</v>
+      </c>
+      <c r="L5" s="18">
+        <v>0.39130434782608697</v>
+      </c>
+      <c r="M5" s="18">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="N5" s="18">
+        <v>0.12820512820512819</v>
+      </c>
+      <c r="O5" s="18">
+        <v>0.26923076923076922</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="19"/>
+      <c r="B6" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" s="18">
+        <v>0.3235294117647059</v>
+      </c>
+      <c r="D6" s="18">
+        <v>0.25925925925925924</v>
+      </c>
+      <c r="E6" s="18">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="F6" s="18">
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="G6" s="18">
+        <v>0.29629629629629628</v>
+      </c>
+      <c r="H6" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="I6" s="18">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J6" s="18">
+        <v>0.28260869565217389</v>
+      </c>
+      <c r="K6" s="18">
+        <v>0.2413793103448276</v>
+      </c>
+      <c r="L6" s="18">
+        <v>0.34615384615384615</v>
+      </c>
+      <c r="M6" s="18">
+        <v>0.10344827586206896</v>
+      </c>
+      <c r="N6" s="18">
+        <v>0.12195121951219512</v>
+      </c>
+      <c r="O6" s="18">
+        <v>0.26107226107226106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" s="18">
+        <v>0.13793103448275862</v>
+      </c>
+      <c r="D7" s="18">
+        <v>0.19230769230769232</v>
+      </c>
+      <c r="E7" s="18">
+        <v>3.5714285714285712E-2</v>
+      </c>
+      <c r="F7" s="18">
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="G7" s="18">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H7" s="18">
+        <v>0.11428571428571428</v>
+      </c>
+      <c r="I7" s="18">
+        <v>6.0606060606060608E-2</v>
+      </c>
+      <c r="J7" s="18">
+        <v>0.12195121951219512</v>
+      </c>
+      <c r="K7" s="18">
+        <v>3.4482758620689655E-2</v>
+      </c>
+      <c r="L7" s="18">
+        <v>8.6956521739130432E-2</v>
+      </c>
+      <c r="M7" s="18">
+        <v>7.407407407407407E-2</v>
+      </c>
+      <c r="N7" s="18">
+        <v>0.17948717948717949</v>
+      </c>
+      <c r="O7" s="18">
+        <v>0.1076923076923077</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="19"/>
+      <c r="B8" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" s="18">
+        <v>0.11764705882352941</v>
+      </c>
+      <c r="D8" s="18">
+        <v>0.18518518518518517</v>
+      </c>
+      <c r="E8" s="18">
+        <v>3.5714285714285712E-2</v>
+      </c>
+      <c r="F8" s="18">
+        <v>6.0606060606060608E-2</v>
+      </c>
+      <c r="G8" s="18">
+        <v>0.12962962962962962</v>
+      </c>
+      <c r="H8" s="18">
+        <v>0.125</v>
+      </c>
+      <c r="I8" s="18">
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="J8" s="18">
+        <v>0.13043478260869565</v>
+      </c>
+      <c r="K8" s="18">
+        <v>3.4482758620689655E-2</v>
+      </c>
+      <c r="L8" s="18">
+        <v>0.11538461538461539</v>
+      </c>
+      <c r="M8" s="18">
+        <v>6.8965517241379309E-2</v>
+      </c>
+      <c r="N8" s="18">
+        <v>0.17073170731707318</v>
+      </c>
+      <c r="O8" s="18">
+        <v>0.10722610722610723</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9" s="18">
+        <v>0.20689655172413793</v>
+      </c>
+      <c r="D9" s="18">
+        <v>0.11538461538461539</v>
+      </c>
+      <c r="E9" s="18">
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="F9" s="18">
+        <v>0</v>
+      </c>
+      <c r="G9" s="18">
+        <v>0.02</v>
+      </c>
+      <c r="H9" s="18">
+        <v>0</v>
+      </c>
+      <c r="I9" s="18">
+        <v>0.15151515151515152</v>
+      </c>
+      <c r="J9" s="18">
+        <v>0.14634146341463414</v>
+      </c>
+      <c r="K9" s="18">
+        <v>3.4482758620689655E-2</v>
+      </c>
+      <c r="L9" s="18">
+        <v>4.3478260869565216E-2</v>
+      </c>
+      <c r="M9" s="18">
+        <v>0.14814814814814814</v>
+      </c>
+      <c r="N9" s="18">
+        <v>5.128205128205128E-2</v>
+      </c>
+      <c r="O9" s="18">
+        <v>7.9487179487179482E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="19"/>
+      <c r="B10" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C10" s="18">
+        <v>0.20588235294117646</v>
+      </c>
+      <c r="D10" s="18">
+        <v>0.14814814814814814</v>
+      </c>
+      <c r="E10" s="18">
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="F10" s="18">
+        <v>0</v>
+      </c>
+      <c r="G10" s="18">
+        <v>1.8518518518518517E-2</v>
+      </c>
+      <c r="H10" s="18">
+        <v>0</v>
+      </c>
+      <c r="I10" s="18">
+        <v>0.11904761904761904</v>
+      </c>
+      <c r="J10" s="18">
+        <v>0.17391304347826086</v>
+      </c>
+      <c r="K10" s="18">
+        <v>3.4482758620689655E-2</v>
+      </c>
+      <c r="L10" s="18">
+        <v>3.8461538461538464E-2</v>
+      </c>
+      <c r="M10" s="18">
+        <v>0.13793103448275862</v>
+      </c>
+      <c r="N10" s="18">
+        <v>4.878048780487805E-2</v>
+      </c>
+      <c r="O10" s="18">
+        <v>8.1585081585081584E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" s="18">
+        <v>3.4482758620689655E-2</v>
+      </c>
+      <c r="D11" s="18">
+        <v>0</v>
+      </c>
+      <c r="E11" s="18">
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="F11" s="18">
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="G11" s="18">
+        <v>0.26</v>
+      </c>
+      <c r="H11" s="18">
+        <v>2.8571428571428571E-2</v>
+      </c>
+      <c r="I11" s="18">
+        <v>0.15151515151515152</v>
+      </c>
+      <c r="J11" s="18">
+        <v>0</v>
+      </c>
+      <c r="K11" s="18">
+        <v>6.8965517241379309E-2</v>
+      </c>
+      <c r="L11" s="18">
+        <v>8.6956521739130432E-2</v>
+      </c>
+      <c r="M11" s="18">
+        <v>3.7037037037037035E-2</v>
+      </c>
+      <c r="N11" s="18">
+        <v>0.10256410256410256</v>
+      </c>
+      <c r="O11" s="18">
+        <v>8.461538461538462E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="19"/>
+      <c r="B12" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12" s="18">
+        <v>2.9411764705882353E-2</v>
+      </c>
+      <c r="D12" s="18">
+        <v>0</v>
+      </c>
+      <c r="E12" s="18">
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="F12" s="18">
+        <v>6.0606060606060608E-2</v>
+      </c>
+      <c r="G12" s="18">
+        <v>0.24074074074074073</v>
+      </c>
+      <c r="H12" s="18">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I12" s="18">
+        <v>0.11904761904761904</v>
+      </c>
+      <c r="J12" s="18">
+        <v>0</v>
+      </c>
+      <c r="K12" s="18">
+        <v>6.8965517241379309E-2</v>
+      </c>
+      <c r="L12" s="18">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="M12" s="18">
+        <v>3.4482758620689655E-2</v>
+      </c>
+      <c r="N12" s="18">
+        <v>9.7560975609756101E-2</v>
+      </c>
+      <c r="O12" s="18">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C13" s="18">
+        <v>0</v>
+      </c>
+      <c r="D13" s="18">
+        <v>0</v>
+      </c>
+      <c r="E13" s="18">
+        <v>0</v>
+      </c>
+      <c r="F13" s="18">
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="G13" s="18">
+        <v>0</v>
+      </c>
+      <c r="H13" s="18">
+        <v>5.7142857142857141E-2</v>
+      </c>
+      <c r="I13" s="18">
+        <v>0</v>
+      </c>
+      <c r="J13" s="18">
+        <v>0</v>
+      </c>
+      <c r="K13" s="18">
+        <v>0</v>
+      </c>
+      <c r="L13" s="18">
+        <v>0</v>
+      </c>
+      <c r="M13" s="18">
+        <v>0</v>
+      </c>
+      <c r="N13" s="18">
+        <v>0</v>
+      </c>
+      <c r="O13" s="18">
+        <v>7.6923076923076927E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="19"/>
+      <c r="B14" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C14" s="18">
+        <v>0</v>
+      </c>
+      <c r="D14" s="18">
+        <v>0</v>
+      </c>
+      <c r="E14" s="18">
+        <v>0</v>
+      </c>
+      <c r="F14" s="18">
+        <v>3.0303030303030304E-2</v>
+      </c>
+      <c r="G14" s="18">
+        <v>0</v>
+      </c>
+      <c r="H14" s="18">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="I14" s="18">
+        <v>0</v>
+      </c>
+      <c r="J14" s="18">
+        <v>0</v>
+      </c>
+      <c r="K14" s="18">
+        <v>0</v>
+      </c>
+      <c r="L14" s="18">
+        <v>0</v>
+      </c>
+      <c r="M14" s="18">
+        <v>0</v>
+      </c>
+      <c r="N14" s="18">
+        <v>0</v>
+      </c>
+      <c r="O14" s="18">
+        <v>9.324009324009324E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="C1:N1"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22BBA4D-C85A-4304-A112-5E7EF2BBD7F1}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="53.44140625" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" customWidth="1"/>
@@ -4589,4 +5335,3492 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{615EFB19-F474-4215-A4C4-27A7F36F1049}">
+  <dimension ref="A1:F164"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G158" sqref="G158"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>60</v>
+      </c>
+      <c r="D2">
+        <v>61</v>
+      </c>
+      <c r="E2">
+        <f>IF(D2-C2&gt;0,D2-C2,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <f>IF(D2-C2&lt;0,C2-D2,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3">
+        <v>60</v>
+      </c>
+      <c r="D3">
+        <v>56</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E66" si="0">IF(D3-C3&gt;0,D3-C3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F66" si="1">IF(D3-C3&lt;0,C3-D3,0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>60</v>
+      </c>
+      <c r="D4">
+        <v>68</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>60</v>
+      </c>
+      <c r="D5">
+        <v>67</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C6">
+        <v>60</v>
+      </c>
+      <c r="D6">
+        <v>52</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>60</v>
+      </c>
+      <c r="D7">
+        <v>67</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>60</v>
+      </c>
+      <c r="D8">
+        <v>79</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9">
+        <v>60</v>
+      </c>
+      <c r="D9">
+        <v>36</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>60</v>
+      </c>
+      <c r="D10">
+        <v>71</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>60</v>
+      </c>
+      <c r="D11">
+        <v>57</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>60</v>
+      </c>
+      <c r="D12">
+        <v>79</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>60</v>
+      </c>
+      <c r="D13">
+        <v>72</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>60</v>
+      </c>
+      <c r="D14">
+        <v>79</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>124</v>
+      </c>
+      <c r="C15">
+        <v>60</v>
+      </c>
+      <c r="D15">
+        <v>59</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>60</v>
+      </c>
+      <c r="D16">
+        <v>40</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>60</v>
+      </c>
+      <c r="D17">
+        <v>63</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>125</v>
+      </c>
+      <c r="C18">
+        <v>60</v>
+      </c>
+      <c r="D18">
+        <v>75</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>60</v>
+      </c>
+      <c r="D19">
+        <v>73</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>60</v>
+      </c>
+      <c r="D20">
+        <v>51</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C21">
+        <v>60</v>
+      </c>
+      <c r="D21">
+        <v>79</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>60</v>
+      </c>
+      <c r="D22">
+        <v>54</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23">
+        <v>60</v>
+      </c>
+      <c r="D23">
+        <v>54</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24">
+        <v>60</v>
+      </c>
+      <c r="D24">
+        <v>59</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25">
+        <v>60</v>
+      </c>
+      <c r="D25">
+        <v>75</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>60</v>
+      </c>
+      <c r="D26">
+        <v>58</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" t="s">
+        <v>124</v>
+      </c>
+      <c r="C27">
+        <v>60</v>
+      </c>
+      <c r="D27">
+        <v>63</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>60</v>
+      </c>
+      <c r="D28">
+        <v>48</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>60</v>
+      </c>
+      <c r="D29">
+        <v>51</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" t="s">
+        <v>125</v>
+      </c>
+      <c r="C30">
+        <v>60</v>
+      </c>
+      <c r="D30">
+        <v>69</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <v>60</v>
+      </c>
+      <c r="D31">
+        <v>72</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32">
+        <v>60</v>
+      </c>
+      <c r="D32">
+        <v>71</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" t="s">
+        <v>115</v>
+      </c>
+      <c r="C33">
+        <v>60</v>
+      </c>
+      <c r="D33">
+        <v>46</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34">
+        <v>60</v>
+      </c>
+      <c r="D34">
+        <v>60</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35">
+        <v>60</v>
+      </c>
+      <c r="D35">
+        <v>46</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36">
+        <v>60</v>
+      </c>
+      <c r="D36">
+        <v>63</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37">
+        <v>60</v>
+      </c>
+      <c r="D37">
+        <v>66</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>60</v>
+      </c>
+      <c r="D38">
+        <v>67</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39" t="s">
+        <v>124</v>
+      </c>
+      <c r="C39">
+        <v>60</v>
+      </c>
+      <c r="D39">
+        <v>75</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <v>60</v>
+      </c>
+      <c r="D40">
+        <v>32</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41">
+        <v>60</v>
+      </c>
+      <c r="D41">
+        <v>63</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" t="s">
+        <v>125</v>
+      </c>
+      <c r="C42">
+        <v>60</v>
+      </c>
+      <c r="D42">
+        <v>60</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>17</v>
+      </c>
+      <c r="B43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43">
+        <v>60</v>
+      </c>
+      <c r="D43">
+        <v>55</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>17</v>
+      </c>
+      <c r="B44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44">
+        <v>60</v>
+      </c>
+      <c r="D44">
+        <v>58</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45" t="s">
+        <v>115</v>
+      </c>
+      <c r="C45">
+        <v>60</v>
+      </c>
+      <c r="D45">
+        <v>52</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>17</v>
+      </c>
+      <c r="B46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46">
+        <v>60</v>
+      </c>
+      <c r="D46">
+        <v>68</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47">
+        <v>60</v>
+      </c>
+      <c r="D47">
+        <v>49</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>17</v>
+      </c>
+      <c r="B48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48">
+        <v>60</v>
+      </c>
+      <c r="D48">
+        <v>53</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>17</v>
+      </c>
+      <c r="B49" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49">
+        <v>60</v>
+      </c>
+      <c r="D49">
+        <v>50</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>17</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>60</v>
+      </c>
+      <c r="D50">
+        <v>58</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>18</v>
+      </c>
+      <c r="B51" t="s">
+        <v>124</v>
+      </c>
+      <c r="C51">
+        <v>440</v>
+      </c>
+      <c r="D51">
+        <v>446</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>18</v>
+      </c>
+      <c r="B52" t="s">
+        <v>2</v>
+      </c>
+      <c r="C52">
+        <v>440</v>
+      </c>
+      <c r="D52">
+        <v>437</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>18</v>
+      </c>
+      <c r="B53" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53">
+        <v>440</v>
+      </c>
+      <c r="D53">
+        <v>413</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>18</v>
+      </c>
+      <c r="B54" t="s">
+        <v>125</v>
+      </c>
+      <c r="C54">
+        <v>440</v>
+      </c>
+      <c r="D54">
+        <v>454</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>18</v>
+      </c>
+      <c r="B55" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55">
+        <v>440</v>
+      </c>
+      <c r="D55">
+        <v>436</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>18</v>
+      </c>
+      <c r="B56" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56">
+        <v>440</v>
+      </c>
+      <c r="D56">
+        <v>429</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>18</v>
+      </c>
+      <c r="B57" t="s">
+        <v>115</v>
+      </c>
+      <c r="C57">
+        <v>440</v>
+      </c>
+      <c r="D57">
+        <v>414</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>18</v>
+      </c>
+      <c r="B58" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58">
+        <v>440</v>
+      </c>
+      <c r="D58">
+        <v>402</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>18</v>
+      </c>
+      <c r="B59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59">
+        <v>440</v>
+      </c>
+      <c r="D59">
+        <v>459</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>18</v>
+      </c>
+      <c r="B60" t="s">
+        <v>10</v>
+      </c>
+      <c r="C60">
+        <v>440</v>
+      </c>
+      <c r="D60">
+        <v>403</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>18</v>
+      </c>
+      <c r="B61" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61">
+        <v>440</v>
+      </c>
+      <c r="D61">
+        <v>437</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>18</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>440</v>
+      </c>
+      <c r="D62">
+        <v>409</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>18</v>
+      </c>
+      <c r="B63" t="s">
+        <v>124</v>
+      </c>
+      <c r="C63">
+        <v>440</v>
+      </c>
+      <c r="D63">
+        <v>417</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>18</v>
+      </c>
+      <c r="B64" t="s">
+        <v>2</v>
+      </c>
+      <c r="C64">
+        <v>440</v>
+      </c>
+      <c r="D64">
+        <v>420</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>18</v>
+      </c>
+      <c r="B65" t="s">
+        <v>3</v>
+      </c>
+      <c r="C65">
+        <v>440</v>
+      </c>
+      <c r="D65">
+        <v>390</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>18</v>
+      </c>
+      <c r="B66" t="s">
+        <v>125</v>
+      </c>
+      <c r="C66">
+        <v>440</v>
+      </c>
+      <c r="D66">
+        <v>370</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>18</v>
+      </c>
+      <c r="B67" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67">
+        <v>440</v>
+      </c>
+      <c r="D67">
+        <v>412</v>
+      </c>
+      <c r="E67">
+        <f t="shared" ref="E67:E130" si="2">IF(D67-C67&gt;0,D67-C67,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <f t="shared" ref="F67:F130" si="3">IF(D67-C67&lt;0,C67-D67,0)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>18</v>
+      </c>
+      <c r="B68" t="s">
+        <v>6</v>
+      </c>
+      <c r="C68">
+        <v>440</v>
+      </c>
+      <c r="D68">
+        <v>391</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>18</v>
+      </c>
+      <c r="B69" t="s">
+        <v>115</v>
+      </c>
+      <c r="C69">
+        <v>440</v>
+      </c>
+      <c r="D69">
+        <v>383</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <f t="shared" si="3"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>18</v>
+      </c>
+      <c r="B70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C70">
+        <v>440</v>
+      </c>
+      <c r="D70">
+        <v>421</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>18</v>
+      </c>
+      <c r="B71" t="s">
+        <v>9</v>
+      </c>
+      <c r="C71">
+        <v>440</v>
+      </c>
+      <c r="D71">
+        <v>374</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="3"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>18</v>
+      </c>
+      <c r="B72" t="s">
+        <v>10</v>
+      </c>
+      <c r="C72">
+        <v>440</v>
+      </c>
+      <c r="D72">
+        <v>417</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>18</v>
+      </c>
+      <c r="B73" t="s">
+        <v>11</v>
+      </c>
+      <c r="C73">
+        <v>440</v>
+      </c>
+      <c r="D73">
+        <v>448</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>18</v>
+      </c>
+      <c r="B74" t="s">
+        <v>1</v>
+      </c>
+      <c r="C74">
+        <v>440</v>
+      </c>
+      <c r="D74">
+        <v>461</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="F74">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>18</v>
+      </c>
+      <c r="B75" t="s">
+        <v>124</v>
+      </c>
+      <c r="C75">
+        <v>440</v>
+      </c>
+      <c r="D75">
+        <v>397</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>18</v>
+      </c>
+      <c r="B76" t="s">
+        <v>2</v>
+      </c>
+      <c r="C76">
+        <v>440</v>
+      </c>
+      <c r="D76">
+        <v>428</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>18</v>
+      </c>
+      <c r="B77" t="s">
+        <v>3</v>
+      </c>
+      <c r="C77">
+        <v>440</v>
+      </c>
+      <c r="D77">
+        <v>419</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>18</v>
+      </c>
+      <c r="B78" t="s">
+        <v>125</v>
+      </c>
+      <c r="C78">
+        <v>440</v>
+      </c>
+      <c r="D78">
+        <v>413</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F78">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>18</v>
+      </c>
+      <c r="B79" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79">
+        <v>440</v>
+      </c>
+      <c r="D79">
+        <v>435</v>
+      </c>
+      <c r="E79">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F79">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>18</v>
+      </c>
+      <c r="B80" t="s">
+        <v>6</v>
+      </c>
+      <c r="C80">
+        <v>440</v>
+      </c>
+      <c r="D80">
+        <v>451</v>
+      </c>
+      <c r="E80">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="F80">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>18</v>
+      </c>
+      <c r="B81" t="s">
+        <v>115</v>
+      </c>
+      <c r="C81">
+        <v>440</v>
+      </c>
+      <c r="D81">
+        <v>436</v>
+      </c>
+      <c r="E81">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F81">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>18</v>
+      </c>
+      <c r="B82" t="s">
+        <v>8</v>
+      </c>
+      <c r="C82">
+        <v>440</v>
+      </c>
+      <c r="D82">
+        <v>385</v>
+      </c>
+      <c r="E82">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F82">
+        <f t="shared" si="3"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>18</v>
+      </c>
+      <c r="B83" t="s">
+        <v>9</v>
+      </c>
+      <c r="C83">
+        <v>440</v>
+      </c>
+      <c r="D83">
+        <v>397</v>
+      </c>
+      <c r="E83">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F83">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>18</v>
+      </c>
+      <c r="B84" t="s">
+        <v>10</v>
+      </c>
+      <c r="C84">
+        <v>440</v>
+      </c>
+      <c r="D84">
+        <v>429</v>
+      </c>
+      <c r="E84">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F84">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>18</v>
+      </c>
+      <c r="B85" t="s">
+        <v>11</v>
+      </c>
+      <c r="C85">
+        <v>440</v>
+      </c>
+      <c r="D85">
+        <v>392</v>
+      </c>
+      <c r="E85">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F85">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>18</v>
+      </c>
+      <c r="B86" t="s">
+        <v>1</v>
+      </c>
+      <c r="C86">
+        <v>440</v>
+      </c>
+      <c r="D86">
+        <v>385</v>
+      </c>
+      <c r="E86">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F86">
+        <f t="shared" si="3"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>18</v>
+      </c>
+      <c r="B87" t="s">
+        <v>124</v>
+      </c>
+      <c r="C87">
+        <v>440</v>
+      </c>
+      <c r="D87">
+        <v>433</v>
+      </c>
+      <c r="E87">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F87">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>18</v>
+      </c>
+      <c r="B88" t="s">
+        <v>2</v>
+      </c>
+      <c r="C88">
+        <v>440</v>
+      </c>
+      <c r="D88">
+        <v>472</v>
+      </c>
+      <c r="E88">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="F88">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>18</v>
+      </c>
+      <c r="B89" t="s">
+        <v>3</v>
+      </c>
+      <c r="C89">
+        <v>440</v>
+      </c>
+      <c r="D89">
+        <v>403</v>
+      </c>
+      <c r="E89">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F89">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>18</v>
+      </c>
+      <c r="B90" t="s">
+        <v>125</v>
+      </c>
+      <c r="C90">
+        <v>440</v>
+      </c>
+      <c r="D90">
+        <v>365</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F90">
+        <f t="shared" si="3"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>18</v>
+      </c>
+      <c r="B91" t="s">
+        <v>5</v>
+      </c>
+      <c r="C91">
+        <v>440</v>
+      </c>
+      <c r="D91">
+        <v>403</v>
+      </c>
+      <c r="E91">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F91">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>18</v>
+      </c>
+      <c r="B92" t="s">
+        <v>6</v>
+      </c>
+      <c r="C92">
+        <v>440</v>
+      </c>
+      <c r="D92">
+        <v>427</v>
+      </c>
+      <c r="E92">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F92">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>18</v>
+      </c>
+      <c r="B93" t="s">
+        <v>115</v>
+      </c>
+      <c r="C93">
+        <v>440</v>
+      </c>
+      <c r="D93">
+        <v>432</v>
+      </c>
+      <c r="E93">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F93">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>18</v>
+      </c>
+      <c r="B94" t="s">
+        <v>8</v>
+      </c>
+      <c r="C94">
+        <v>440</v>
+      </c>
+      <c r="D94">
+        <v>419</v>
+      </c>
+      <c r="E94">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F94">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>18</v>
+      </c>
+      <c r="B95" t="s">
+        <v>9</v>
+      </c>
+      <c r="C95">
+        <v>440</v>
+      </c>
+      <c r="D95">
+        <v>415</v>
+      </c>
+      <c r="E95">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F95">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>18</v>
+      </c>
+      <c r="B96" t="s">
+        <v>10</v>
+      </c>
+      <c r="C96">
+        <v>440</v>
+      </c>
+      <c r="D96">
+        <v>379</v>
+      </c>
+      <c r="E96">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F96">
+        <f t="shared" si="3"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>18</v>
+      </c>
+      <c r="B97" t="s">
+        <v>11</v>
+      </c>
+      <c r="C97">
+        <v>440</v>
+      </c>
+      <c r="D97">
+        <v>430</v>
+      </c>
+      <c r="E97">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F97">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>18</v>
+      </c>
+      <c r="B98" t="s">
+        <v>1</v>
+      </c>
+      <c r="C98">
+        <v>440</v>
+      </c>
+      <c r="D98">
+        <v>410</v>
+      </c>
+      <c r="E98">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F98">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>18</v>
+      </c>
+      <c r="B99" t="s">
+        <v>124</v>
+      </c>
+      <c r="C99">
+        <v>440</v>
+      </c>
+      <c r="D99">
+        <v>393</v>
+      </c>
+      <c r="E99">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F99">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>18</v>
+      </c>
+      <c r="B100" t="s">
+        <v>2</v>
+      </c>
+      <c r="C100">
+        <v>440</v>
+      </c>
+      <c r="D100">
+        <v>446</v>
+      </c>
+      <c r="E100">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="F100">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>19</v>
+      </c>
+      <c r="B101" t="s">
+        <v>3</v>
+      </c>
+      <c r="C101">
+        <v>120</v>
+      </c>
+      <c r="D101">
+        <v>166</v>
+      </c>
+      <c r="E101">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="F101">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>19</v>
+      </c>
+      <c r="B102" t="s">
+        <v>125</v>
+      </c>
+      <c r="C102">
+        <v>120</v>
+      </c>
+      <c r="D102">
+        <v>135</v>
+      </c>
+      <c r="E102">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="F102">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>19</v>
+      </c>
+      <c r="B103" t="s">
+        <v>5</v>
+      </c>
+      <c r="C103">
+        <v>120</v>
+      </c>
+      <c r="D103">
+        <v>149</v>
+      </c>
+      <c r="E103">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="F103">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>19</v>
+      </c>
+      <c r="B104" t="s">
+        <v>6</v>
+      </c>
+      <c r="C104">
+        <v>120</v>
+      </c>
+      <c r="D104">
+        <v>116</v>
+      </c>
+      <c r="E104">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F104">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>19</v>
+      </c>
+      <c r="B105" t="s">
+        <v>115</v>
+      </c>
+      <c r="C105">
+        <v>120</v>
+      </c>
+      <c r="D105">
+        <v>155</v>
+      </c>
+      <c r="E105">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="F105">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>19</v>
+      </c>
+      <c r="B106" t="s">
+        <v>8</v>
+      </c>
+      <c r="C106">
+        <v>120</v>
+      </c>
+      <c r="D106">
+        <v>137</v>
+      </c>
+      <c r="E106">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="F106">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>19</v>
+      </c>
+      <c r="B107" t="s">
+        <v>9</v>
+      </c>
+      <c r="C107">
+        <v>120</v>
+      </c>
+      <c r="D107">
+        <v>175</v>
+      </c>
+      <c r="E107">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="F107">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>19</v>
+      </c>
+      <c r="B108" t="s">
+        <v>10</v>
+      </c>
+      <c r="C108">
+        <v>120</v>
+      </c>
+      <c r="D108">
+        <v>181</v>
+      </c>
+      <c r="E108">
+        <f t="shared" si="2"/>
+        <v>61</v>
+      </c>
+      <c r="F108">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>19</v>
+      </c>
+      <c r="B109" t="s">
+        <v>11</v>
+      </c>
+      <c r="C109">
+        <v>120</v>
+      </c>
+      <c r="D109">
+        <v>210</v>
+      </c>
+      <c r="E109">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="F109">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>19</v>
+      </c>
+      <c r="B110" t="s">
+        <v>1</v>
+      </c>
+      <c r="C110">
+        <v>120</v>
+      </c>
+      <c r="D110">
+        <v>152</v>
+      </c>
+      <c r="E110">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="F110">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>19</v>
+      </c>
+      <c r="B111" t="s">
+        <v>124</v>
+      </c>
+      <c r="C111">
+        <v>120</v>
+      </c>
+      <c r="D111">
+        <v>172</v>
+      </c>
+      <c r="E111">
+        <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
+      <c r="F111">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>19</v>
+      </c>
+      <c r="B112" t="s">
+        <v>2</v>
+      </c>
+      <c r="C112">
+        <v>120</v>
+      </c>
+      <c r="D112">
+        <v>170</v>
+      </c>
+      <c r="E112">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="F112">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>19</v>
+      </c>
+      <c r="B113" t="s">
+        <v>3</v>
+      </c>
+      <c r="C113">
+        <v>120</v>
+      </c>
+      <c r="D113">
+        <v>146</v>
+      </c>
+      <c r="E113">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="F113">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>19</v>
+      </c>
+      <c r="B114" t="s">
+        <v>125</v>
+      </c>
+      <c r="C114">
+        <v>120</v>
+      </c>
+      <c r="D114">
+        <v>146</v>
+      </c>
+      <c r="E114">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="F114">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>19</v>
+      </c>
+      <c r="B115" t="s">
+        <v>5</v>
+      </c>
+      <c r="C115">
+        <v>120</v>
+      </c>
+      <c r="D115">
+        <v>130</v>
+      </c>
+      <c r="E115">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="F115">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>19</v>
+      </c>
+      <c r="B116" t="s">
+        <v>6</v>
+      </c>
+      <c r="C116">
+        <v>120</v>
+      </c>
+      <c r="D116">
+        <v>112</v>
+      </c>
+      <c r="E116">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F116">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>19</v>
+      </c>
+      <c r="B117" t="s">
+        <v>115</v>
+      </c>
+      <c r="C117">
+        <v>120</v>
+      </c>
+      <c r="D117">
+        <v>150</v>
+      </c>
+      <c r="E117">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F117">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>19</v>
+      </c>
+      <c r="B118" t="s">
+        <v>8</v>
+      </c>
+      <c r="C118">
+        <v>120</v>
+      </c>
+      <c r="D118">
+        <v>118</v>
+      </c>
+      <c r="E118">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F118">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>19</v>
+      </c>
+      <c r="B119" t="s">
+        <v>9</v>
+      </c>
+      <c r="C119">
+        <v>120</v>
+      </c>
+      <c r="D119">
+        <v>163</v>
+      </c>
+      <c r="E119">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="F119">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>19</v>
+      </c>
+      <c r="B120" t="s">
+        <v>10</v>
+      </c>
+      <c r="C120">
+        <v>120</v>
+      </c>
+      <c r="D120">
+        <v>131</v>
+      </c>
+      <c r="E120">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="F120">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>19</v>
+      </c>
+      <c r="B121" t="s">
+        <v>11</v>
+      </c>
+      <c r="C121">
+        <v>120</v>
+      </c>
+      <c r="D121">
+        <v>88</v>
+      </c>
+      <c r="E121">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F121">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>19</v>
+      </c>
+      <c r="B122" t="s">
+        <v>1</v>
+      </c>
+      <c r="C122">
+        <v>120</v>
+      </c>
+      <c r="D122">
+        <v>137</v>
+      </c>
+      <c r="E122">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="F122">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>19</v>
+      </c>
+      <c r="B123" t="s">
+        <v>124</v>
+      </c>
+      <c r="C123">
+        <v>120</v>
+      </c>
+      <c r="D123">
+        <v>136</v>
+      </c>
+      <c r="E123">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="F123">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>19</v>
+      </c>
+      <c r="B124" t="s">
+        <v>2</v>
+      </c>
+      <c r="C124">
+        <v>120</v>
+      </c>
+      <c r="D124">
+        <v>155</v>
+      </c>
+      <c r="E124">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="F124">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>19</v>
+      </c>
+      <c r="B125" t="s">
+        <v>3</v>
+      </c>
+      <c r="C125">
+        <v>120</v>
+      </c>
+      <c r="D125">
+        <v>166</v>
+      </c>
+      <c r="E125">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="F125">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>19</v>
+      </c>
+      <c r="B126" t="s">
+        <v>125</v>
+      </c>
+      <c r="C126">
+        <v>120</v>
+      </c>
+      <c r="D126">
+        <v>95</v>
+      </c>
+      <c r="E126">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F126">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>19</v>
+      </c>
+      <c r="B127" t="s">
+        <v>5</v>
+      </c>
+      <c r="C127">
+        <v>120</v>
+      </c>
+      <c r="D127">
+        <v>133</v>
+      </c>
+      <c r="E127">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="F127">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>19</v>
+      </c>
+      <c r="B128" t="s">
+        <v>6</v>
+      </c>
+      <c r="C128">
+        <v>120</v>
+      </c>
+      <c r="D128">
+        <v>131</v>
+      </c>
+      <c r="E128">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="F128">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>19</v>
+      </c>
+      <c r="B129" t="s">
+        <v>115</v>
+      </c>
+      <c r="C129">
+        <v>120</v>
+      </c>
+      <c r="D129">
+        <v>185</v>
+      </c>
+      <c r="E129">
+        <f t="shared" si="2"/>
+        <v>65</v>
+      </c>
+      <c r="F129">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>19</v>
+      </c>
+      <c r="B130" t="s">
+        <v>8</v>
+      </c>
+      <c r="C130">
+        <v>120</v>
+      </c>
+      <c r="D130">
+        <v>150</v>
+      </c>
+      <c r="E130">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F130">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>19</v>
+      </c>
+      <c r="B131" t="s">
+        <v>9</v>
+      </c>
+      <c r="C131">
+        <v>120</v>
+      </c>
+      <c r="D131">
+        <v>111</v>
+      </c>
+      <c r="E131">
+        <f t="shared" ref="E131:E150" si="4">IF(D131-C131&gt;0,D131-C131,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F131">
+        <f t="shared" ref="F131:F150" si="5">IF(D131-C131&lt;0,C131-D131,0)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>19</v>
+      </c>
+      <c r="B132" t="s">
+        <v>10</v>
+      </c>
+      <c r="C132">
+        <v>120</v>
+      </c>
+      <c r="D132">
+        <v>172</v>
+      </c>
+      <c r="E132">
+        <f t="shared" si="4"/>
+        <v>52</v>
+      </c>
+      <c r="F132">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>19</v>
+      </c>
+      <c r="B133" t="s">
+        <v>11</v>
+      </c>
+      <c r="C133">
+        <v>120</v>
+      </c>
+      <c r="D133">
+        <v>180</v>
+      </c>
+      <c r="E133">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+      <c r="F133">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>19</v>
+      </c>
+      <c r="B134" t="s">
+        <v>1</v>
+      </c>
+      <c r="C134">
+        <v>120</v>
+      </c>
+      <c r="D134">
+        <v>163</v>
+      </c>
+      <c r="E134">
+        <f t="shared" si="4"/>
+        <v>43</v>
+      </c>
+      <c r="F134">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>19</v>
+      </c>
+      <c r="B135" t="s">
+        <v>124</v>
+      </c>
+      <c r="C135">
+        <v>120</v>
+      </c>
+      <c r="D135">
+        <v>152</v>
+      </c>
+      <c r="E135">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+      <c r="F135">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>19</v>
+      </c>
+      <c r="B136" t="s">
+        <v>2</v>
+      </c>
+      <c r="C136">
+        <v>120</v>
+      </c>
+      <c r="D136">
+        <v>120</v>
+      </c>
+      <c r="E136">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F136">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>19</v>
+      </c>
+      <c r="B137" t="s">
+        <v>3</v>
+      </c>
+      <c r="C137">
+        <v>120</v>
+      </c>
+      <c r="D137">
+        <v>201</v>
+      </c>
+      <c r="E137">
+        <f t="shared" si="4"/>
+        <v>81</v>
+      </c>
+      <c r="F137">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>19</v>
+      </c>
+      <c r="B138" t="s">
+        <v>125</v>
+      </c>
+      <c r="C138">
+        <v>120</v>
+      </c>
+      <c r="D138">
+        <v>150</v>
+      </c>
+      <c r="E138">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="F138">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>19</v>
+      </c>
+      <c r="B139" t="s">
+        <v>5</v>
+      </c>
+      <c r="C139">
+        <v>120</v>
+      </c>
+      <c r="D139">
+        <v>191</v>
+      </c>
+      <c r="E139">
+        <f t="shared" si="4"/>
+        <v>71</v>
+      </c>
+      <c r="F139">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>19</v>
+      </c>
+      <c r="B140" t="s">
+        <v>6</v>
+      </c>
+      <c r="C140">
+        <v>120</v>
+      </c>
+      <c r="D140">
+        <v>185</v>
+      </c>
+      <c r="E140">
+        <f t="shared" si="4"/>
+        <v>65</v>
+      </c>
+      <c r="F140">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>19</v>
+      </c>
+      <c r="B141" t="s">
+        <v>115</v>
+      </c>
+      <c r="C141">
+        <v>120</v>
+      </c>
+      <c r="D141">
+        <v>194</v>
+      </c>
+      <c r="E141">
+        <f t="shared" si="4"/>
+        <v>74</v>
+      </c>
+      <c r="F141">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>19</v>
+      </c>
+      <c r="B142" t="s">
+        <v>8</v>
+      </c>
+      <c r="C142">
+        <v>120</v>
+      </c>
+      <c r="D142">
+        <v>93</v>
+      </c>
+      <c r="E142">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F142">
+        <f t="shared" si="5"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>19</v>
+      </c>
+      <c r="B143" t="s">
+        <v>9</v>
+      </c>
+      <c r="C143">
+        <v>120</v>
+      </c>
+      <c r="D143">
+        <v>213</v>
+      </c>
+      <c r="E143">
+        <f t="shared" si="4"/>
+        <v>93</v>
+      </c>
+      <c r="F143">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>19</v>
+      </c>
+      <c r="B144" t="s">
+        <v>10</v>
+      </c>
+      <c r="C144">
+        <v>120</v>
+      </c>
+      <c r="D144">
+        <v>104</v>
+      </c>
+      <c r="E144">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F144">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>19</v>
+      </c>
+      <c r="B145" t="s">
+        <v>11</v>
+      </c>
+      <c r="C145">
+        <v>120</v>
+      </c>
+      <c r="D145">
+        <v>128</v>
+      </c>
+      <c r="E145">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="F145">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>19</v>
+      </c>
+      <c r="B146" t="s">
+        <v>1</v>
+      </c>
+      <c r="C146">
+        <v>120</v>
+      </c>
+      <c r="D146">
+        <v>165</v>
+      </c>
+      <c r="E146">
+        <f t="shared" si="4"/>
+        <v>45</v>
+      </c>
+      <c r="F146">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>19</v>
+      </c>
+      <c r="B147" t="s">
+        <v>124</v>
+      </c>
+      <c r="C147">
+        <v>120</v>
+      </c>
+      <c r="D147">
+        <v>118</v>
+      </c>
+      <c r="E147">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F147">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>19</v>
+      </c>
+      <c r="B148" t="s">
+        <v>2</v>
+      </c>
+      <c r="C148">
+        <v>120</v>
+      </c>
+      <c r="D148">
+        <v>197</v>
+      </c>
+      <c r="E148">
+        <f t="shared" si="4"/>
+        <v>77</v>
+      </c>
+      <c r="F148">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>19</v>
+      </c>
+      <c r="B149" t="s">
+        <v>3</v>
+      </c>
+      <c r="C149">
+        <v>120</v>
+      </c>
+      <c r="D149">
+        <v>134</v>
+      </c>
+      <c r="E149">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="F149">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>19</v>
+      </c>
+      <c r="B150" t="s">
+        <v>125</v>
+      </c>
+      <c r="C150">
+        <v>120</v>
+      </c>
+      <c r="D150">
+        <v>122</v>
+      </c>
+      <c r="E150">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F150">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D151" t="s">
+        <v>123</v>
+      </c>
+      <c r="E151">
+        <f>SUM(E2:E150)</f>
+        <v>1970</v>
+      </c>
+      <c r="F151">
+        <f>SUM(F2:F150)</f>
+        <v>1611</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D153" t="s">
+        <v>1</v>
+      </c>
+      <c r="E153">
+        <f>SUMIF(B2:B150,D153,E2:E150)</f>
+        <v>185</v>
+      </c>
+      <c r="F153">
+        <f>SUMIF(B2:B150,D153,F2:F150)</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D154" t="s">
+        <v>124</v>
+      </c>
+      <c r="E154">
+        <f t="shared" ref="E154:F164" si="6">SUMIF(B3:B151,D154,E3:E151)</f>
+        <v>124</v>
+      </c>
+      <c r="F154">
+        <f t="shared" ref="F154:F164" si="7">SUMIF(B3:B151,D154,F3:F151)</f>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D155" t="s">
+        <v>2</v>
+      </c>
+      <c r="E155">
+        <f t="shared" si="6"/>
+        <v>208</v>
+      </c>
+      <c r="F155">
+        <f t="shared" si="7"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D156" t="s">
+        <v>3</v>
+      </c>
+      <c r="E156">
+        <f t="shared" si="6"/>
+        <v>226</v>
+      </c>
+      <c r="F156">
+        <f t="shared" si="7"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D157" t="s">
+        <v>125</v>
+      </c>
+      <c r="E157">
+        <f t="shared" si="6"/>
+        <v>111</v>
+      </c>
+      <c r="F157">
+        <f t="shared" si="7"/>
+        <v>205</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D158" t="s">
+        <v>5</v>
+      </c>
+      <c r="E158">
+        <f t="shared" si="6"/>
+        <v>155</v>
+      </c>
+      <c r="F158">
+        <f t="shared" si="7"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D159" t="s">
+        <v>6</v>
+      </c>
+      <c r="E159">
+        <f t="shared" si="6"/>
+        <v>117</v>
+      </c>
+      <c r="F159">
+        <f t="shared" si="7"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D160" t="s">
+        <v>115</v>
+      </c>
+      <c r="E160">
+        <f t="shared" si="6"/>
+        <v>223</v>
+      </c>
+      <c r="F160">
+        <f t="shared" si="7"/>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="161" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D161" t="s">
+        <v>8</v>
+      </c>
+      <c r="E161">
+        <f t="shared" si="6"/>
+        <v>66</v>
+      </c>
+      <c r="F161">
+        <f t="shared" si="7"/>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="162" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D162" t="s">
+        <v>9</v>
+      </c>
+      <c r="E162">
+        <f t="shared" si="6"/>
+        <v>210</v>
+      </c>
+      <c r="F162">
+        <f t="shared" si="7"/>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="163" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D163" t="s">
+        <v>10</v>
+      </c>
+      <c r="E163">
+        <f t="shared" si="6"/>
+        <v>146</v>
+      </c>
+      <c r="F163">
+        <f t="shared" si="7"/>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="164" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D164" t="s">
+        <v>11</v>
+      </c>
+      <c r="E164">
+        <f t="shared" si="6"/>
+        <v>199</v>
+      </c>
+      <c r="F164">
+        <f t="shared" si="7"/>
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
se actualiza grafico de barra en suspensiones.
</commit_message>
<xml_diff>
--- a/app_salud/app/logic/data/set_de_datos_1.xlsx
+++ b/app_salud/app/logic/data/set_de_datos_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rstudio\software_salud\app_salud\app\logic\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\documentos juan\Salud\software_salud\app_salud\app\logic\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8707F22-8D35-452A-8175-E929C2622363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C9CDF3-2699-4922-AF22-B3F5BB587103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{A035267E-5D3E-4097-B788-79B64BEF5509}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="947" activeTab="4" xr2:uid="{A035267E-5D3E-4097-B788-79B64BEF5509}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1237" uniqueCount="139">
   <si>
     <t>Febrero</t>
   </si>
@@ -448,6 +448,15 @@
   </si>
   <si>
     <t>INFRAESTRUCTURA</t>
+  </si>
+  <si>
+    <t>porcentaje</t>
+  </si>
+  <si>
+    <t>Causa de suspension</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
   </si>
 </sst>
 </file>
@@ -538,7 +547,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -565,34 +574,43 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{E3156AE8-1855-485A-AE3C-7436025EFAA8}"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -657,7 +675,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -959,7 +977,7 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" customWidth="1"/>
@@ -1173,7 +1191,7 @@
       <selection activeCell="B148" sqref="B148"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.88671875" customWidth="1"/>
   </cols>
@@ -2391,7 +2409,7 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="31" customWidth="1"/>
     <col min="3" max="3" width="20.5546875" customWidth="1"/>
@@ -2838,11 +2856,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9808375D-D5D5-4E71-A87A-5B28F2320F53}">
   <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E37"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="36.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.109375" bestFit="1" customWidth="1"/>
@@ -2892,7 +2910,7 @@
       <c r="M1" s="9"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="18" t="s">
         <v>101</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -2930,7 +2948,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="4" t="s">
         <v>104</v>
       </c>
@@ -2966,7 +2984,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="4" t="s">
         <v>105</v>
       </c>
@@ -3002,7 +3020,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="4" t="s">
         <v>106</v>
       </c>
@@ -3038,7 +3056,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="4" t="s">
         <v>107</v>
       </c>
@@ -3074,7 +3092,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="4" t="s">
         <v>108</v>
       </c>
@@ -3110,7 +3128,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="4" t="s">
         <v>109</v>
       </c>
@@ -3146,7 +3164,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="4" t="s">
         <v>110</v>
       </c>
@@ -3182,7 +3200,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="4" t="s">
         <v>111</v>
       </c>
@@ -3218,7 +3236,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
+      <c r="A11" s="18"/>
       <c r="B11" s="4" t="s">
         <v>112</v>
       </c>
@@ -3254,7 +3272,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="4" t="s">
         <v>113</v>
       </c>
@@ -3290,13 +3308,13 @@
       </c>
     </row>
     <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="18" t="s">
         <v>52</v>
       </c>
       <c r="D13" s="5">
@@ -4086,17 +4104,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7253C5DD-76E0-4DAF-B9AF-4AE6D659DCEE}">
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:O160"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.77734375" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="14"/>
-      <c r="B1" s="14"/>
+      <c r="A1" s="13"/>
+      <c r="B1" s="13"/>
       <c r="C1" s="20" t="s">
         <v>101</v>
       </c>
@@ -4115,45 +4138,47 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="48" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:15" ht="48.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="16" t="s">
+      <c r="B2" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="J2" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="L2" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="M2" s="16" t="s">
+      <c r="M2" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="N2" s="15" t="s">
         <v>127</v>
       </c>
       <c r="O2" s="20" t="s">
@@ -4164,91 +4189,91 @@
       <c r="A3" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="17">
         <v>0.31034482758620691</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="17">
         <v>0.42307692307692307</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="17">
         <v>0.5357142857142857</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="17">
         <v>0.53333333333333333</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G3" s="17">
         <v>0.26</v>
       </c>
-      <c r="H3" s="18">
+      <c r="H3" s="17">
         <v>0.51428571428571423</v>
       </c>
-      <c r="I3" s="18">
+      <c r="I3" s="17">
         <v>0.36363636363636365</v>
       </c>
-      <c r="J3" s="18">
+      <c r="J3" s="17">
         <v>0.41463414634146339</v>
       </c>
-      <c r="K3" s="18">
+      <c r="K3" s="17">
         <v>0.62068965517241381</v>
       </c>
-      <c r="L3" s="18">
+      <c r="L3" s="17">
         <v>0.39130434782608697</v>
       </c>
-      <c r="M3" s="18">
+      <c r="M3" s="17">
         <v>0.62962962962962965</v>
       </c>
-      <c r="N3" s="18">
+      <c r="N3" s="17">
         <v>0.53846153846153844</v>
       </c>
-      <c r="O3" s="18">
+      <c r="O3" s="17">
         <v>0.45128205128205129</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="19"/>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="17">
         <v>0.3235294117647059</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="17">
         <v>0.40740740740740738</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="17">
         <v>0.5357142857142857</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="17">
         <v>0.5757575757575758</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="17">
         <v>0.31481481481481483</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H4" s="17">
         <v>0.52500000000000002</v>
       </c>
-      <c r="I4" s="18">
+      <c r="I4" s="17">
         <v>0.35714285714285715</v>
       </c>
-      <c r="J4" s="18">
+      <c r="J4" s="17">
         <v>0.41304347826086957</v>
       </c>
-      <c r="K4" s="18">
+      <c r="K4" s="17">
         <v>0.62068965517241381</v>
       </c>
-      <c r="L4" s="18">
+      <c r="L4" s="17">
         <v>0.42307692307692307</v>
       </c>
-      <c r="M4" s="18">
+      <c r="M4" s="17">
         <v>0.65517241379310343</v>
       </c>
-      <c r="N4" s="18">
+      <c r="N4" s="17">
         <v>0.56097560975609762</v>
       </c>
-      <c r="O4" s="18">
+      <c r="O4" s="17">
         <v>0.46386946386946387</v>
       </c>
     </row>
@@ -4256,91 +4281,91 @@
       <c r="A5" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="17">
         <v>0.31034482758620691</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="17">
         <v>0.26923076923076922</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="17">
         <v>0.2857142857142857</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="17">
         <v>0.3</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="17">
         <v>0.32</v>
       </c>
-      <c r="H5" s="18">
+      <c r="H5" s="17">
         <v>0.2857142857142857</v>
       </c>
-      <c r="I5" s="18">
+      <c r="I5" s="17">
         <v>0.27272727272727271</v>
       </c>
-      <c r="J5" s="18">
+      <c r="J5" s="17">
         <v>0.31707317073170732</v>
       </c>
-      <c r="K5" s="18">
+      <c r="K5" s="17">
         <v>0.2413793103448276</v>
       </c>
-      <c r="L5" s="18">
+      <c r="L5" s="17">
         <v>0.39130434782608697</v>
       </c>
-      <c r="M5" s="18">
+      <c r="M5" s="17">
         <v>0.1111111111111111</v>
       </c>
-      <c r="N5" s="18">
+      <c r="N5" s="17">
         <v>0.12820512820512819</v>
       </c>
-      <c r="O5" s="18">
+      <c r="O5" s="17">
         <v>0.26923076923076922</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="19"/>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="17">
         <v>0.3235294117647059</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="17">
         <v>0.25925925925925924</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="17">
         <v>0.2857142857142857</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="17">
         <v>0.27272727272727271</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="17">
         <v>0.29629629629629628</v>
       </c>
-      <c r="H6" s="18">
+      <c r="H6" s="17">
         <v>0.25</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="17">
         <v>0.33333333333333331</v>
       </c>
-      <c r="J6" s="18">
+      <c r="J6" s="17">
         <v>0.28260869565217389</v>
       </c>
-      <c r="K6" s="18">
+      <c r="K6" s="17">
         <v>0.2413793103448276</v>
       </c>
-      <c r="L6" s="18">
+      <c r="L6" s="17">
         <v>0.34615384615384615</v>
       </c>
-      <c r="M6" s="18">
+      <c r="M6" s="17">
         <v>0.10344827586206896</v>
       </c>
-      <c r="N6" s="18">
+      <c r="N6" s="17">
         <v>0.12195121951219512</v>
       </c>
-      <c r="O6" s="18">
+      <c r="O6" s="17">
         <v>0.26107226107226106</v>
       </c>
     </row>
@@ -4348,91 +4373,91 @@
       <c r="A7" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="17">
         <v>0.13793103448275862</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="17">
         <v>0.19230769230769232</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="17">
         <v>3.5714285714285712E-2</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="17">
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="17">
         <v>0.14000000000000001</v>
       </c>
-      <c r="H7" s="18">
+      <c r="H7" s="17">
         <v>0.11428571428571428</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="17">
         <v>6.0606060606060608E-2</v>
       </c>
-      <c r="J7" s="18">
+      <c r="J7" s="17">
         <v>0.12195121951219512</v>
       </c>
-      <c r="K7" s="18">
+      <c r="K7" s="17">
         <v>3.4482758620689655E-2</v>
       </c>
-      <c r="L7" s="18">
+      <c r="L7" s="17">
         <v>8.6956521739130432E-2</v>
       </c>
-      <c r="M7" s="18">
+      <c r="M7" s="17">
         <v>7.407407407407407E-2</v>
       </c>
-      <c r="N7" s="18">
+      <c r="N7" s="17">
         <v>0.17948717948717949</v>
       </c>
-      <c r="O7" s="18">
+      <c r="O7" s="17">
         <v>0.1076923076923077</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="19"/>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="17">
         <v>0.11764705882352941</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="17">
         <v>0.18518518518518517</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="17">
         <v>3.5714285714285712E-2</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="17">
         <v>6.0606060606060608E-2</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="17">
         <v>0.12962962962962962</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="17">
         <v>0.125</v>
       </c>
-      <c r="I8" s="18">
+      <c r="I8" s="17">
         <v>7.1428571428571425E-2</v>
       </c>
-      <c r="J8" s="18">
+      <c r="J8" s="17">
         <v>0.13043478260869565</v>
       </c>
-      <c r="K8" s="18">
+      <c r="K8" s="17">
         <v>3.4482758620689655E-2</v>
       </c>
-      <c r="L8" s="18">
+      <c r="L8" s="17">
         <v>0.11538461538461539</v>
       </c>
-      <c r="M8" s="18">
+      <c r="M8" s="17">
         <v>6.8965517241379309E-2</v>
       </c>
-      <c r="N8" s="18">
+      <c r="N8" s="17">
         <v>0.17073170731707318</v>
       </c>
-      <c r="O8" s="18">
+      <c r="O8" s="17">
         <v>0.10722610722610723</v>
       </c>
     </row>
@@ -4440,91 +4465,91 @@
       <c r="A9" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="17">
         <v>0.20689655172413793</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="17">
         <v>0.11538461538461539</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="17">
         <v>7.1428571428571425E-2</v>
       </c>
-      <c r="F9" s="18">
-        <v>0</v>
-      </c>
-      <c r="G9" s="18">
+      <c r="F9" s="17">
+        <v>0</v>
+      </c>
+      <c r="G9" s="17">
         <v>0.02</v>
       </c>
-      <c r="H9" s="18">
-        <v>0</v>
-      </c>
-      <c r="I9" s="18">
+      <c r="H9" s="17">
+        <v>0</v>
+      </c>
+      <c r="I9" s="17">
         <v>0.15151515151515152</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J9" s="17">
         <v>0.14634146341463414</v>
       </c>
-      <c r="K9" s="18">
+      <c r="K9" s="17">
         <v>3.4482758620689655E-2</v>
       </c>
-      <c r="L9" s="18">
+      <c r="L9" s="17">
         <v>4.3478260869565216E-2</v>
       </c>
-      <c r="M9" s="18">
+      <c r="M9" s="17">
         <v>0.14814814814814814</v>
       </c>
-      <c r="N9" s="18">
+      <c r="N9" s="17">
         <v>5.128205128205128E-2</v>
       </c>
-      <c r="O9" s="18">
+      <c r="O9" s="17">
         <v>7.9487179487179482E-2</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="19"/>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="17">
         <v>0.20588235294117646</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="17">
         <v>0.14814814814814814</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="17">
         <v>7.1428571428571425E-2</v>
       </c>
-      <c r="F10" s="18">
-        <v>0</v>
-      </c>
-      <c r="G10" s="18">
+      <c r="F10" s="17">
+        <v>0</v>
+      </c>
+      <c r="G10" s="17">
         <v>1.8518518518518517E-2</v>
       </c>
-      <c r="H10" s="18">
-        <v>0</v>
-      </c>
-      <c r="I10" s="18">
+      <c r="H10" s="17">
+        <v>0</v>
+      </c>
+      <c r="I10" s="17">
         <v>0.11904761904761904</v>
       </c>
-      <c r="J10" s="18">
+      <c r="J10" s="17">
         <v>0.17391304347826086</v>
       </c>
-      <c r="K10" s="18">
+      <c r="K10" s="17">
         <v>3.4482758620689655E-2</v>
       </c>
-      <c r="L10" s="18">
+      <c r="L10" s="17">
         <v>3.8461538461538464E-2</v>
       </c>
-      <c r="M10" s="18">
+      <c r="M10" s="17">
         <v>0.13793103448275862</v>
       </c>
-      <c r="N10" s="18">
+      <c r="N10" s="17">
         <v>4.878048780487805E-2</v>
       </c>
-      <c r="O10" s="18">
+      <c r="O10" s="17">
         <v>8.1585081585081584E-2</v>
       </c>
     </row>
@@ -4532,91 +4557,91 @@
       <c r="A11" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="17">
         <v>3.4482758620689655E-2</v>
       </c>
-      <c r="D11" s="18">
-        <v>0</v>
-      </c>
-      <c r="E11" s="18">
+      <c r="D11" s="17">
+        <v>0</v>
+      </c>
+      <c r="E11" s="17">
         <v>7.1428571428571425E-2</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="17">
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="17">
         <v>0.26</v>
       </c>
-      <c r="H11" s="18">
+      <c r="H11" s="17">
         <v>2.8571428571428571E-2</v>
       </c>
-      <c r="I11" s="18">
+      <c r="I11" s="17">
         <v>0.15151515151515152</v>
       </c>
-      <c r="J11" s="18">
-        <v>0</v>
-      </c>
-      <c r="K11" s="18">
+      <c r="J11" s="17">
+        <v>0</v>
+      </c>
+      <c r="K11" s="17">
         <v>6.8965517241379309E-2</v>
       </c>
-      <c r="L11" s="18">
+      <c r="L11" s="17">
         <v>8.6956521739130432E-2</v>
       </c>
-      <c r="M11" s="18">
+      <c r="M11" s="17">
         <v>3.7037037037037035E-2</v>
       </c>
-      <c r="N11" s="18">
+      <c r="N11" s="17">
         <v>0.10256410256410256</v>
       </c>
-      <c r="O11" s="18">
+      <c r="O11" s="17">
         <v>8.461538461538462E-2</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="19"/>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="17">
         <v>2.9411764705882353E-2</v>
       </c>
-      <c r="D12" s="18">
-        <v>0</v>
-      </c>
-      <c r="E12" s="18">
+      <c r="D12" s="17">
+        <v>0</v>
+      </c>
+      <c r="E12" s="17">
         <v>7.1428571428571425E-2</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="17">
         <v>6.0606060606060608E-2</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="17">
         <v>0.24074074074074073</v>
       </c>
-      <c r="H12" s="18">
+      <c r="H12" s="17">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="I12" s="18">
+      <c r="I12" s="17">
         <v>0.11904761904761904</v>
       </c>
-      <c r="J12" s="18">
-        <v>0</v>
-      </c>
-      <c r="K12" s="18">
+      <c r="J12" s="17">
+        <v>0</v>
+      </c>
+      <c r="K12" s="17">
         <v>6.8965517241379309E-2</v>
       </c>
-      <c r="L12" s="18">
+      <c r="L12" s="17">
         <v>7.6923076923076927E-2</v>
       </c>
-      <c r="M12" s="18">
+      <c r="M12" s="17">
         <v>3.4482758620689655E-2</v>
       </c>
-      <c r="N12" s="18">
+      <c r="N12" s="17">
         <v>9.7560975609756101E-2</v>
       </c>
-      <c r="O12" s="18">
+      <c r="O12" s="17">
         <v>7.6923076923076927E-2</v>
       </c>
     </row>
@@ -4624,92 +4649,2122 @@
       <c r="A13" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="C13" s="18">
-        <v>0</v>
-      </c>
-      <c r="D13" s="18">
-        <v>0</v>
-      </c>
-      <c r="E13" s="18">
-        <v>0</v>
-      </c>
-      <c r="F13" s="18">
+      <c r="C13" s="17">
+        <v>0</v>
+      </c>
+      <c r="D13" s="17">
+        <v>0</v>
+      </c>
+      <c r="E13" s="17">
+        <v>0</v>
+      </c>
+      <c r="F13" s="17">
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="G13" s="18">
-        <v>0</v>
-      </c>
-      <c r="H13" s="18">
+      <c r="G13" s="17">
+        <v>0</v>
+      </c>
+      <c r="H13" s="17">
         <v>5.7142857142857141E-2</v>
       </c>
-      <c r="I13" s="18">
-        <v>0</v>
-      </c>
-      <c r="J13" s="18">
-        <v>0</v>
-      </c>
-      <c r="K13" s="18">
-        <v>0</v>
-      </c>
-      <c r="L13" s="18">
-        <v>0</v>
-      </c>
-      <c r="M13" s="18">
-        <v>0</v>
-      </c>
-      <c r="N13" s="18">
-        <v>0</v>
-      </c>
-      <c r="O13" s="18">
+      <c r="I13" s="17">
+        <v>0</v>
+      </c>
+      <c r="J13" s="17">
+        <v>0</v>
+      </c>
+      <c r="K13" s="17">
+        <v>0</v>
+      </c>
+      <c r="L13" s="17">
+        <v>0</v>
+      </c>
+      <c r="M13" s="17">
+        <v>0</v>
+      </c>
+      <c r="N13" s="17">
+        <v>0</v>
+      </c>
+      <c r="O13" s="17">
         <v>7.6923076923076927E-3</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="19"/>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="C14" s="18">
-        <v>0</v>
-      </c>
-      <c r="D14" s="18">
-        <v>0</v>
-      </c>
-      <c r="E14" s="18">
-        <v>0</v>
-      </c>
-      <c r="F14" s="18">
+      <c r="C14" s="17">
+        <v>0</v>
+      </c>
+      <c r="D14" s="17">
+        <v>0</v>
+      </c>
+      <c r="E14" s="17">
+        <v>0</v>
+      </c>
+      <c r="F14" s="17">
         <v>3.0303030303030304E-2</v>
       </c>
-      <c r="G14" s="18">
-        <v>0</v>
-      </c>
-      <c r="H14" s="18">
+      <c r="G14" s="17">
+        <v>0</v>
+      </c>
+      <c r="H14" s="17">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="I14" s="18">
-        <v>0</v>
-      </c>
-      <c r="J14" s="18">
-        <v>0</v>
-      </c>
-      <c r="K14" s="18">
-        <v>0</v>
-      </c>
-      <c r="L14" s="18">
-        <v>0</v>
-      </c>
-      <c r="M14" s="18">
-        <v>0</v>
-      </c>
-      <c r="N14" s="18">
-        <v>0</v>
-      </c>
-      <c r="O14" s="18">
+      <c r="I14" s="17">
+        <v>0</v>
+      </c>
+      <c r="J14" s="17">
+        <v>0</v>
+      </c>
+      <c r="K14" s="17">
+        <v>0</v>
+      </c>
+      <c r="L14" s="17">
+        <v>0</v>
+      </c>
+      <c r="M14" s="17">
+        <v>0</v>
+      </c>
+      <c r="N14" s="17">
+        <v>0</v>
+      </c>
+      <c r="O14" s="17">
         <v>9.324009324009324E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B16" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>137</v>
+      </c>
+      <c r="D16" t="s">
+        <v>138</v>
+      </c>
+      <c r="E16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E17" s="17">
+        <v>0.31034482758620691</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E18" s="17">
+        <v>0.3235294117647059</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E19" s="17">
+        <v>0.31034482758620691</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E20" s="17">
+        <v>0.3235294117647059</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>132</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E21" s="17">
+        <v>0.13793103448275862</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>132</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E22" s="17">
+        <v>0.11764705882352941</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>133</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E23" s="17">
+        <v>0.20689655172413793</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>133</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E24" s="17">
+        <v>0.20588235294117646</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>134</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E25" s="17">
+        <v>3.4482758620689655E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>134</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E26" s="17">
+        <v>2.9411764705882353E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>135</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E27" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>135</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E28" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E29" s="17">
+        <v>0.42307692307692307</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E30" s="17">
+        <v>0.40740740740740738</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E31" s="17">
+        <v>0.26923076923076922</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E32" s="17">
+        <v>0.25925925925925924</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" t="s">
+        <v>132</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E33" s="17">
+        <v>0.19230769230769232</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" t="s">
+        <v>132</v>
+      </c>
+      <c r="D34" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E34" s="17">
+        <v>0.18518518518518517</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" t="s">
+        <v>133</v>
+      </c>
+      <c r="D35" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E35" s="17">
+        <v>0.11538461538461539</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>133</v>
+      </c>
+      <c r="D36" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E36" s="17">
+        <v>0.14814814814814814</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>134</v>
+      </c>
+      <c r="D37" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E37" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" t="s">
+        <v>134</v>
+      </c>
+      <c r="D38" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E38" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" t="s">
+        <v>135</v>
+      </c>
+      <c r="D39" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E39" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>135</v>
+      </c>
+      <c r="D40" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E40" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D41" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E41" s="17">
+        <v>0.5357142857142857</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D42" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E42" s="17">
+        <v>0.5357142857142857</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D43" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E43" s="17">
+        <v>0.2857142857142857</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D44" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E44" s="17">
+        <v>0.2857142857142857</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" t="s">
+        <v>132</v>
+      </c>
+      <c r="D45" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E45" s="17">
+        <v>3.5714285714285712E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" t="s">
+        <v>132</v>
+      </c>
+      <c r="D46" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E46" s="17">
+        <v>3.5714285714285712E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" t="s">
+        <v>133</v>
+      </c>
+      <c r="D47" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E47" s="17">
+        <v>7.1428571428571425E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" t="s">
+        <v>133</v>
+      </c>
+      <c r="D48" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E48" s="17">
+        <v>7.1428571428571425E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C49" t="s">
+        <v>134</v>
+      </c>
+      <c r="D49" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E49" s="17">
+        <v>7.1428571428571425E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C50" t="s">
+        <v>134</v>
+      </c>
+      <c r="D50" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E50" s="17">
+        <v>7.1428571428571425E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C51" t="s">
+        <v>135</v>
+      </c>
+      <c r="D51" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E51" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C52" t="s">
+        <v>135</v>
+      </c>
+      <c r="D52" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E52" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D53" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E53" s="17">
+        <v>0.53333333333333333</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D54" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E54" s="17">
+        <v>0.5757575757575758</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D55" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E55" s="17">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C56" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D56" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E56" s="17">
+        <v>0.27272727272727271</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C57" t="s">
+        <v>132</v>
+      </c>
+      <c r="D57" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E57" s="17">
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C58" t="s">
+        <v>132</v>
+      </c>
+      <c r="D58" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E58" s="17">
+        <v>6.0606060606060608E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C59" t="s">
+        <v>133</v>
+      </c>
+      <c r="D59" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E59" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C60" t="s">
+        <v>133</v>
+      </c>
+      <c r="D60" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E60" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C61" t="s">
+        <v>134</v>
+      </c>
+      <c r="D61" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E61" s="17">
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C62" t="s">
+        <v>134</v>
+      </c>
+      <c r="D62" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E62" s="17">
+        <v>6.0606060606060608E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C63" t="s">
+        <v>135</v>
+      </c>
+      <c r="D63" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E63" s="17">
+        <v>3.3333333333333333E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C64" t="s">
+        <v>135</v>
+      </c>
+      <c r="D64" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E64" s="17">
+        <v>3.0303030303030304E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D65" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E65" s="17">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C66" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D66" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E66" s="17">
+        <v>0.31481481481481483</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C67" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D67" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E67" s="17">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C68" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D68" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E68" s="17">
+        <v>0.29629629629629628</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C69" t="s">
+        <v>132</v>
+      </c>
+      <c r="D69" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E69" s="17">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C70" t="s">
+        <v>132</v>
+      </c>
+      <c r="D70" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E70" s="17">
+        <v>0.12962962962962962</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C71" t="s">
+        <v>133</v>
+      </c>
+      <c r="D71" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E71" s="17">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C72" t="s">
+        <v>133</v>
+      </c>
+      <c r="D72" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E72" s="17">
+        <v>1.8518518518518517E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C73" t="s">
+        <v>134</v>
+      </c>
+      <c r="D73" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E73" s="17">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C74" t="s">
+        <v>134</v>
+      </c>
+      <c r="D74" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E74" s="17">
+        <v>0.24074074074074073</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C75" t="s">
+        <v>135</v>
+      </c>
+      <c r="D75" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E75" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C76" t="s">
+        <v>135</v>
+      </c>
+      <c r="D76" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E76" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B77" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C77" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D77" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E77" s="17">
+        <v>0.51428571428571423</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C78" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D78" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E78" s="17">
+        <v>0.52500000000000002</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D79" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E79" s="17">
+        <v>0.2857142857142857</v>
+      </c>
+    </row>
+    <row r="80" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B80" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D80" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E80" s="17">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B81" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" t="s">
+        <v>132</v>
+      </c>
+      <c r="D81" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E81" s="17">
+        <v>0.11428571428571428</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B82" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C82" t="s">
+        <v>132</v>
+      </c>
+      <c r="D82" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E82" s="17">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B83" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C83" t="s">
+        <v>133</v>
+      </c>
+      <c r="D83" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E83" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B84" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84" t="s">
+        <v>133</v>
+      </c>
+      <c r="D84" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E84" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B85" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C85" t="s">
+        <v>134</v>
+      </c>
+      <c r="D85" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E85" s="17">
+        <v>2.8571428571428571E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B86" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C86" t="s">
+        <v>134</v>
+      </c>
+      <c r="D86" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E86" s="17">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B87" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" t="s">
+        <v>135</v>
+      </c>
+      <c r="D87" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E87" s="17">
+        <v>5.7142857142857141E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B88" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" t="s">
+        <v>135</v>
+      </c>
+      <c r="D88" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E88" s="17">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B89" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C89" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D89" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E89" s="17">
+        <v>0.36363636363636365</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B90" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C90" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D90" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E90" s="17">
+        <v>0.35714285714285715</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B91" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C91" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D91" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E91" s="17">
+        <v>0.27272727272727271</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B92" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C92" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D92" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E92" s="17">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="93" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B93" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C93" t="s">
+        <v>132</v>
+      </c>
+      <c r="D93" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E93" s="17">
+        <v>6.0606060606060608E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B94" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C94" t="s">
+        <v>132</v>
+      </c>
+      <c r="D94" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E94" s="17">
+        <v>7.1428571428571425E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B95" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C95" t="s">
+        <v>133</v>
+      </c>
+      <c r="D95" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E95" s="17">
+        <v>0.15151515151515152</v>
+      </c>
+    </row>
+    <row r="96" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B96" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C96" t="s">
+        <v>133</v>
+      </c>
+      <c r="D96" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E96" s="17">
+        <v>0.11904761904761904</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B97" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C97" t="s">
+        <v>134</v>
+      </c>
+      <c r="D97" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E97" s="17">
+        <v>0.15151515151515152</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B98" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C98" t="s">
+        <v>134</v>
+      </c>
+      <c r="D98" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E98" s="17">
+        <v>0.11904761904761904</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B99" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C99" t="s">
+        <v>135</v>
+      </c>
+      <c r="D99" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E99" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B100" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C100" t="s">
+        <v>135</v>
+      </c>
+      <c r="D100" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E100" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B101" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C101" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D101" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E101" s="17">
+        <v>0.41463414634146339</v>
+      </c>
+    </row>
+    <row r="102" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B102" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C102" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D102" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E102" s="17">
+        <v>0.41304347826086957</v>
+      </c>
+    </row>
+    <row r="103" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B103" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C103" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D103" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E103" s="17">
+        <v>0.31707317073170732</v>
+      </c>
+    </row>
+    <row r="104" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B104" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C104" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D104" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E104" s="17">
+        <v>0.28260869565217389</v>
+      </c>
+    </row>
+    <row r="105" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B105" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C105" t="s">
+        <v>132</v>
+      </c>
+      <c r="D105" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E105" s="17">
+        <v>0.12195121951219512</v>
+      </c>
+    </row>
+    <row r="106" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B106" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C106" t="s">
+        <v>132</v>
+      </c>
+      <c r="D106" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E106" s="17">
+        <v>0.13043478260869565</v>
+      </c>
+    </row>
+    <row r="107" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B107" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C107" t="s">
+        <v>133</v>
+      </c>
+      <c r="D107" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E107" s="17">
+        <v>0.14634146341463414</v>
+      </c>
+    </row>
+    <row r="108" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B108" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C108" t="s">
+        <v>133</v>
+      </c>
+      <c r="D108" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E108" s="17">
+        <v>0.17391304347826086</v>
+      </c>
+    </row>
+    <row r="109" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B109" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C109" t="s">
+        <v>134</v>
+      </c>
+      <c r="D109" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E109" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B110" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C110" t="s">
+        <v>134</v>
+      </c>
+      <c r="D110" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E110" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B111" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C111" t="s">
+        <v>135</v>
+      </c>
+      <c r="D111" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E111" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B112" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C112" t="s">
+        <v>135</v>
+      </c>
+      <c r="D112" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E112" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B113" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C113" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D113" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E113" s="17">
+        <v>0.62068965517241381</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B114" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C114" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D114" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E114" s="17">
+        <v>0.62068965517241381</v>
+      </c>
+    </row>
+    <row r="115" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B115" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C115" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D115" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E115" s="17">
+        <v>0.2413793103448276</v>
+      </c>
+    </row>
+    <row r="116" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B116" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C116" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D116" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E116" s="17">
+        <v>0.2413793103448276</v>
+      </c>
+    </row>
+    <row r="117" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B117" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C117" t="s">
+        <v>132</v>
+      </c>
+      <c r="D117" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E117" s="17">
+        <v>3.4482758620689655E-2</v>
+      </c>
+    </row>
+    <row r="118" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B118" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C118" t="s">
+        <v>132</v>
+      </c>
+      <c r="D118" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E118" s="17">
+        <v>3.4482758620689655E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B119" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C119" t="s">
+        <v>133</v>
+      </c>
+      <c r="D119" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E119" s="17">
+        <v>3.4482758620689655E-2</v>
+      </c>
+    </row>
+    <row r="120" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B120" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C120" t="s">
+        <v>133</v>
+      </c>
+      <c r="D120" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E120" s="17">
+        <v>3.4482758620689655E-2</v>
+      </c>
+    </row>
+    <row r="121" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B121" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C121" t="s">
+        <v>134</v>
+      </c>
+      <c r="D121" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E121" s="17">
+        <v>6.8965517241379309E-2</v>
+      </c>
+    </row>
+    <row r="122" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B122" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C122" t="s">
+        <v>134</v>
+      </c>
+      <c r="D122" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E122" s="17">
+        <v>6.8965517241379309E-2</v>
+      </c>
+    </row>
+    <row r="123" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B123" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C123" t="s">
+        <v>135</v>
+      </c>
+      <c r="D123" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E123" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B124" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C124" t="s">
+        <v>135</v>
+      </c>
+      <c r="D124" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E124" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B125" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C125" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D125" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E125" s="17">
+        <v>0.39130434782608697</v>
+      </c>
+    </row>
+    <row r="126" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B126" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C126" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D126" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E126" s="17">
+        <v>0.42307692307692307</v>
+      </c>
+    </row>
+    <row r="127" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B127" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C127" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D127" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E127" s="17">
+        <v>0.39130434782608697</v>
+      </c>
+    </row>
+    <row r="128" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B128" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C128" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D128" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E128" s="17">
+        <v>0.34615384615384615</v>
+      </c>
+    </row>
+    <row r="129" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B129" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C129" t="s">
+        <v>132</v>
+      </c>
+      <c r="D129" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E129" s="17">
+        <v>8.6956521739130432E-2</v>
+      </c>
+    </row>
+    <row r="130" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B130" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C130" t="s">
+        <v>132</v>
+      </c>
+      <c r="D130" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E130" s="17">
+        <v>0.11538461538461539</v>
+      </c>
+    </row>
+    <row r="131" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B131" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C131" t="s">
+        <v>133</v>
+      </c>
+      <c r="D131" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E131" s="17">
+        <v>4.3478260869565216E-2</v>
+      </c>
+    </row>
+    <row r="132" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B132" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C132" t="s">
+        <v>133</v>
+      </c>
+      <c r="D132" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E132" s="17">
+        <v>3.8461538461538464E-2</v>
+      </c>
+    </row>
+    <row r="133" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B133" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C133" t="s">
+        <v>134</v>
+      </c>
+      <c r="D133" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E133" s="17">
+        <v>8.6956521739130432E-2</v>
+      </c>
+    </row>
+    <row r="134" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B134" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C134" t="s">
+        <v>134</v>
+      </c>
+      <c r="D134" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E134" s="17">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="135" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B135" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C135" t="s">
+        <v>135</v>
+      </c>
+      <c r="D135" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E135" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B136" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C136" t="s">
+        <v>135</v>
+      </c>
+      <c r="D136" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E136" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B137" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C137" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D137" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E137" s="17">
+        <v>0.62962962962962965</v>
+      </c>
+    </row>
+    <row r="138" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B138" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C138" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D138" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E138" s="17">
+        <v>0.65517241379310343</v>
+      </c>
+    </row>
+    <row r="139" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B139" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C139" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D139" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E139" s="17">
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="140" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B140" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C140" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D140" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E140" s="17">
+        <v>0.10344827586206896</v>
+      </c>
+    </row>
+    <row r="141" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B141" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C141" t="s">
+        <v>132</v>
+      </c>
+      <c r="D141" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E141" s="17">
+        <v>7.407407407407407E-2</v>
+      </c>
+    </row>
+    <row r="142" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B142" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C142" t="s">
+        <v>132</v>
+      </c>
+      <c r="D142" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E142" s="17">
+        <v>6.8965517241379309E-2</v>
+      </c>
+    </row>
+    <row r="143" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B143" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C143" t="s">
+        <v>133</v>
+      </c>
+      <c r="D143" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E143" s="17">
+        <v>0.14814814814814814</v>
+      </c>
+    </row>
+    <row r="144" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B144" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C144" t="s">
+        <v>133</v>
+      </c>
+      <c r="D144" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E144" s="17">
+        <v>0.13793103448275862</v>
+      </c>
+    </row>
+    <row r="145" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B145" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C145" t="s">
+        <v>134</v>
+      </c>
+      <c r="D145" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E145" s="17">
+        <v>3.7037037037037035E-2</v>
+      </c>
+    </row>
+    <row r="146" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B146" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C146" t="s">
+        <v>134</v>
+      </c>
+      <c r="D146" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E146" s="17">
+        <v>3.4482758620689655E-2</v>
+      </c>
+    </row>
+    <row r="147" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B147" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C147" t="s">
+        <v>135</v>
+      </c>
+      <c r="D147" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E147" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B148" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C148" t="s">
+        <v>135</v>
+      </c>
+      <c r="D148" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E148" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B149" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C149" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D149" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E149" s="17">
+        <v>0.53846153846153844</v>
+      </c>
+    </row>
+    <row r="150" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B150" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C150" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D150" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E150" s="17">
+        <v>0.56097560975609762</v>
+      </c>
+    </row>
+    <row r="151" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B151" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C151" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D151" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E151" s="17">
+        <v>0.12820512820512819</v>
+      </c>
+    </row>
+    <row r="152" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B152" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C152" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D152" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E152" s="17">
+        <v>0.12195121951219512</v>
+      </c>
+    </row>
+    <row r="153" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B153" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C153" t="s">
+        <v>132</v>
+      </c>
+      <c r="D153" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E153" s="17">
+        <v>0.17948717948717949</v>
+      </c>
+    </row>
+    <row r="154" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B154" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C154" t="s">
+        <v>132</v>
+      </c>
+      <c r="D154" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E154" s="17">
+        <v>0.17073170731707318</v>
+      </c>
+    </row>
+    <row r="155" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B155" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C155" t="s">
+        <v>133</v>
+      </c>
+      <c r="D155" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E155" s="17">
+        <v>5.128205128205128E-2</v>
+      </c>
+    </row>
+    <row r="156" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B156" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C156" t="s">
+        <v>133</v>
+      </c>
+      <c r="D156" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E156" s="17">
+        <v>4.878048780487805E-2</v>
+      </c>
+    </row>
+    <row r="157" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B157" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C157" t="s">
+        <v>134</v>
+      </c>
+      <c r="D157" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E157" s="17">
+        <v>0.10256410256410256</v>
+      </c>
+    </row>
+    <row r="158" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B158" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C158" t="s">
+        <v>134</v>
+      </c>
+      <c r="D158" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E158" s="17">
+        <v>9.7560975609756101E-2</v>
+      </c>
+    </row>
+    <row r="159" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B159" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C159" t="s">
+        <v>135</v>
+      </c>
+      <c r="D159" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E159" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B160" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C160" t="s">
+        <v>135</v>
+      </c>
+      <c r="D160" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E160" s="17">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4735,7 +6790,7 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="53.44140625" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" customWidth="1"/>
@@ -5341,11 +7396,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{615EFB19-F474-4215-A4C4-27A7F36F1049}">
   <dimension ref="A1:F164"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G158" sqref="G158"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="14.6640625" customWidth="1"/>
     <col min="3" max="3" width="17.5546875" customWidth="1"/>
@@ -5354,22 +7409,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>122</v>
       </c>
     </row>
@@ -8682,7 +10737,7 @@
         <v>124</v>
       </c>
       <c r="E154">
-        <f t="shared" ref="E154:F164" si="6">SUMIF(B3:B151,D154,E3:E151)</f>
+        <f t="shared" ref="E154:E164" si="6">SUMIF(B3:B151,D154,E3:E151)</f>
         <v>124</v>
       </c>
       <c r="F154">

</xml_diff>

<commit_message>
se añade grafico horizontal
</commit_message>
<xml_diff>
--- a/app_salud/app/logic/data/set_de_datos_1.xlsx
+++ b/app_salud/app/logic/data/set_de_datos_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rstudio\software_salud\app_salud\app\logic\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ECA945A-87E9-4CBA-A4DD-2CAE5D2C3C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6186A29-FBB7-4DA0-8F5B-5EAFE03369C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{A035267E-5D3E-4097-B788-79B64BEF5509}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1447" uniqueCount="141">
   <si>
     <t>Febrero</t>
   </si>
@@ -457,6 +457,12 @@
   </si>
   <si>
     <t>Tiempo de inactividad</t>
+  </si>
+  <si>
+    <t>Otorrinolaringología</t>
+  </si>
+  <si>
+    <t>Oftalmología</t>
   </si>
 </sst>
 </file>
@@ -7389,15 +7395,16 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{615EFB19-F474-4215-A4C4-27A7F36F1049}">
-  <dimension ref="A1:F170"/>
+  <dimension ref="A1:F272"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="D167" sqref="D167:F170"/>
+    <sheetView tabSelected="1" topLeftCell="A250" workbookViewId="0">
+      <selection activeCell="F273" sqref="F273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="29.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
     <col min="3" max="3" width="17.5546875" customWidth="1"/>
     <col min="5" max="5" width="16.77734375" customWidth="1"/>
     <col min="6" max="6" width="20.33203125" customWidth="1"/>
@@ -7416,6 +7423,12 @@
       <c r="D1" s="12" t="s">
         <v>120</v>
       </c>
+      <c r="E1" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -10696,227 +10709,2459 @@
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D151" t="s">
-        <v>122</v>
+      <c r="A151" t="s">
+        <v>139</v>
+      </c>
+      <c r="B151" t="s">
+        <v>5</v>
+      </c>
+      <c r="C151">
+        <v>180</v>
+      </c>
+      <c r="D151">
+        <v>221</v>
       </c>
       <c r="E151">
-        <f>SUM(E2:E150)</f>
-        <v>1970</v>
+        <f t="shared" ref="E151:E214" si="6">IF(D151-C151&gt;0,D151-C151,0)</f>
+        <v>41</v>
       </c>
       <c r="F151">
-        <f>SUM(F2:F150)</f>
-        <v>1611</v>
+        <f t="shared" ref="F151:F214" si="7">IF(D151-C151&lt;0,C151-D151,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>139</v>
+      </c>
+      <c r="B152" t="s">
+        <v>6</v>
+      </c>
+      <c r="C152">
+        <v>180</v>
+      </c>
+      <c r="D152">
+        <v>158</v>
+      </c>
+      <c r="E152">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F152">
+        <f t="shared" si="7"/>
+        <v>22</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D153" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E153" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="F153" s="12" t="s">
-        <v>135</v>
+      <c r="A153" t="s">
+        <v>139</v>
+      </c>
+      <c r="B153" t="s">
+        <v>115</v>
+      </c>
+      <c r="C153">
+        <v>180</v>
+      </c>
+      <c r="D153">
+        <v>191</v>
+      </c>
+      <c r="E153">
+        <f t="shared" si="6"/>
+        <v>11</v>
+      </c>
+      <c r="F153">
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D154" t="s">
-        <v>1</v>
+      <c r="A154" t="s">
+        <v>139</v>
+      </c>
+      <c r="B154" t="s">
+        <v>8</v>
+      </c>
+      <c r="C154">
+        <v>180</v>
+      </c>
+      <c r="D154">
+        <v>151</v>
       </c>
       <c r="E154">
-        <f>SUMIF($B$2:$B$150,$D154,E$2:E$150)</f>
-        <v>185</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="F154">
-        <f>SUMIF($B$2:$B$150,$D154,F$2:F$150)</f>
-        <v>120</v>
+        <f t="shared" si="7"/>
+        <v>29</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D155" t="s">
-        <v>123</v>
+      <c r="A155" t="s">
+        <v>139</v>
+      </c>
+      <c r="B155" t="s">
+        <v>9</v>
+      </c>
+      <c r="C155">
+        <v>180</v>
+      </c>
+      <c r="D155">
+        <v>190</v>
       </c>
       <c r="E155">
-        <f t="shared" ref="E155:F165" si="6">SUMIF($B$2:$B$150,$D155,E$2:E$150)</f>
-        <v>124</v>
+        <f t="shared" si="6"/>
+        <v>10</v>
       </c>
       <c r="F155">
-        <f t="shared" si="6"/>
-        <v>127</v>
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D156" t="s">
-        <v>2</v>
+      <c r="A156" t="s">
+        <v>139</v>
+      </c>
+      <c r="B156" t="s">
+        <v>10</v>
+      </c>
+      <c r="C156">
+        <v>180</v>
+      </c>
+      <c r="D156">
+        <v>190</v>
       </c>
       <c r="E156">
         <f t="shared" si="6"/>
-        <v>208</v>
+        <v>10</v>
       </c>
       <c r="F156">
-        <f t="shared" si="6"/>
-        <v>95</v>
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D157" t="s">
-        <v>3</v>
+      <c r="A157" t="s">
+        <v>139</v>
+      </c>
+      <c r="B157" t="s">
+        <v>11</v>
+      </c>
+      <c r="C157">
+        <v>180</v>
+      </c>
+      <c r="D157">
+        <v>170</v>
       </c>
       <c r="E157">
         <f t="shared" si="6"/>
-        <v>226</v>
+        <v>0</v>
       </c>
       <c r="F157">
-        <f t="shared" si="6"/>
-        <v>144</v>
+        <f t="shared" si="7"/>
+        <v>10</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D158" t="s">
-        <v>124</v>
+      <c r="A158" t="s">
+        <v>139</v>
+      </c>
+      <c r="B158" t="s">
+        <v>1</v>
+      </c>
+      <c r="C158">
+        <v>180</v>
+      </c>
+      <c r="D158">
+        <v>160</v>
       </c>
       <c r="E158">
         <f t="shared" si="6"/>
-        <v>111</v>
+        <v>0</v>
       </c>
       <c r="F158">
-        <f t="shared" si="6"/>
-        <v>205</v>
+        <f t="shared" si="7"/>
+        <v>20</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D159" t="s">
-        <v>5</v>
+      <c r="A159" t="s">
+        <v>139</v>
+      </c>
+      <c r="B159" t="s">
+        <v>123</v>
+      </c>
+      <c r="C159">
+        <v>180</v>
+      </c>
+      <c r="D159">
+        <v>147</v>
       </c>
       <c r="E159">
         <f t="shared" si="6"/>
-        <v>155</v>
+        <v>0</v>
       </c>
       <c r="F159">
-        <f t="shared" si="6"/>
-        <v>79</v>
+        <f t="shared" si="7"/>
+        <v>33</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D160" t="s">
-        <v>6</v>
+      <c r="A160" t="s">
+        <v>139</v>
+      </c>
+      <c r="B160" t="s">
+        <v>2</v>
+      </c>
+      <c r="C160">
+        <v>180</v>
+      </c>
+      <c r="D160">
+        <v>178</v>
       </c>
       <c r="E160">
         <f t="shared" si="6"/>
-        <v>117</v>
+        <v>0</v>
       </c>
       <c r="F160">
-        <f t="shared" si="6"/>
-        <v>96</v>
-      </c>
-    </row>
-    <row r="161" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D161" t="s">
-        <v>115</v>
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>139</v>
+      </c>
+      <c r="B161" t="s">
+        <v>3</v>
+      </c>
+      <c r="C161">
+        <v>180</v>
+      </c>
+      <c r="D161">
+        <v>140</v>
       </c>
       <c r="E161">
         <f t="shared" si="6"/>
-        <v>223</v>
+        <v>0</v>
       </c>
       <c r="F161">
-        <f t="shared" si="6"/>
-        <v>141</v>
-      </c>
-    </row>
-    <row r="162" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D162" t="s">
-        <v>8</v>
+        <f t="shared" si="7"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>139</v>
+      </c>
+      <c r="B162" t="s">
+        <v>124</v>
+      </c>
+      <c r="C162">
+        <v>180</v>
+      </c>
+      <c r="D162">
+        <v>158</v>
       </c>
       <c r="E162">
         <f t="shared" si="6"/>
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="F162">
-        <f t="shared" si="6"/>
-        <v>168</v>
-      </c>
-    </row>
-    <row r="163" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D163" t="s">
-        <v>9</v>
+        <f t="shared" si="7"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>139</v>
+      </c>
+      <c r="B163" t="s">
+        <v>5</v>
+      </c>
+      <c r="C163">
+        <v>180</v>
+      </c>
+      <c r="D163">
+        <v>153</v>
       </c>
       <c r="E163">
         <f t="shared" si="6"/>
-        <v>210</v>
+        <v>0</v>
       </c>
       <c r="F163">
-        <f t="shared" si="6"/>
-        <v>177</v>
-      </c>
-    </row>
-    <row r="164" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D164" t="s">
-        <v>10</v>
+        <f t="shared" si="7"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>139</v>
+      </c>
+      <c r="B164" t="s">
+        <v>6</v>
+      </c>
+      <c r="C164">
+        <v>180</v>
+      </c>
+      <c r="D164">
+        <v>176</v>
       </c>
       <c r="E164">
         <f t="shared" si="6"/>
-        <v>146</v>
+        <v>0</v>
       </c>
       <c r="F164">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>139</v>
+      </c>
+      <c r="B165" t="s">
+        <v>115</v>
+      </c>
+      <c r="C165">
+        <v>180</v>
+      </c>
+      <c r="D165">
+        <v>166</v>
+      </c>
+      <c r="E165">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F165">
+        <f t="shared" si="7"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>139</v>
+      </c>
+      <c r="B166" t="s">
+        <v>8</v>
+      </c>
+      <c r="C166">
+        <v>180</v>
+      </c>
+      <c r="D166">
+        <v>172</v>
+      </c>
+      <c r="E166">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F166">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>139</v>
+      </c>
+      <c r="B167" t="s">
+        <v>9</v>
+      </c>
+      <c r="C167">
+        <v>180</v>
+      </c>
+      <c r="D167">
+        <v>173</v>
+      </c>
+      <c r="E167">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F167">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>139</v>
+      </c>
+      <c r="B168" t="s">
+        <v>10</v>
+      </c>
+      <c r="C168">
+        <v>180</v>
+      </c>
+      <c r="D168">
+        <v>170</v>
+      </c>
+      <c r="E168">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F168">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>139</v>
+      </c>
+      <c r="B169" t="s">
+        <v>11</v>
+      </c>
+      <c r="C169">
+        <v>180</v>
+      </c>
+      <c r="D169">
+        <v>190</v>
+      </c>
+      <c r="E169">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="F169">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>139</v>
+      </c>
+      <c r="B170" t="s">
+        <v>1</v>
+      </c>
+      <c r="C170">
+        <v>180</v>
+      </c>
+      <c r="D170">
+        <v>171</v>
+      </c>
+      <c r="E170">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F170">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>139</v>
+      </c>
+      <c r="B171" t="s">
+        <v>123</v>
+      </c>
+      <c r="C171">
+        <v>180</v>
+      </c>
+      <c r="D171">
+        <v>112</v>
+      </c>
+      <c r="E171">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F171">
+        <f t="shared" si="7"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>139</v>
+      </c>
+      <c r="B172" t="s">
+        <v>2</v>
+      </c>
+      <c r="C172">
+        <v>180</v>
+      </c>
+      <c r="D172">
+        <v>147</v>
+      </c>
+      <c r="E172">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F172">
+        <f t="shared" si="7"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>139</v>
+      </c>
+      <c r="B173" t="s">
+        <v>3</v>
+      </c>
+      <c r="C173">
+        <v>180</v>
+      </c>
+      <c r="D173">
+        <v>179</v>
+      </c>
+      <c r="E173">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F173">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>139</v>
+      </c>
+      <c r="B174" t="s">
+        <v>124</v>
+      </c>
+      <c r="C174">
+        <v>180</v>
+      </c>
+      <c r="D174">
+        <v>159</v>
+      </c>
+      <c r="E174">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F174">
+        <f t="shared" si="7"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>139</v>
+      </c>
+      <c r="B175" t="s">
+        <v>5</v>
+      </c>
+      <c r="C175">
+        <v>180</v>
+      </c>
+      <c r="D175">
+        <v>125</v>
+      </c>
+      <c r="E175">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F175">
+        <f t="shared" si="7"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>139</v>
+      </c>
+      <c r="B176" t="s">
+        <v>6</v>
+      </c>
+      <c r="C176">
+        <v>180</v>
+      </c>
+      <c r="D176">
+        <v>141</v>
+      </c>
+      <c r="E176">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F176">
+        <f t="shared" si="7"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>139</v>
+      </c>
+      <c r="B177" t="s">
+        <v>115</v>
+      </c>
+      <c r="C177">
+        <v>180</v>
+      </c>
+      <c r="D177">
         <v>156</v>
       </c>
-    </row>
-    <row r="165" spans="4:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D165" t="s">
+      <c r="E177">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F177">
+        <f t="shared" si="7"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>139</v>
+      </c>
+      <c r="B178" t="s">
+        <v>8</v>
+      </c>
+      <c r="C178">
+        <v>180</v>
+      </c>
+      <c r="D178">
+        <v>150</v>
+      </c>
+      <c r="E178">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F178">
+        <f t="shared" si="7"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>139</v>
+      </c>
+      <c r="B179" t="s">
+        <v>9</v>
+      </c>
+      <c r="C179">
+        <v>180</v>
+      </c>
+      <c r="D179">
+        <v>153</v>
+      </c>
+      <c r="E179">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F179">
+        <f t="shared" si="7"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>139</v>
+      </c>
+      <c r="B180" t="s">
+        <v>10</v>
+      </c>
+      <c r="C180">
+        <v>180</v>
+      </c>
+      <c r="D180">
+        <v>137</v>
+      </c>
+      <c r="E180">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F180">
+        <f t="shared" si="7"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>139</v>
+      </c>
+      <c r="B181" t="s">
         <v>11</v>
       </c>
-      <c r="E165">
-        <f>SUMIF($B$2:$B$150,$D165,E$2:E$150)</f>
+      <c r="C181">
+        <v>180</v>
+      </c>
+      <c r="D181">
+        <v>170</v>
+      </c>
+      <c r="E181">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F181">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
+        <v>139</v>
+      </c>
+      <c r="B182" t="s">
+        <v>1</v>
+      </c>
+      <c r="C182">
+        <v>180</v>
+      </c>
+      <c r="D182">
+        <v>163</v>
+      </c>
+      <c r="E182">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F182">
+        <f t="shared" si="7"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>139</v>
+      </c>
+      <c r="B183" t="s">
+        <v>123</v>
+      </c>
+      <c r="C183">
+        <v>180</v>
+      </c>
+      <c r="D183">
+        <v>209</v>
+      </c>
+      <c r="E183">
+        <f t="shared" si="6"/>
+        <v>29</v>
+      </c>
+      <c r="F183">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>139</v>
+      </c>
+      <c r="B184" t="s">
+        <v>2</v>
+      </c>
+      <c r="C184">
+        <v>180</v>
+      </c>
+      <c r="D184">
+        <v>174</v>
+      </c>
+      <c r="E184">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F184">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>139</v>
+      </c>
+      <c r="B185" t="s">
+        <v>3</v>
+      </c>
+      <c r="C185">
+        <v>180</v>
+      </c>
+      <c r="D185">
+        <v>166</v>
+      </c>
+      <c r="E185">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F185">
+        <f t="shared" si="7"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
+        <v>139</v>
+      </c>
+      <c r="B186" t="s">
+        <v>124</v>
+      </c>
+      <c r="C186">
+        <v>180</v>
+      </c>
+      <c r="D186">
+        <v>194</v>
+      </c>
+      <c r="E186">
+        <f t="shared" si="6"/>
+        <v>14</v>
+      </c>
+      <c r="F186">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
+        <v>139</v>
+      </c>
+      <c r="B187" t="s">
+        <v>5</v>
+      </c>
+      <c r="C187">
+        <v>180</v>
+      </c>
+      <c r="D187">
+        <v>192</v>
+      </c>
+      <c r="E187">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="F187">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
+        <v>139</v>
+      </c>
+      <c r="B188" t="s">
+        <v>6</v>
+      </c>
+      <c r="C188">
+        <v>180</v>
+      </c>
+      <c r="D188">
+        <v>159</v>
+      </c>
+      <c r="E188">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F188">
+        <f t="shared" si="7"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
+        <v>139</v>
+      </c>
+      <c r="B189" t="s">
+        <v>115</v>
+      </c>
+      <c r="C189">
+        <v>180</v>
+      </c>
+      <c r="D189">
+        <v>149</v>
+      </c>
+      <c r="E189">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F189">
+        <f t="shared" si="7"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
+        <v>139</v>
+      </c>
+      <c r="B190" t="s">
+        <v>8</v>
+      </c>
+      <c r="C190">
+        <v>180</v>
+      </c>
+      <c r="D190">
+        <v>160</v>
+      </c>
+      <c r="E190">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F190">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
+        <v>139</v>
+      </c>
+      <c r="B191" t="s">
+        <v>9</v>
+      </c>
+      <c r="C191">
+        <v>180</v>
+      </c>
+      <c r="D191">
+        <v>173</v>
+      </c>
+      <c r="E191">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F191">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>139</v>
+      </c>
+      <c r="B192" t="s">
+        <v>10</v>
+      </c>
+      <c r="C192">
+        <v>180</v>
+      </c>
+      <c r="D192">
+        <v>134</v>
+      </c>
+      <c r="E192">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F192">
+        <f t="shared" si="7"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>139</v>
+      </c>
+      <c r="B193" t="s">
+        <v>11</v>
+      </c>
+      <c r="C193">
+        <v>180</v>
+      </c>
+      <c r="D193">
+        <v>151</v>
+      </c>
+      <c r="E193">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F193">
+        <f t="shared" si="7"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>139</v>
+      </c>
+      <c r="B194" t="s">
+        <v>1</v>
+      </c>
+      <c r="C194">
+        <v>180</v>
+      </c>
+      <c r="D194">
+        <v>154</v>
+      </c>
+      <c r="E194">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F194">
+        <f t="shared" si="7"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A195" t="s">
+        <v>139</v>
+      </c>
+      <c r="B195" t="s">
+        <v>123</v>
+      </c>
+      <c r="C195">
+        <v>180</v>
+      </c>
+      <c r="D195">
+        <v>162</v>
+      </c>
+      <c r="E195">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F195">
+        <f t="shared" si="7"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>139</v>
+      </c>
+      <c r="B196" t="s">
+        <v>2</v>
+      </c>
+      <c r="C196">
+        <v>180</v>
+      </c>
+      <c r="D196">
+        <v>147</v>
+      </c>
+      <c r="E196">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F196">
+        <f t="shared" si="7"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
+        <v>139</v>
+      </c>
+      <c r="B197" t="s">
+        <v>3</v>
+      </c>
+      <c r="C197">
+        <v>180</v>
+      </c>
+      <c r="D197">
+        <v>164</v>
+      </c>
+      <c r="E197">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F197">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
+        <v>139</v>
+      </c>
+      <c r="B198" t="s">
+        <v>124</v>
+      </c>
+      <c r="C198">
+        <v>180</v>
+      </c>
+      <c r="D198">
+        <v>225</v>
+      </c>
+      <c r="E198">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+      <c r="F198">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A199" t="s">
+        <v>139</v>
+      </c>
+      <c r="B199" t="s">
+        <v>5</v>
+      </c>
+      <c r="C199">
+        <v>180</v>
+      </c>
+      <c r="D199">
+        <v>168</v>
+      </c>
+      <c r="E199">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F199">
+        <f t="shared" si="7"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
+        <v>139</v>
+      </c>
+      <c r="B200" t="s">
+        <v>6</v>
+      </c>
+      <c r="C200">
+        <v>180</v>
+      </c>
+      <c r="D200">
+        <v>164</v>
+      </c>
+      <c r="E200">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F200">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A201" t="s">
+        <v>140</v>
+      </c>
+      <c r="B201" t="s">
+        <v>115</v>
+      </c>
+      <c r="C201">
+        <v>90</v>
+      </c>
+      <c r="D201">
+        <v>99</v>
+      </c>
+      <c r="E201">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="F201">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>140</v>
+      </c>
+      <c r="B202" t="s">
+        <v>8</v>
+      </c>
+      <c r="C202">
+        <v>90</v>
+      </c>
+      <c r="D202">
+        <v>67</v>
+      </c>
+      <c r="E202">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F202">
+        <f t="shared" si="7"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
+        <v>140</v>
+      </c>
+      <c r="B203" t="s">
+        <v>9</v>
+      </c>
+      <c r="C203">
+        <v>90</v>
+      </c>
+      <c r="D203">
+        <v>120</v>
+      </c>
+      <c r="E203">
+        <f t="shared" si="6"/>
+        <v>30</v>
+      </c>
+      <c r="F203">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A204" t="s">
+        <v>140</v>
+      </c>
+      <c r="B204" t="s">
+        <v>10</v>
+      </c>
+      <c r="C204">
+        <v>90</v>
+      </c>
+      <c r="D204">
+        <v>84</v>
+      </c>
+      <c r="E204">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F204">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A205" t="s">
+        <v>140</v>
+      </c>
+      <c r="B205" t="s">
+        <v>11</v>
+      </c>
+      <c r="C205">
+        <v>90</v>
+      </c>
+      <c r="D205">
+        <v>96</v>
+      </c>
+      <c r="E205">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="F205">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A206" t="s">
+        <v>140</v>
+      </c>
+      <c r="B206" t="s">
+        <v>1</v>
+      </c>
+      <c r="C206">
+        <v>90</v>
+      </c>
+      <c r="D206">
+        <v>113</v>
+      </c>
+      <c r="E206">
+        <f t="shared" si="6"/>
+        <v>23</v>
+      </c>
+      <c r="F206">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
+        <v>140</v>
+      </c>
+      <c r="B207" t="s">
+        <v>123</v>
+      </c>
+      <c r="C207">
+        <v>90</v>
+      </c>
+      <c r="D207">
+        <v>102</v>
+      </c>
+      <c r="E207">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="F207">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
+        <v>140</v>
+      </c>
+      <c r="B208" t="s">
+        <v>2</v>
+      </c>
+      <c r="C208">
+        <v>90</v>
+      </c>
+      <c r="D208">
+        <v>114</v>
+      </c>
+      <c r="E208">
+        <f t="shared" si="6"/>
+        <v>24</v>
+      </c>
+      <c r="F208">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A209" t="s">
+        <v>140</v>
+      </c>
+      <c r="B209" t="s">
+        <v>3</v>
+      </c>
+      <c r="C209">
+        <v>90</v>
+      </c>
+      <c r="D209">
+        <v>84</v>
+      </c>
+      <c r="E209">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F209">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
+        <v>140</v>
+      </c>
+      <c r="B210" t="s">
+        <v>124</v>
+      </c>
+      <c r="C210">
+        <v>90</v>
+      </c>
+      <c r="D210">
+        <v>79</v>
+      </c>
+      <c r="E210">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F210">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
+        <v>140</v>
+      </c>
+      <c r="B211" t="s">
+        <v>5</v>
+      </c>
+      <c r="C211">
+        <v>90</v>
+      </c>
+      <c r="D211">
+        <v>50</v>
+      </c>
+      <c r="E211">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F211">
+        <f t="shared" si="7"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A212" t="s">
+        <v>140</v>
+      </c>
+      <c r="B212" t="s">
+        <v>6</v>
+      </c>
+      <c r="C212">
+        <v>90</v>
+      </c>
+      <c r="D212">
+        <v>94</v>
+      </c>
+      <c r="E212">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="F212">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
+        <v>140</v>
+      </c>
+      <c r="B213" t="s">
+        <v>115</v>
+      </c>
+      <c r="C213">
+        <v>90</v>
+      </c>
+      <c r="D213">
+        <v>87</v>
+      </c>
+      <c r="E213">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F213">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A214" t="s">
+        <v>140</v>
+      </c>
+      <c r="B214" t="s">
+        <v>8</v>
+      </c>
+      <c r="C214">
+        <v>90</v>
+      </c>
+      <c r="D214">
+        <v>97</v>
+      </c>
+      <c r="E214">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="F214">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A215" t="s">
+        <v>140</v>
+      </c>
+      <c r="B215" t="s">
+        <v>9</v>
+      </c>
+      <c r="C215">
+        <v>90</v>
+      </c>
+      <c r="D215">
+        <v>117</v>
+      </c>
+      <c r="E215">
+        <f t="shared" ref="E215:E250" si="8">IF(D215-C215&gt;0,D215-C215,0)</f>
+        <v>27</v>
+      </c>
+      <c r="F215">
+        <f t="shared" ref="F215:F250" si="9">IF(D215-C215&lt;0,C215-D215,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A216" t="s">
+        <v>140</v>
+      </c>
+      <c r="B216" t="s">
+        <v>10</v>
+      </c>
+      <c r="C216">
+        <v>90</v>
+      </c>
+      <c r="D216">
+        <v>79</v>
+      </c>
+      <c r="E216">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F216">
+        <f t="shared" si="9"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
+        <v>140</v>
+      </c>
+      <c r="B217" t="s">
+        <v>11</v>
+      </c>
+      <c r="C217">
+        <v>90</v>
+      </c>
+      <c r="D217">
+        <v>82</v>
+      </c>
+      <c r="E217">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F217">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A218" t="s">
+        <v>140</v>
+      </c>
+      <c r="B218" t="s">
+        <v>1</v>
+      </c>
+      <c r="C218">
+        <v>90</v>
+      </c>
+      <c r="D218">
+        <v>90</v>
+      </c>
+      <c r="E218">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F218">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A219" t="s">
+        <v>140</v>
+      </c>
+      <c r="B219" t="s">
+        <v>123</v>
+      </c>
+      <c r="C219">
+        <v>90</v>
+      </c>
+      <c r="D219">
+        <v>127</v>
+      </c>
+      <c r="E219">
+        <f t="shared" si="8"/>
+        <v>37</v>
+      </c>
+      <c r="F219">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A220" t="s">
+        <v>140</v>
+      </c>
+      <c r="B220" t="s">
+        <v>2</v>
+      </c>
+      <c r="C220">
+        <v>90</v>
+      </c>
+      <c r="D220">
+        <v>74</v>
+      </c>
+      <c r="E220">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F220">
+        <f t="shared" si="9"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A221" t="s">
+        <v>140</v>
+      </c>
+      <c r="B221" t="s">
+        <v>3</v>
+      </c>
+      <c r="C221">
+        <v>90</v>
+      </c>
+      <c r="D221">
+        <v>59</v>
+      </c>
+      <c r="E221">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F221">
+        <f t="shared" si="9"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A222" t="s">
+        <v>140</v>
+      </c>
+      <c r="B222" t="s">
+        <v>124</v>
+      </c>
+      <c r="C222">
+        <v>90</v>
+      </c>
+      <c r="D222">
+        <v>94</v>
+      </c>
+      <c r="E222">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="F222">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A223" t="s">
+        <v>140</v>
+      </c>
+      <c r="B223" t="s">
+        <v>5</v>
+      </c>
+      <c r="C223">
+        <v>90</v>
+      </c>
+      <c r="D223">
+        <v>105</v>
+      </c>
+      <c r="E223">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+      <c r="F223">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A224" t="s">
+        <v>140</v>
+      </c>
+      <c r="B224" t="s">
+        <v>6</v>
+      </c>
+      <c r="C224">
+        <v>90</v>
+      </c>
+      <c r="D224">
+        <v>71</v>
+      </c>
+      <c r="E224">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F224">
+        <f t="shared" si="9"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A225" t="s">
+        <v>140</v>
+      </c>
+      <c r="B225" t="s">
+        <v>115</v>
+      </c>
+      <c r="C225">
+        <v>90</v>
+      </c>
+      <c r="D225">
+        <v>94</v>
+      </c>
+      <c r="E225">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="F225">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A226" t="s">
+        <v>140</v>
+      </c>
+      <c r="B226" t="s">
+        <v>8</v>
+      </c>
+      <c r="C226">
+        <v>90</v>
+      </c>
+      <c r="D226">
+        <v>65</v>
+      </c>
+      <c r="E226">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F226">
+        <f t="shared" si="9"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A227" t="s">
+        <v>140</v>
+      </c>
+      <c r="B227" t="s">
+        <v>9</v>
+      </c>
+      <c r="C227">
+        <v>90</v>
+      </c>
+      <c r="D227">
+        <v>87</v>
+      </c>
+      <c r="E227">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F227">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A228" t="s">
+        <v>140</v>
+      </c>
+      <c r="B228" t="s">
+        <v>10</v>
+      </c>
+      <c r="C228">
+        <v>90</v>
+      </c>
+      <c r="D228">
+        <v>99</v>
+      </c>
+      <c r="E228">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="F228">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A229" t="s">
+        <v>140</v>
+      </c>
+      <c r="B229" t="s">
+        <v>11</v>
+      </c>
+      <c r="C229">
+        <v>90</v>
+      </c>
+      <c r="D229">
+        <v>102</v>
+      </c>
+      <c r="E229">
+        <f t="shared" si="8"/>
+        <v>12</v>
+      </c>
+      <c r="F229">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A230" t="s">
+        <v>140</v>
+      </c>
+      <c r="B230" t="s">
+        <v>1</v>
+      </c>
+      <c r="C230">
+        <v>90</v>
+      </c>
+      <c r="D230">
+        <v>82</v>
+      </c>
+      <c r="E230">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F230">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A231" t="s">
+        <v>140</v>
+      </c>
+      <c r="B231" t="s">
+        <v>123</v>
+      </c>
+      <c r="C231">
+        <v>90</v>
+      </c>
+      <c r="D231">
+        <v>87</v>
+      </c>
+      <c r="E231">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F231">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A232" t="s">
+        <v>140</v>
+      </c>
+      <c r="B232" t="s">
+        <v>2</v>
+      </c>
+      <c r="C232">
+        <v>90</v>
+      </c>
+      <c r="D232">
+        <v>105</v>
+      </c>
+      <c r="E232">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+      <c r="F232">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A233" t="s">
+        <v>140</v>
+      </c>
+      <c r="B233" t="s">
+        <v>3</v>
+      </c>
+      <c r="C233">
+        <v>90</v>
+      </c>
+      <c r="D233">
+        <v>104</v>
+      </c>
+      <c r="E233">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+      <c r="F233">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A234" t="s">
+        <v>140</v>
+      </c>
+      <c r="B234" t="s">
+        <v>124</v>
+      </c>
+      <c r="C234">
+        <v>90</v>
+      </c>
+      <c r="D234">
+        <v>95</v>
+      </c>
+      <c r="E234">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="F234">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A235" t="s">
+        <v>140</v>
+      </c>
+      <c r="B235" t="s">
+        <v>5</v>
+      </c>
+      <c r="C235">
+        <v>90</v>
+      </c>
+      <c r="D235">
+        <v>81</v>
+      </c>
+      <c r="E235">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F235">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A236" t="s">
+        <v>140</v>
+      </c>
+      <c r="B236" t="s">
+        <v>6</v>
+      </c>
+      <c r="C236">
+        <v>90</v>
+      </c>
+      <c r="D236">
+        <v>125</v>
+      </c>
+      <c r="E236">
+        <f t="shared" si="8"/>
+        <v>35</v>
+      </c>
+      <c r="F236">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A237" t="s">
+        <v>140</v>
+      </c>
+      <c r="B237" t="s">
+        <v>115</v>
+      </c>
+      <c r="C237">
+        <v>90</v>
+      </c>
+      <c r="D237">
+        <v>110</v>
+      </c>
+      <c r="E237">
+        <f t="shared" si="8"/>
+        <v>20</v>
+      </c>
+      <c r="F237">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A238" t="s">
+        <v>140</v>
+      </c>
+      <c r="B238" t="s">
+        <v>8</v>
+      </c>
+      <c r="C238">
+        <v>90</v>
+      </c>
+      <c r="D238">
+        <v>88</v>
+      </c>
+      <c r="E238">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F238">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A239" t="s">
+        <v>140</v>
+      </c>
+      <c r="B239" t="s">
+        <v>9</v>
+      </c>
+      <c r="C239">
+        <v>90</v>
+      </c>
+      <c r="D239">
+        <v>65</v>
+      </c>
+      <c r="E239">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F239">
+        <f t="shared" si="9"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A240" t="s">
+        <v>140</v>
+      </c>
+      <c r="B240" t="s">
+        <v>10</v>
+      </c>
+      <c r="C240">
+        <v>90</v>
+      </c>
+      <c r="D240">
+        <v>83</v>
+      </c>
+      <c r="E240">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F240">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A241" t="s">
+        <v>140</v>
+      </c>
+      <c r="B241" t="s">
+        <v>11</v>
+      </c>
+      <c r="C241">
+        <v>90</v>
+      </c>
+      <c r="D241">
+        <v>80</v>
+      </c>
+      <c r="E241">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F241">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A242" t="s">
+        <v>140</v>
+      </c>
+      <c r="B242" t="s">
+        <v>1</v>
+      </c>
+      <c r="C242">
+        <v>90</v>
+      </c>
+      <c r="D242">
+        <v>92</v>
+      </c>
+      <c r="E242">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="F242">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A243" t="s">
+        <v>140</v>
+      </c>
+      <c r="B243" t="s">
+        <v>123</v>
+      </c>
+      <c r="C243">
+        <v>90</v>
+      </c>
+      <c r="D243">
+        <v>106</v>
+      </c>
+      <c r="E243">
+        <f t="shared" si="8"/>
+        <v>16</v>
+      </c>
+      <c r="F243">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A244" t="s">
+        <v>140</v>
+      </c>
+      <c r="B244" t="s">
+        <v>2</v>
+      </c>
+      <c r="C244">
+        <v>90</v>
+      </c>
+      <c r="D244">
+        <v>109</v>
+      </c>
+      <c r="E244">
+        <f t="shared" si="8"/>
+        <v>19</v>
+      </c>
+      <c r="F244">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A245" t="s">
+        <v>140</v>
+      </c>
+      <c r="B245" t="s">
+        <v>3</v>
+      </c>
+      <c r="C245">
+        <v>90</v>
+      </c>
+      <c r="D245">
+        <v>95</v>
+      </c>
+      <c r="E245">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="F245">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A246" t="s">
+        <v>140</v>
+      </c>
+      <c r="B246" t="s">
+        <v>124</v>
+      </c>
+      <c r="C246">
+        <v>90</v>
+      </c>
+      <c r="D246">
+        <v>110</v>
+      </c>
+      <c r="E246">
+        <f t="shared" si="8"/>
+        <v>20</v>
+      </c>
+      <c r="F246">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A247" t="s">
+        <v>140</v>
+      </c>
+      <c r="B247" t="s">
+        <v>5</v>
+      </c>
+      <c r="C247">
+        <v>90</v>
+      </c>
+      <c r="D247">
+        <v>98</v>
+      </c>
+      <c r="E247">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="F247">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A248" t="s">
+        <v>140</v>
+      </c>
+      <c r="B248" t="s">
+        <v>6</v>
+      </c>
+      <c r="C248">
+        <v>90</v>
+      </c>
+      <c r="D248">
+        <v>70</v>
+      </c>
+      <c r="E248">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F248">
+        <f t="shared" si="9"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A249" t="s">
+        <v>140</v>
+      </c>
+      <c r="B249" t="s">
+        <v>115</v>
+      </c>
+      <c r="C249">
+        <v>90</v>
+      </c>
+      <c r="D249">
+        <v>101</v>
+      </c>
+      <c r="E249">
+        <f t="shared" si="8"/>
+        <v>11</v>
+      </c>
+      <c r="F249">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A250" t="s">
+        <v>140</v>
+      </c>
+      <c r="B250" t="s">
+        <v>8</v>
+      </c>
+      <c r="C250">
+        <v>90</v>
+      </c>
+      <c r="D250">
+        <v>98</v>
+      </c>
+      <c r="E250">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="F250">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D251" t="s">
+        <v>122</v>
+      </c>
+      <c r="E251">
+        <f>SUM(E2:E250)</f>
+        <v>2553</v>
+      </c>
+      <c r="F251">
+        <f>SUM(F2:F250)</f>
+        <v>2817</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D253" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E253" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="F253" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D254" t="s">
+        <v>1</v>
+      </c>
+      <c r="E254">
+        <f>SUMIF($B$2:$B$250,$D254,E$2:E$250)</f>
+        <v>210</v>
+      </c>
+      <c r="F254">
+        <f>SUMIF($B$2:$B$250,$D254,F$2:F$250)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D255" t="s">
+        <v>123</v>
+      </c>
+      <c r="E255">
+        <f t="shared" ref="E255:F265" si="10">SUMIF($B$2:$B$250,$D255,E$2:E$250)</f>
+        <v>218</v>
+      </c>
+      <c r="F255">
+        <f t="shared" si="10"/>
+        <v>249</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D256" t="s">
+        <v>2</v>
+      </c>
+      <c r="E256">
+        <f t="shared" si="10"/>
+        <v>266</v>
+      </c>
+      <c r="F256">
+        <f t="shared" si="10"/>
+        <v>185</v>
+      </c>
+    </row>
+    <row r="257" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D257" t="s">
+        <v>3</v>
+      </c>
+      <c r="E257">
+        <f t="shared" si="10"/>
+        <v>245</v>
+      </c>
+      <c r="F257">
+        <f t="shared" si="10"/>
+        <v>252</v>
+      </c>
+    </row>
+    <row r="258" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D258" t="s">
+        <v>124</v>
+      </c>
+      <c r="E258">
+        <f t="shared" si="10"/>
         <v>199</v>
       </c>
-      <c r="F165">
-        <f t="shared" si="6"/>
-        <v>103</v>
-      </c>
-    </row>
-    <row r="167" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D167" t="s">
+      <c r="F258">
+        <f t="shared" si="10"/>
+        <v>259</v>
+      </c>
+    </row>
+    <row r="259" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D259" t="s">
+        <v>5</v>
+      </c>
+      <c r="E259">
+        <f t="shared" si="10"/>
+        <v>231</v>
+      </c>
+      <c r="F259">
+        <f t="shared" si="10"/>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="260" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D260" t="s">
+        <v>6</v>
+      </c>
+      <c r="E260">
+        <f t="shared" si="10"/>
+        <v>156</v>
+      </c>
+      <c r="F260">
+        <f t="shared" si="10"/>
+        <v>237</v>
+      </c>
+    </row>
+    <row r="261" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D261" t="s">
+        <v>115</v>
+      </c>
+      <c r="E261">
+        <f t="shared" si="10"/>
+        <v>278</v>
+      </c>
+      <c r="F261">
+        <f t="shared" si="10"/>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="262" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D262" t="s">
+        <v>8</v>
+      </c>
+      <c r="E262">
+        <f t="shared" si="10"/>
+        <v>81</v>
+      </c>
+      <c r="F262">
+        <f t="shared" si="10"/>
+        <v>305</v>
+      </c>
+    </row>
+    <row r="263" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D263" t="s">
+        <v>9</v>
+      </c>
+      <c r="E263">
+        <f t="shared" si="10"/>
+        <v>277</v>
+      </c>
+      <c r="F263">
+        <f t="shared" si="10"/>
+        <v>246</v>
+      </c>
+    </row>
+    <row r="264" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D264" t="s">
+        <v>10</v>
+      </c>
+      <c r="E264">
+        <f t="shared" si="10"/>
+        <v>165</v>
+      </c>
+      <c r="F264">
+        <f t="shared" si="10"/>
+        <v>279</v>
+      </c>
+    </row>
+    <row r="265" spans="4:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D265" t="s">
+        <v>11</v>
+      </c>
+      <c r="E265">
+        <f t="shared" si="10"/>
+        <v>227</v>
+      </c>
+      <c r="F265">
+        <f t="shared" si="10"/>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="267" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D267" t="s">
         <v>16</v>
       </c>
-      <c r="E167" s="12" t="s">
+      <c r="E267" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="F167" s="12" t="s">
+      <c r="F267" s="12" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="168" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D168" t="s">
+    <row r="268" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D268" t="s">
         <v>17</v>
       </c>
-      <c r="E168" s="20">
+      <c r="E268" s="20">
+        <f>AVERAGEIF($A$2:$A$250,$D268,E$2:E$250)</f>
         <v>5</v>
       </c>
-      <c r="F168" s="20">
+      <c r="F268" s="20">
+        <f>AVERAGEIF($A$2:$A$250,$D268,F$2:F$250)</f>
         <v>4.204081632653061</v>
       </c>
     </row>
-    <row r="169" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D169" t="s">
+    <row r="269" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D269" t="s">
         <v>18</v>
       </c>
-      <c r="E169" s="20">
+      <c r="E269" s="20">
+        <f t="shared" ref="E269:F272" si="11">AVERAGEIF($A$2:$A$250,$D269,E$2:E$250)</f>
         <v>2.34</v>
       </c>
-      <c r="F169" s="20">
+      <c r="F269" s="20">
+        <f t="shared" si="11"/>
         <v>25.6</v>
       </c>
     </row>
-    <row r="170" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D170" t="s">
+    <row r="270" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D270" t="s">
         <v>19</v>
       </c>
-      <c r="E170" s="20">
+      <c r="E270" s="20">
+        <f t="shared" si="11"/>
         <v>32.159999999999997</v>
       </c>
-      <c r="F170" s="20">
+      <c r="F270" s="20">
+        <f t="shared" si="11"/>
         <v>2.5</v>
+      </c>
+    </row>
+    <row r="271" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D271" t="s">
+        <v>139</v>
+      </c>
+      <c r="E271" s="20">
+        <f t="shared" si="11"/>
+        <v>3.64</v>
+      </c>
+      <c r="F271" s="20">
+        <f t="shared" si="11"/>
+        <v>18.399999999999999</v>
+      </c>
+    </row>
+    <row r="272" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D272" t="s">
+        <v>140</v>
+      </c>
+      <c r="E272" s="20">
+        <f t="shared" si="11"/>
+        <v>8.02</v>
+      </c>
+      <c r="F272" s="20">
+        <f>AVERAGEIF($A$2:$A$250,$D272,F$2:F$250)</f>
+        <v>5.72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nuevas gráficas tiempo extra e inactividad
</commit_message>
<xml_diff>
--- a/app_salud/app/logic/data/set_de_datos_1.xlsx
+++ b/app_salud/app/logic/data/set_de_datos_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rstudio\software_salud\app_salud\app\logic\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6186A29-FBB7-4DA0-8F5B-5EAFE03369C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA7162E-67CB-4B98-A025-FD14D2B4E4B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{A035267E-5D3E-4097-B788-79B64BEF5509}"/>
   </bookViews>
@@ -469,9 +469,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m\-d\-yyyy\ h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -554,7 +553,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -601,7 +600,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2915,7 +2913,7 @@
       <c r="M1" s="9"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
         <v>101</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -2953,7 +2951,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="21"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="4" t="s">
         <v>104</v>
       </c>
@@ -2989,7 +2987,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="21"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="4" t="s">
         <v>105</v>
       </c>
@@ -3025,7 +3023,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="21"/>
+      <c r="A5" s="20"/>
       <c r="B5" s="4" t="s">
         <v>106</v>
       </c>
@@ -3061,7 +3059,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="21"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="4" t="s">
         <v>107</v>
       </c>
@@ -3097,7 +3095,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="21"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="4" t="s">
         <v>108</v>
       </c>
@@ -3133,7 +3131,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="21"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="4" t="s">
         <v>109</v>
       </c>
@@ -3169,7 +3167,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="21"/>
+      <c r="A9" s="20"/>
       <c r="B9" s="4" t="s">
         <v>110</v>
       </c>
@@ -3205,7 +3203,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="21"/>
+      <c r="A10" s="20"/>
       <c r="B10" s="4" t="s">
         <v>111</v>
       </c>
@@ -3241,7 +3239,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="21"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="4" t="s">
         <v>112</v>
       </c>
@@ -3277,7 +3275,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="21"/>
+      <c r="A12" s="20"/>
       <c r="B12" s="4" t="s">
         <v>113</v>
       </c>
@@ -3313,13 +3311,13 @@
       </c>
     </row>
     <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="20" t="s">
         <v>52</v>
       </c>
       <c r="D13" s="5">
@@ -4123,21 +4121,21 @@
     <row r="1" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="13"/>
       <c r="B1" s="13"/>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23" t="s">
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22" t="s">
         <v>89</v>
       </c>
     </row>
@@ -4182,12 +4180,12 @@
       <c r="N2" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="O2" s="23" t="s">
+      <c r="O2" s="22" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>127</v>
       </c>
       <c r="B3" s="14" t="s">
@@ -4234,7 +4232,7 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="22"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="14" t="s">
         <v>129</v>
       </c>
@@ -4279,7 +4277,7 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="21" t="s">
         <v>130</v>
       </c>
       <c r="B5" s="14" t="s">
@@ -4326,7 +4324,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="22"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="14" t="s">
         <v>129</v>
       </c>
@@ -4371,7 +4369,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="21" t="s">
         <v>131</v>
       </c>
       <c r="B7" s="14" t="s">
@@ -4418,7 +4416,7 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="22"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="14" t="s">
         <v>129</v>
       </c>
@@ -4463,7 +4461,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="21" t="s">
         <v>132</v>
       </c>
       <c r="B9" s="14" t="s">
@@ -4510,7 +4508,7 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="22"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="14" t="s">
         <v>129</v>
       </c>
@@ -4555,7 +4553,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="21" t="s">
         <v>133</v>
       </c>
       <c r="B11" s="14" t="s">
@@ -4602,7 +4600,7 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="22"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="14" t="s">
         <v>129</v>
       </c>
@@ -4647,7 +4645,7 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="21" t="s">
         <v>134</v>
       </c>
       <c r="B13" s="14" t="s">
@@ -4694,7 +4692,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="22"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="14" t="s">
         <v>129</v>
       </c>
@@ -7397,8 +7395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{615EFB19-F474-4215-A4C4-27A7F36F1049}">
   <dimension ref="A1:F272"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A250" workbookViewId="0">
-      <selection activeCell="F273" sqref="F273"/>
+    <sheetView tabSelected="1" topLeftCell="A247" workbookViewId="0">
+      <selection activeCell="F255" sqref="F255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7448,7 +7446,7 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <f>IF(D2-C2&lt;0,C2-D2,0)</f>
+        <f>IF(D2-C2&lt;0,D2-C2,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -7470,8 +7468,8 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F66" si="1">IF(D3-C3&lt;0,C3-D3,0)</f>
-        <v>4</v>
+        <f t="shared" ref="F3:F66" si="1">IF(D3-C3&lt;0,D3-C3,0)</f>
+        <v>-4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -7537,7 +7535,7 @@
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -7603,7 +7601,7 @@
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>-24</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -7647,7 +7645,7 @@
       </c>
       <c r="F11">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -7735,7 +7733,7 @@
       </c>
       <c r="F15">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -7757,7 +7755,7 @@
       </c>
       <c r="F16">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -7845,7 +7843,7 @@
       </c>
       <c r="F20">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -7889,7 +7887,7 @@
       </c>
       <c r="F22">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -7911,7 +7909,7 @@
       </c>
       <c r="F23">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -7933,7 +7931,7 @@
       </c>
       <c r="F24">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -7977,7 +7975,7 @@
       </c>
       <c r="F26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -8021,7 +8019,7 @@
       </c>
       <c r="F28">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>-12</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -8043,7 +8041,7 @@
       </c>
       <c r="F29">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -8131,7 +8129,7 @@
       </c>
       <c r="F33">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>-14</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -8175,7 +8173,7 @@
       </c>
       <c r="F35">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>-14</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -8285,7 +8283,7 @@
       </c>
       <c r="F40">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>-28</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -8351,7 +8349,7 @@
       </c>
       <c r="F43">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -8373,7 +8371,7 @@
       </c>
       <c r="F44">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -8395,7 +8393,7 @@
       </c>
       <c r="F45">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -8439,7 +8437,7 @@
       </c>
       <c r="F47">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>-11</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -8461,7 +8459,7 @@
       </c>
       <c r="F48">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -8483,7 +8481,7 @@
       </c>
       <c r="F49">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -8505,7 +8503,7 @@
       </c>
       <c r="F50">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -8549,7 +8547,7 @@
       </c>
       <c r="F52">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -8571,7 +8569,7 @@
       </c>
       <c r="F53">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>-27</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -8615,7 +8613,7 @@
       </c>
       <c r="F55">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -8637,7 +8635,7 @@
       </c>
       <c r="F56">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>-11</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -8659,7 +8657,7 @@
       </c>
       <c r="F57">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>-26</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -8681,7 +8679,7 @@
       </c>
       <c r="F58">
         <f t="shared" si="1"/>
-        <v>38</v>
+        <v>-38</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -8725,7 +8723,7 @@
       </c>
       <c r="F60">
         <f t="shared" si="1"/>
-        <v>37</v>
+        <v>-37</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -8747,7 +8745,7 @@
       </c>
       <c r="F61">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -8769,7 +8767,7 @@
       </c>
       <c r="F62">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>-31</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -8791,7 +8789,7 @@
       </c>
       <c r="F63">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>-23</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -8813,7 +8811,7 @@
       </c>
       <c r="F64">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -8835,7 +8833,7 @@
       </c>
       <c r="F65">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -8857,7 +8855,7 @@
       </c>
       <c r="F66">
         <f t="shared" si="1"/>
-        <v>70</v>
+        <v>-70</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -8878,8 +8876,8 @@
         <v>0</v>
       </c>
       <c r="F67">
-        <f t="shared" ref="F67:F130" si="3">IF(D67-C67&lt;0,C67-D67,0)</f>
-        <v>28</v>
+        <f t="shared" ref="F67:F130" si="3">IF(D67-C67&lt;0,D67-C67,0)</f>
+        <v>-28</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -8901,7 +8899,7 @@
       </c>
       <c r="F68">
         <f t="shared" si="3"/>
-        <v>49</v>
+        <v>-49</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -8923,7 +8921,7 @@
       </c>
       <c r="F69">
         <f t="shared" si="3"/>
-        <v>57</v>
+        <v>-57</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -8945,7 +8943,7 @@
       </c>
       <c r="F70">
         <f t="shared" si="3"/>
-        <v>19</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -8967,7 +8965,7 @@
       </c>
       <c r="F71">
         <f t="shared" si="3"/>
-        <v>66</v>
+        <v>-66</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -8989,7 +8987,7 @@
       </c>
       <c r="F72">
         <f t="shared" si="3"/>
-        <v>23</v>
+        <v>-23</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -9055,7 +9053,7 @@
       </c>
       <c r="F75">
         <f t="shared" si="3"/>
-        <v>43</v>
+        <v>-43</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -9077,7 +9075,7 @@
       </c>
       <c r="F76">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>-12</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -9099,7 +9097,7 @@
       </c>
       <c r="F77">
         <f t="shared" si="3"/>
-        <v>21</v>
+        <v>-21</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -9121,7 +9119,7 @@
       </c>
       <c r="F78">
         <f t="shared" si="3"/>
-        <v>27</v>
+        <v>-27</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -9143,7 +9141,7 @@
       </c>
       <c r="F79">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -9187,7 +9185,7 @@
       </c>
       <c r="F81">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -9209,7 +9207,7 @@
       </c>
       <c r="F82">
         <f t="shared" si="3"/>
-        <v>55</v>
+        <v>-55</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -9231,7 +9229,7 @@
       </c>
       <c r="F83">
         <f t="shared" si="3"/>
-        <v>43</v>
+        <v>-43</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -9253,7 +9251,7 @@
       </c>
       <c r="F84">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>-11</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -9275,7 +9273,7 @@
       </c>
       <c r="F85">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>-48</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -9297,7 +9295,7 @@
       </c>
       <c r="F86">
         <f t="shared" si="3"/>
-        <v>55</v>
+        <v>-55</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -9319,7 +9317,7 @@
       </c>
       <c r="F87">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -9363,7 +9361,7 @@
       </c>
       <c r="F89">
         <f t="shared" si="3"/>
-        <v>37</v>
+        <v>-37</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -9385,7 +9383,7 @@
       </c>
       <c r="F90">
         <f t="shared" si="3"/>
-        <v>75</v>
+        <v>-75</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -9407,7 +9405,7 @@
       </c>
       <c r="F91">
         <f t="shared" si="3"/>
-        <v>37</v>
+        <v>-37</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -9429,7 +9427,7 @@
       </c>
       <c r="F92">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>-13</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -9451,7 +9449,7 @@
       </c>
       <c r="F93">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -9473,7 +9471,7 @@
       </c>
       <c r="F94">
         <f t="shared" si="3"/>
-        <v>21</v>
+        <v>-21</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -9495,7 +9493,7 @@
       </c>
       <c r="F95">
         <f t="shared" si="3"/>
-        <v>25</v>
+        <v>-25</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -9517,7 +9515,7 @@
       </c>
       <c r="F96">
         <f t="shared" si="3"/>
-        <v>61</v>
+        <v>-61</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -9539,7 +9537,7 @@
       </c>
       <c r="F97">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -9561,7 +9559,7 @@
       </c>
       <c r="F98">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>-30</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -9583,7 +9581,7 @@
       </c>
       <c r="F99">
         <f t="shared" si="3"/>
-        <v>47</v>
+        <v>-47</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -9693,7 +9691,7 @@
       </c>
       <c r="F104">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -9957,7 +9955,7 @@
       </c>
       <c r="F116">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -10001,7 +9999,7 @@
       </c>
       <c r="F118">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
@@ -10067,7 +10065,7 @@
       </c>
       <c r="F121">
         <f t="shared" si="3"/>
-        <v>32</v>
+        <v>-32</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -10177,7 +10175,7 @@
       </c>
       <c r="F126">
         <f t="shared" si="3"/>
-        <v>25</v>
+        <v>-25</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
@@ -10286,8 +10284,8 @@
         <v>0</v>
       </c>
       <c r="F131">
-        <f t="shared" ref="F131:F150" si="5">IF(D131-C131&lt;0,C131-D131,0)</f>
-        <v>9</v>
+        <f t="shared" ref="F131:F194" si="5">IF(D131-C131&lt;0,D131-C131,0)</f>
+        <v>-9</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
@@ -10529,7 +10527,7 @@
       </c>
       <c r="F142">
         <f t="shared" si="5"/>
-        <v>27</v>
+        <v>-27</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
@@ -10573,7 +10571,7 @@
       </c>
       <c r="F144">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>-16</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
@@ -10639,7 +10637,7 @@
       </c>
       <c r="F147">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
@@ -10726,7 +10724,7 @@
         <v>41</v>
       </c>
       <c r="F151">
-        <f t="shared" ref="F151:F214" si="7">IF(D151-C151&lt;0,C151-D151,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -10748,8 +10746,8 @@
         <v>0</v>
       </c>
       <c r="F152">
-        <f t="shared" si="7"/>
-        <v>22</v>
+        <f t="shared" si="5"/>
+        <v>-22</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.3">
@@ -10770,7 +10768,7 @@
         <v>11</v>
       </c>
       <c r="F153">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -10792,8 +10790,8 @@
         <v>0</v>
       </c>
       <c r="F154">
-        <f t="shared" si="7"/>
-        <v>29</v>
+        <f t="shared" si="5"/>
+        <v>-29</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
@@ -10814,7 +10812,7 @@
         <v>10</v>
       </c>
       <c r="F155">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -10836,7 +10834,7 @@
         <v>10</v>
       </c>
       <c r="F156">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -10858,8 +10856,8 @@
         <v>0</v>
       </c>
       <c r="F157">
-        <f t="shared" si="7"/>
-        <v>10</v>
+        <f t="shared" si="5"/>
+        <v>-10</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.3">
@@ -10880,8 +10878,8 @@
         <v>0</v>
       </c>
       <c r="F158">
-        <f t="shared" si="7"/>
-        <v>20</v>
+        <f t="shared" si="5"/>
+        <v>-20</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.3">
@@ -10902,8 +10900,8 @@
         <v>0</v>
       </c>
       <c r="F159">
-        <f t="shared" si="7"/>
-        <v>33</v>
+        <f t="shared" si="5"/>
+        <v>-33</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.3">
@@ -10924,8 +10922,8 @@
         <v>0</v>
       </c>
       <c r="F160">
-        <f t="shared" si="7"/>
-        <v>2</v>
+        <f t="shared" si="5"/>
+        <v>-2</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.3">
@@ -10946,8 +10944,8 @@
         <v>0</v>
       </c>
       <c r="F161">
-        <f t="shared" si="7"/>
-        <v>40</v>
+        <f t="shared" si="5"/>
+        <v>-40</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.3">
@@ -10968,8 +10966,8 @@
         <v>0</v>
       </c>
       <c r="F162">
-        <f t="shared" si="7"/>
-        <v>22</v>
+        <f t="shared" si="5"/>
+        <v>-22</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.3">
@@ -10990,8 +10988,8 @@
         <v>0</v>
       </c>
       <c r="F163">
-        <f t="shared" si="7"/>
-        <v>27</v>
+        <f t="shared" si="5"/>
+        <v>-27</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.3">
@@ -11012,8 +11010,8 @@
         <v>0</v>
       </c>
       <c r="F164">
-        <f t="shared" si="7"/>
-        <v>4</v>
+        <f t="shared" si="5"/>
+        <v>-4</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.3">
@@ -11034,8 +11032,8 @@
         <v>0</v>
       </c>
       <c r="F165">
-        <f t="shared" si="7"/>
-        <v>14</v>
+        <f t="shared" si="5"/>
+        <v>-14</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.3">
@@ -11056,8 +11054,8 @@
         <v>0</v>
       </c>
       <c r="F166">
-        <f t="shared" si="7"/>
-        <v>8</v>
+        <f t="shared" si="5"/>
+        <v>-8</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.3">
@@ -11078,8 +11076,8 @@
         <v>0</v>
       </c>
       <c r="F167">
-        <f t="shared" si="7"/>
-        <v>7</v>
+        <f t="shared" si="5"/>
+        <v>-7</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.3">
@@ -11100,8 +11098,8 @@
         <v>0</v>
       </c>
       <c r="F168">
-        <f t="shared" si="7"/>
-        <v>10</v>
+        <f t="shared" si="5"/>
+        <v>-10</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.3">
@@ -11122,7 +11120,7 @@
         <v>10</v>
       </c>
       <c r="F169">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -11144,8 +11142,8 @@
         <v>0</v>
       </c>
       <c r="F170">
-        <f t="shared" si="7"/>
-        <v>9</v>
+        <f t="shared" si="5"/>
+        <v>-9</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.3">
@@ -11166,8 +11164,8 @@
         <v>0</v>
       </c>
       <c r="F171">
-        <f t="shared" si="7"/>
-        <v>68</v>
+        <f t="shared" si="5"/>
+        <v>-68</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.3">
@@ -11188,8 +11186,8 @@
         <v>0</v>
       </c>
       <c r="F172">
-        <f t="shared" si="7"/>
-        <v>33</v>
+        <f t="shared" si="5"/>
+        <v>-33</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.3">
@@ -11210,8 +11208,8 @@
         <v>0</v>
       </c>
       <c r="F173">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f t="shared" si="5"/>
+        <v>-1</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.3">
@@ -11232,8 +11230,8 @@
         <v>0</v>
       </c>
       <c r="F174">
-        <f t="shared" si="7"/>
-        <v>21</v>
+        <f t="shared" si="5"/>
+        <v>-21</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.3">
@@ -11254,8 +11252,8 @@
         <v>0</v>
       </c>
       <c r="F175">
-        <f t="shared" si="7"/>
-        <v>55</v>
+        <f t="shared" si="5"/>
+        <v>-55</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.3">
@@ -11276,8 +11274,8 @@
         <v>0</v>
       </c>
       <c r="F176">
-        <f t="shared" si="7"/>
-        <v>39</v>
+        <f t="shared" si="5"/>
+        <v>-39</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.3">
@@ -11298,8 +11296,8 @@
         <v>0</v>
       </c>
       <c r="F177">
-        <f t="shared" si="7"/>
-        <v>24</v>
+        <f t="shared" si="5"/>
+        <v>-24</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.3">
@@ -11320,8 +11318,8 @@
         <v>0</v>
       </c>
       <c r="F178">
-        <f t="shared" si="7"/>
-        <v>30</v>
+        <f t="shared" si="5"/>
+        <v>-30</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.3">
@@ -11342,8 +11340,8 @@
         <v>0</v>
       </c>
       <c r="F179">
-        <f t="shared" si="7"/>
-        <v>27</v>
+        <f t="shared" si="5"/>
+        <v>-27</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.3">
@@ -11364,8 +11362,8 @@
         <v>0</v>
       </c>
       <c r="F180">
-        <f t="shared" si="7"/>
-        <v>43</v>
+        <f t="shared" si="5"/>
+        <v>-43</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.3">
@@ -11386,8 +11384,8 @@
         <v>0</v>
       </c>
       <c r="F181">
-        <f t="shared" si="7"/>
-        <v>10</v>
+        <f t="shared" si="5"/>
+        <v>-10</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.3">
@@ -11408,8 +11406,8 @@
         <v>0</v>
       </c>
       <c r="F182">
-        <f t="shared" si="7"/>
-        <v>17</v>
+        <f t="shared" si="5"/>
+        <v>-17</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.3">
@@ -11430,7 +11428,7 @@
         <v>29</v>
       </c>
       <c r="F183">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -11452,8 +11450,8 @@
         <v>0</v>
       </c>
       <c r="F184">
-        <f t="shared" si="7"/>
-        <v>6</v>
+        <f t="shared" si="5"/>
+        <v>-6</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.3">
@@ -11474,8 +11472,8 @@
         <v>0</v>
       </c>
       <c r="F185">
-        <f t="shared" si="7"/>
-        <v>14</v>
+        <f t="shared" si="5"/>
+        <v>-14</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.3">
@@ -11496,7 +11494,7 @@
         <v>14</v>
       </c>
       <c r="F186">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -11518,7 +11516,7 @@
         <v>12</v>
       </c>
       <c r="F187">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -11540,8 +11538,8 @@
         <v>0</v>
       </c>
       <c r="F188">
-        <f t="shared" si="7"/>
-        <v>21</v>
+        <f t="shared" si="5"/>
+        <v>-21</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.3">
@@ -11562,8 +11560,8 @@
         <v>0</v>
       </c>
       <c r="F189">
-        <f t="shared" si="7"/>
-        <v>31</v>
+        <f t="shared" si="5"/>
+        <v>-31</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.3">
@@ -11584,8 +11582,8 @@
         <v>0</v>
       </c>
       <c r="F190">
-        <f t="shared" si="7"/>
-        <v>20</v>
+        <f t="shared" si="5"/>
+        <v>-20</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.3">
@@ -11606,8 +11604,8 @@
         <v>0</v>
       </c>
       <c r="F191">
-        <f t="shared" si="7"/>
-        <v>7</v>
+        <f t="shared" si="5"/>
+        <v>-7</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.3">
@@ -11628,8 +11626,8 @@
         <v>0</v>
       </c>
       <c r="F192">
-        <f t="shared" si="7"/>
-        <v>46</v>
+        <f t="shared" si="5"/>
+        <v>-46</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.3">
@@ -11650,8 +11648,8 @@
         <v>0</v>
       </c>
       <c r="F193">
-        <f t="shared" si="7"/>
-        <v>29</v>
+        <f t="shared" si="5"/>
+        <v>-29</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.3">
@@ -11672,8 +11670,8 @@
         <v>0</v>
       </c>
       <c r="F194">
-        <f t="shared" si="7"/>
-        <v>26</v>
+        <f t="shared" si="5"/>
+        <v>-26</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.3">
@@ -11694,8 +11692,8 @@
         <v>0</v>
       </c>
       <c r="F195">
-        <f t="shared" si="7"/>
-        <v>18</v>
+        <f t="shared" ref="F195:F250" si="7">IF(D195-C195&lt;0,D195-C195,0)</f>
+        <v>-18</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.3">
@@ -11717,7 +11715,7 @@
       </c>
       <c r="F196">
         <f t="shared" si="7"/>
-        <v>33</v>
+        <v>-33</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.3">
@@ -11739,7 +11737,7 @@
       </c>
       <c r="F197">
         <f t="shared" si="7"/>
-        <v>16</v>
+        <v>-16</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.3">
@@ -11783,7 +11781,7 @@
       </c>
       <c r="F199">
         <f t="shared" si="7"/>
-        <v>12</v>
+        <v>-12</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.3">
@@ -11805,7 +11803,7 @@
       </c>
       <c r="F200">
         <f t="shared" si="7"/>
-        <v>16</v>
+        <v>-16</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.3">
@@ -11849,7 +11847,7 @@
       </c>
       <c r="F202">
         <f t="shared" si="7"/>
-        <v>23</v>
+        <v>-23</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.3">
@@ -11893,7 +11891,7 @@
       </c>
       <c r="F204">
         <f t="shared" si="7"/>
-        <v>6</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.3">
@@ -12003,7 +12001,7 @@
       </c>
       <c r="F209">
         <f t="shared" si="7"/>
-        <v>6</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.3">
@@ -12025,7 +12023,7 @@
       </c>
       <c r="F210">
         <f t="shared" si="7"/>
-        <v>11</v>
+        <v>-11</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.3">
@@ -12047,7 +12045,7 @@
       </c>
       <c r="F211">
         <f t="shared" si="7"/>
-        <v>40</v>
+        <v>-40</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.3">
@@ -12091,7 +12089,7 @@
       </c>
       <c r="F213">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.3">
@@ -12134,7 +12132,7 @@
         <v>27</v>
       </c>
       <c r="F215">
-        <f t="shared" ref="F215:F250" si="9">IF(D215-C215&lt;0,C215-D215,0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -12156,8 +12154,8 @@
         <v>0</v>
       </c>
       <c r="F216">
-        <f t="shared" si="9"/>
-        <v>11</v>
+        <f t="shared" si="7"/>
+        <v>-11</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.3">
@@ -12178,8 +12176,8 @@
         <v>0</v>
       </c>
       <c r="F217">
-        <f t="shared" si="9"/>
-        <v>8</v>
+        <f t="shared" si="7"/>
+        <v>-8</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.3">
@@ -12200,7 +12198,7 @@
         <v>0</v>
       </c>
       <c r="F218">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -12222,7 +12220,7 @@
         <v>37</v>
       </c>
       <c r="F219">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -12244,8 +12242,8 @@
         <v>0</v>
       </c>
       <c r="F220">
-        <f t="shared" si="9"/>
-        <v>16</v>
+        <f t="shared" si="7"/>
+        <v>-16</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.3">
@@ -12266,8 +12264,8 @@
         <v>0</v>
       </c>
       <c r="F221">
-        <f t="shared" si="9"/>
-        <v>31</v>
+        <f t="shared" si="7"/>
+        <v>-31</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.3">
@@ -12288,7 +12286,7 @@
         <v>4</v>
       </c>
       <c r="F222">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -12310,7 +12308,7 @@
         <v>15</v>
       </c>
       <c r="F223">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -12332,8 +12330,8 @@
         <v>0</v>
       </c>
       <c r="F224">
-        <f t="shared" si="9"/>
-        <v>19</v>
+        <f t="shared" si="7"/>
+        <v>-19</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.3">
@@ -12354,7 +12352,7 @@
         <v>4</v>
       </c>
       <c r="F225">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -12376,8 +12374,8 @@
         <v>0</v>
       </c>
       <c r="F226">
-        <f t="shared" si="9"/>
-        <v>25</v>
+        <f t="shared" si="7"/>
+        <v>-25</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.3">
@@ -12398,8 +12396,8 @@
         <v>0</v>
       </c>
       <c r="F227">
-        <f t="shared" si="9"/>
-        <v>3</v>
+        <f t="shared" si="7"/>
+        <v>-3</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.3">
@@ -12420,7 +12418,7 @@
         <v>9</v>
       </c>
       <c r="F228">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -12442,7 +12440,7 @@
         <v>12</v>
       </c>
       <c r="F229">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -12464,8 +12462,8 @@
         <v>0</v>
       </c>
       <c r="F230">
-        <f t="shared" si="9"/>
-        <v>8</v>
+        <f t="shared" si="7"/>
+        <v>-8</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.3">
@@ -12486,8 +12484,8 @@
         <v>0</v>
       </c>
       <c r="F231">
-        <f t="shared" si="9"/>
-        <v>3</v>
+        <f t="shared" si="7"/>
+        <v>-3</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.3">
@@ -12508,7 +12506,7 @@
         <v>15</v>
       </c>
       <c r="F232">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -12530,7 +12528,7 @@
         <v>14</v>
       </c>
       <c r="F233">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -12552,7 +12550,7 @@
         <v>5</v>
       </c>
       <c r="F234">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -12574,8 +12572,8 @@
         <v>0</v>
       </c>
       <c r="F235">
-        <f t="shared" si="9"/>
-        <v>9</v>
+        <f t="shared" si="7"/>
+        <v>-9</v>
       </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.3">
@@ -12596,7 +12594,7 @@
         <v>35</v>
       </c>
       <c r="F236">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -12618,7 +12616,7 @@
         <v>20</v>
       </c>
       <c r="F237">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -12640,8 +12638,8 @@
         <v>0</v>
       </c>
       <c r="F238">
-        <f t="shared" si="9"/>
-        <v>2</v>
+        <f t="shared" si="7"/>
+        <v>-2</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.3">
@@ -12662,8 +12660,8 @@
         <v>0</v>
       </c>
       <c r="F239">
-        <f t="shared" si="9"/>
-        <v>25</v>
+        <f t="shared" si="7"/>
+        <v>-25</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.3">
@@ -12684,8 +12682,8 @@
         <v>0</v>
       </c>
       <c r="F240">
-        <f t="shared" si="9"/>
-        <v>7</v>
+        <f t="shared" si="7"/>
+        <v>-7</v>
       </c>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.3">
@@ -12706,8 +12704,8 @@
         <v>0</v>
       </c>
       <c r="F241">
-        <f t="shared" si="9"/>
-        <v>10</v>
+        <f t="shared" si="7"/>
+        <v>-10</v>
       </c>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.3">
@@ -12728,7 +12726,7 @@
         <v>2</v>
       </c>
       <c r="F242">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -12750,7 +12748,7 @@
         <v>16</v>
       </c>
       <c r="F243">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -12772,7 +12770,7 @@
         <v>19</v>
       </c>
       <c r="F244">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -12794,7 +12792,7 @@
         <v>5</v>
       </c>
       <c r="F245">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -12816,7 +12814,7 @@
         <v>20</v>
       </c>
       <c r="F246">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -12838,7 +12836,7 @@
         <v>8</v>
       </c>
       <c r="F247">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -12860,8 +12858,8 @@
         <v>0</v>
       </c>
       <c r="F248">
-        <f t="shared" si="9"/>
-        <v>20</v>
+        <f t="shared" si="7"/>
+        <v>-20</v>
       </c>
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.3">
@@ -12882,7 +12880,7 @@
         <v>11</v>
       </c>
       <c r="F249">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -12904,7 +12902,7 @@
         <v>8</v>
       </c>
       <c r="F250">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -12918,7 +12916,7 @@
       </c>
       <c r="F251">
         <f>SUM(F2:F250)</f>
-        <v>2817</v>
+        <v>-2817</v>
       </c>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.3">
@@ -12942,7 +12940,7 @@
       </c>
       <c r="F254">
         <f>SUMIF($B$2:$B$250,$D254,F$2:F$250)</f>
-        <v>200</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.3">
@@ -12950,12 +12948,12 @@
         <v>123</v>
       </c>
       <c r="E255">
-        <f t="shared" ref="E255:F265" si="10">SUMIF($B$2:$B$250,$D255,E$2:E$250)</f>
+        <f t="shared" ref="E255:F265" si="9">SUMIF($B$2:$B$250,$D255,E$2:E$250)</f>
         <v>218</v>
       </c>
       <c r="F255">
-        <f t="shared" si="10"/>
-        <v>249</v>
+        <f t="shared" si="9"/>
+        <v>-249</v>
       </c>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.3">
@@ -12963,12 +12961,12 @@
         <v>2</v>
       </c>
       <c r="E256">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>266</v>
       </c>
       <c r="F256">
-        <f t="shared" si="10"/>
-        <v>185</v>
+        <f t="shared" si="9"/>
+        <v>-185</v>
       </c>
     </row>
     <row r="257" spans="4:6" x14ac:dyDescent="0.3">
@@ -12976,12 +12974,12 @@
         <v>3</v>
       </c>
       <c r="E257">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>245</v>
       </c>
       <c r="F257">
-        <f t="shared" si="10"/>
-        <v>252</v>
+        <f t="shared" si="9"/>
+        <v>-252</v>
       </c>
     </row>
     <row r="258" spans="4:6" x14ac:dyDescent="0.3">
@@ -12989,12 +12987,12 @@
         <v>124</v>
       </c>
       <c r="E258">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>199</v>
       </c>
       <c r="F258">
-        <f t="shared" si="10"/>
-        <v>259</v>
+        <f t="shared" si="9"/>
+        <v>-259</v>
       </c>
     </row>
     <row r="259" spans="4:6" x14ac:dyDescent="0.3">
@@ -13002,12 +13000,12 @@
         <v>5</v>
       </c>
       <c r="E259">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>231</v>
       </c>
       <c r="F259">
-        <f t="shared" si="10"/>
-        <v>222</v>
+        <f t="shared" si="9"/>
+        <v>-222</v>
       </c>
     </row>
     <row r="260" spans="4:6" x14ac:dyDescent="0.3">
@@ -13015,12 +13013,12 @@
         <v>6</v>
       </c>
       <c r="E260">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>156</v>
       </c>
       <c r="F260">
-        <f t="shared" si="10"/>
-        <v>237</v>
+        <f t="shared" si="9"/>
+        <v>-237</v>
       </c>
     </row>
     <row r="261" spans="4:6" x14ac:dyDescent="0.3">
@@ -13028,12 +13026,12 @@
         <v>115</v>
       </c>
       <c r="E261">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>278</v>
       </c>
       <c r="F261">
-        <f t="shared" si="10"/>
-        <v>213</v>
+        <f t="shared" si="9"/>
+        <v>-213</v>
       </c>
     </row>
     <row r="262" spans="4:6" x14ac:dyDescent="0.3">
@@ -13041,12 +13039,12 @@
         <v>8</v>
       </c>
       <c r="E262">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>81</v>
       </c>
       <c r="F262">
-        <f t="shared" si="10"/>
-        <v>305</v>
+        <f t="shared" si="9"/>
+        <v>-305</v>
       </c>
     </row>
     <row r="263" spans="4:6" x14ac:dyDescent="0.3">
@@ -13054,12 +13052,12 @@
         <v>9</v>
       </c>
       <c r="E263">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>277</v>
       </c>
       <c r="F263">
-        <f t="shared" si="10"/>
-        <v>246</v>
+        <f t="shared" si="9"/>
+        <v>-246</v>
       </c>
     </row>
     <row r="264" spans="4:6" x14ac:dyDescent="0.3">
@@ -13067,12 +13065,12 @@
         <v>10</v>
       </c>
       <c r="E264">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>165</v>
       </c>
       <c r="F264">
-        <f t="shared" si="10"/>
-        <v>279</v>
+        <f t="shared" si="9"/>
+        <v>-279</v>
       </c>
     </row>
     <row r="265" spans="4:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -13080,12 +13078,12 @@
         <v>11</v>
       </c>
       <c r="E265">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>227</v>
       </c>
       <c r="F265">
-        <f t="shared" si="10"/>
-        <v>170</v>
+        <f t="shared" si="9"/>
+        <v>-170</v>
       </c>
     </row>
     <row r="267" spans="4:6" x14ac:dyDescent="0.3">
@@ -13103,65 +13101,65 @@
       <c r="D268" t="s">
         <v>17</v>
       </c>
-      <c r="E268" s="20">
-        <f>AVERAGEIF($A$2:$A$250,$D268,E$2:E$250)</f>
+      <c r="E268" s="10">
+        <f>ROUND(AVERAGEIF($A$2:$A$250,$D268,E$2:E$250),0)</f>
         <v>5</v>
       </c>
-      <c r="F268" s="20">
-        <f>AVERAGEIF($A$2:$A$250,$D268,F$2:F$250)</f>
-        <v>4.204081632653061</v>
+      <c r="F268" s="10">
+        <f>ABS(ROUND(AVERAGEIF($A$2:$A$250,$D268,F$2:F$250),0))</f>
+        <v>4</v>
       </c>
     </row>
     <row r="269" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D269" t="s">
         <v>18</v>
       </c>
-      <c r="E269" s="20">
-        <f t="shared" ref="E269:F272" si="11">AVERAGEIF($A$2:$A$250,$D269,E$2:E$250)</f>
-        <v>2.34</v>
-      </c>
-      <c r="F269" s="20">
-        <f t="shared" si="11"/>
-        <v>25.6</v>
+      <c r="E269" s="10">
+        <f t="shared" ref="E269:F272" si="10">ROUND(AVERAGEIF($A$2:$A$250,$D269,E$2:E$250),0)</f>
+        <v>2</v>
+      </c>
+      <c r="F269" s="10">
+        <f t="shared" ref="F269:F272" si="11">ABS(ROUND(AVERAGEIF($A$2:$A$250,$D269,F$2:F$250),0))</f>
+        <v>26</v>
       </c>
     </row>
     <row r="270" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D270" t="s">
         <v>19</v>
       </c>
-      <c r="E270" s="20">
+      <c r="E270" s="10">
+        <f t="shared" si="10"/>
+        <v>32</v>
+      </c>
+      <c r="F270" s="10">
         <f t="shared" si="11"/>
-        <v>32.159999999999997</v>
-      </c>
-      <c r="F270" s="20">
-        <f t="shared" si="11"/>
-        <v>2.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="271" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D271" t="s">
         <v>139</v>
       </c>
-      <c r="E271" s="20">
+      <c r="E271" s="10">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="F271" s="10">
         <f t="shared" si="11"/>
-        <v>3.64</v>
-      </c>
-      <c r="F271" s="20">
-        <f t="shared" si="11"/>
-        <v>18.399999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="272" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D272" t="s">
         <v>140</v>
       </c>
-      <c r="E272" s="20">
+      <c r="E272" s="10">
+        <f t="shared" si="10"/>
+        <v>8</v>
+      </c>
+      <c r="F272" s="10">
         <f t="shared" si="11"/>
-        <v>8.02</v>
-      </c>
-      <c r="F272" s="20">
-        <f>AVERAGEIF($A$2:$A$250,$D272,F$2:F$250)</f>
-        <v>5.72</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cambio db grafico_circular y grafico_circular2
</commit_message>
<xml_diff>
--- a/app_salud/app/logic/data/set_de_datos_1.xlsx
+++ b/app_salud/app/logic/data/set_de_datos_1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rstudio\software_salud\app_salud\app\logic\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rstudio\software_salud_test_1\app_salud\app\logic\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7E65D4-7815-4BB2-A707-0DE38429EF20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924884B5-B721-4416-A4EF-4C6322F801B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{A035267E-5D3E-4097-B788-79B64BEF5509}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1472" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1473" uniqueCount="143">
   <si>
     <t>Febrero</t>
   </si>
@@ -466,6 +466,9 @@
   </si>
   <si>
     <t>Todo</t>
+  </si>
+  <si>
+    <t>Porcentaje</t>
   </si>
 </sst>
 </file>
@@ -556,7 +559,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -603,6 +606,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -612,9 +617,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2919,7 +2921,7 @@
       <c r="M1" s="9"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="22" t="s">
         <v>101</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -2957,7 +2959,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="20"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="4" t="s">
         <v>104</v>
       </c>
@@ -2993,7 +2995,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="20"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="4" t="s">
         <v>105</v>
       </c>
@@ -3029,7 +3031,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="20"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="4" t="s">
         <v>106</v>
       </c>
@@ -3065,7 +3067,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="20"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="4" t="s">
         <v>107</v>
       </c>
@@ -3101,7 +3103,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="20"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="4" t="s">
         <v>108</v>
       </c>
@@ -3137,7 +3139,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="20"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="4" t="s">
         <v>109</v>
       </c>
@@ -3173,7 +3175,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="20"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="4" t="s">
         <v>110</v>
       </c>
@@ -3209,7 +3211,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="20"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="4" t="s">
         <v>111</v>
       </c>
@@ -3245,7 +3247,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="20"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="4" t="s">
         <v>112</v>
       </c>
@@ -3281,7 +3283,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="20"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="4" t="s">
         <v>113</v>
       </c>
@@ -3317,13 +3319,13 @@
       </c>
     </row>
     <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="22" t="s">
         <v>52</v>
       </c>
       <c r="D13" s="5">
@@ -4127,21 +4129,21 @@
     <row r="1" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="13"/>
       <c r="B1" s="13"/>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22" t="s">
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24" t="s">
         <v>89</v>
       </c>
     </row>
@@ -4186,12 +4188,12 @@
       <c r="N2" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="O2" s="22" t="s">
+      <c r="O2" s="24" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="23" t="s">
         <v>127</v>
       </c>
       <c r="B3" s="14" t="s">
@@ -4238,7 +4240,7 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="21"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="14" t="s">
         <v>129</v>
       </c>
@@ -4283,7 +4285,7 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="23" t="s">
         <v>130</v>
       </c>
       <c r="B5" s="14" t="s">
@@ -4330,7 +4332,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="21"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="14" t="s">
         <v>129</v>
       </c>
@@ -4375,7 +4377,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="23" t="s">
         <v>131</v>
       </c>
       <c r="B7" s="14" t="s">
@@ -4422,7 +4424,7 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="21"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="14" t="s">
         <v>129</v>
       </c>
@@ -4467,7 +4469,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="23" t="s">
         <v>132</v>
       </c>
       <c r="B9" s="14" t="s">
@@ -4514,7 +4516,7 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="21"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="14" t="s">
         <v>129</v>
       </c>
@@ -4559,7 +4561,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="23" t="s">
         <v>133</v>
       </c>
       <c r="B11" s="14" t="s">
@@ -4606,7 +4608,7 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="21"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="14" t="s">
         <v>129</v>
       </c>
@@ -4651,7 +4653,7 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="23" t="s">
         <v>134</v>
       </c>
       <c r="B13" s="14" t="s">
@@ -4698,7 +4700,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="21"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="14" t="s">
         <v>129</v>
       </c>
@@ -6791,7 +6793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22BBA4D-C85A-4304-A112-5E7EF2BBD7F1}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -7402,7 +7404,7 @@
   <dimension ref="A1:F286"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
-      <selection activeCell="F279" sqref="F279"/>
+      <selection activeCell="F285" sqref="F285"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13175,10 +13177,10 @@
         <v/>
       </c>
       <c r="E274" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="F274" s="23">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="F274" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="275" spans="3:6" x14ac:dyDescent="0.3">
@@ -13189,7 +13191,7 @@
       <c r="E275" t="s">
         <v>17</v>
       </c>
-      <c r="F275" s="25">
+      <c r="F275" s="21">
         <f>ROUND(E268/SUM($E$268:$E$272)*100,2)</f>
         <v>9.8000000000000007</v>
       </c>
@@ -13202,8 +13204,8 @@
       <c r="E276" t="s">
         <v>18</v>
       </c>
-      <c r="F276" s="25">
-        <f t="shared" ref="F276:F284" si="12">ROUND(E269/SUM($E$268:$E$272)*100,2)</f>
+      <c r="F276" s="21">
+        <f t="shared" ref="F276:F279" si="12">ROUND(E269/SUM($E$268:$E$272)*100,2)</f>
         <v>3.92</v>
       </c>
     </row>
@@ -13215,7 +13217,7 @@
       <c r="E277" t="s">
         <v>19</v>
       </c>
-      <c r="F277" s="25">
+      <c r="F277" s="21">
         <f t="shared" si="12"/>
         <v>62.75</v>
       </c>
@@ -13228,7 +13230,7 @@
       <c r="E278" t="s">
         <v>139</v>
       </c>
-      <c r="F278" s="25">
+      <c r="F278" s="21">
         <f>ROUND(E271/SUM($E$268:$E$272)*100,2)</f>
         <v>7.84</v>
       </c>
@@ -13241,7 +13243,7 @@
       <c r="E279" t="s">
         <v>140</v>
       </c>
-      <c r="F279" s="25">
+      <c r="F279" s="21">
         <f t="shared" si="12"/>
         <v>15.69</v>
       </c>
@@ -13254,7 +13256,7 @@
       <c r="E280" t="s">
         <v>17</v>
       </c>
-      <c r="F280" s="25">
+      <c r="F280" s="21">
         <f>ROUND(F268/SUM($F$268:$F$272)*100,2)</f>
         <v>7.02</v>
       </c>
@@ -13267,7 +13269,7 @@
       <c r="E281" t="s">
         <v>18</v>
       </c>
-      <c r="F281" s="25">
+      <c r="F281" s="21">
         <f t="shared" ref="F281:F284" si="13">ROUND(F269/SUM($F$268:$F$272)*100,2)</f>
         <v>45.61</v>
       </c>
@@ -13280,7 +13282,7 @@
       <c r="E282" t="s">
         <v>19</v>
       </c>
-      <c r="F282" s="25">
+      <c r="F282" s="21">
         <f t="shared" si="13"/>
         <v>5.26</v>
       </c>
@@ -13293,7 +13295,7 @@
       <c r="E283" t="s">
         <v>139</v>
       </c>
-      <c r="F283" s="25">
+      <c r="F283" s="21">
         <f t="shared" si="13"/>
         <v>31.58</v>
       </c>
@@ -13306,7 +13308,7 @@
       <c r="E284" t="s">
         <v>140</v>
       </c>
-      <c r="F284" s="25">
+      <c r="F284" s="21">
         <f t="shared" si="13"/>
         <v>10.53</v>
       </c>
@@ -13318,7 +13320,7 @@
       <c r="E285" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="F285" s="24">
+      <c r="F285" s="20">
         <f>ROUND(SUM(E268:E272)/SUM(E268:F272)*100,2)</f>
         <v>47.22</v>
       </c>
@@ -13330,7 +13332,7 @@
       <c r="E286" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="F286" s="24">
+      <c r="F286" s="20">
         <f>ROUND(SUM(F268:F272)/SUM(E268:F272)*100,2)</f>
         <v>52.78</v>
       </c>

</xml_diff>